<commit_message>
Divers ajustements avec le ID du client - 2023-12-15
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F04FE60-35E7-49F7-BE06-62DE89AB33AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E95CFAF-11EB-49B1-807C-7783D8A242F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil1" sheetId="5" r:id="rId2"/>
-    <sheet name="Professionnels" sheetId="3" r:id="rId3"/>
-    <sheet name="ProfTaux" sheetId="4" r:id="rId4"/>
-    <sheet name="PlanComptable" sheetId="2" r:id="rId5"/>
+    <sheet name="Professionnels" sheetId="3" r:id="rId2"/>
+    <sheet name="ProfTaux" sheetId="4" r:id="rId3"/>
+    <sheet name="PlanComptable" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2228" uniqueCount="2152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="2153">
   <si>
     <t>Exxon Mobil Corporation</t>
   </si>
@@ -6496,6 +6495,9 @@
   </si>
   <si>
     <t>AB Volvo Car</t>
+  </si>
+  <si>
+    <t>Gestion ABCD inc.</t>
   </si>
 </sst>
 </file>
@@ -6573,7 +6575,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -6716,12 +6718,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="6" tint="-0.499984740745262"/>
+      </left>
+      <right style="hair">
+        <color theme="6" tint="-0.499984740745262"/>
+      </right>
+      <top style="hair">
+        <color theme="6" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color theme="6" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="6" tint="-0.499984740745262"/>
+      </right>
+      <top style="hair">
+        <color theme="6" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6843,12 +6871,66 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="67">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1F5E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1F5E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1F5E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF5F8EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="6" tint="-0.25098422193060094"/>
+          </stop>
+          <stop position="1">
+            <color theme="6" tint="-0.49803155613879818"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -7108,47 +7190,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="6" tint="-0.25098422193060094"/>
-          </stop>
-          <stop position="1">
-            <color theme="6" tint="-0.49803155613879818"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFF5F8EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1F5E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1F5E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1F5E7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7202,6 +7246,27 @@
             <color theme="6" tint="-0.49803155613879818"/>
           </stop>
         </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1F5E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1F5E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1F5E7"/>
+        </patternFill>
       </fill>
     </dxf>
     <dxf>
@@ -7653,10 +7718,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78FFC8C2-57F2-4B29-8BB0-D03F792CD856}">
   <sheetPr codeName="wshClients"/>
-  <dimension ref="A1:K2021"/>
+  <dimension ref="A1:K2022"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23830,12 +23895,20 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="2021" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2021" s="15">
+    <row r="2021" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2021" s="43">
         <v>2020</v>
       </c>
-      <c r="B2021" s="16" t="s">
+      <c r="B2021" s="44" t="s">
         <v>1999</v>
+      </c>
+    </row>
+    <row r="2022" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2022" s="30">
+        <v>2021</v>
+      </c>
+      <c r="B2022" s="45" t="s">
+        <v>2152</v>
       </c>
     </row>
   </sheetData>
@@ -23843,88 +23916,113 @@
     <sortCondition ref="B2:B2011"/>
   </sortState>
   <conditionalFormatting sqref="A2:B2021">
-    <cfRule type="expression" dxfId="62" priority="20">
+    <cfRule type="expression" dxfId="66" priority="25">
       <formula>#REF!=ROW()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:B8 A14:B15 A10:A11">
-    <cfRule type="expression" dxfId="61" priority="21">
+    <cfRule type="expression" dxfId="65" priority="26">
       <formula>AND($L2&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:B2021">
-    <cfRule type="expression" dxfId="60" priority="19">
+    <cfRule type="expression" dxfId="64" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B11">
-    <cfRule type="expression" dxfId="59" priority="22">
+    <cfRule type="expression" dxfId="63" priority="27">
       <formula>AND($L2&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:B4 A14:B14 A2:B2 A12:B12 A10 A7:B8">
-    <cfRule type="expression" dxfId="58" priority="18">
+    <cfRule type="expression" dxfId="62" priority="23">
       <formula>AND($L1048575&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:B2021">
-    <cfRule type="expression" dxfId="57" priority="23">
+    <cfRule type="expression" dxfId="61" priority="28">
       <formula>AND($L1048563&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:B3 A13:B13 A9">
-    <cfRule type="expression" dxfId="56" priority="24">
+    <cfRule type="expression" dxfId="60" priority="29">
       <formula>AND(#REF!&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:B2 A12:B12 A8">
-    <cfRule type="expression" dxfId="55" priority="25">
+    <cfRule type="expression" dxfId="59" priority="30">
       <formula>AND($L1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:B3 A13:B13 A9">
-    <cfRule type="expression" dxfId="54" priority="26">
+    <cfRule type="expression" dxfId="58" priority="31">
       <formula>AND(#REF!&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:B5 A15:B15 A11">
-    <cfRule type="expression" dxfId="53" priority="27">
+    <cfRule type="expression" dxfId="57" priority="32">
       <formula>AND(#REF!&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:B22 A32:B36 A46:B50 A60:B64 A74:B78 A88:B92 A102:B106 A116:B120 A130:B134 A144:B148 A158:B162 A172:B176 A186:B190 A200:B204 A214:B218 A228:B232 A242:B246 A256:B260 A270:B274 A284:B288 A298:B302 A312:B316 A326:B330 A340:B344 A354:B358 A368:B372 A382:B386 A396:B400 A410:B414 A424:B428 A438:B442 A452:B456 A466:B470 A480:B484 A494:B498 A508:B512 A522:B526 A536:B540 A550:B554 A564:B568 A578:B582 A592:B596 A606:B610 A620:B624 A634:B638 A648:B652 A662:B666 A676:B680 A690:B694 A704:B708 A718:B722 A732:B736 A746:B750 A760:B764 A774:B778 A788:B792 A802:B806 A816:B820 A830:B834 A844:B848 A858:B862 A872:B876 A886:B890 A900:B904 A914:B918 A928:B932 A942:B946 A956:B960 A970:B974 A984:B988 A998:B1002 A1012:B1016 A1026:B1030 A1040:B1044 A1054:B1058 A1068:B1072 A1082:B1086 A1096:B1100 A1110:B1114 A1124:B1128 A1138:B1142 A1152:B1156 A1166:B1170 A1180:B1184 A1194:B1198 A1208:B1212 A1222:B1226 A1236:B1240 A1250:B1254 A1264:B1268 A1278:B1282 A1292:B1296 A1306:B1310 A1320:B1324 A1334:B1338 A1348:B1352 A1362:B1366 A1376:B1380 A1390:B1394 A1404:B1408 A1418:B1422 A1432:B1436 A1446:B1450 A1460:B1464 A1474:B1478 A1488:B1492 A1502:B1506 A1516:B1520 A1530:B1534 A1544:B1548 A1558:B1562 A1572:B1576 A1586:B1590 A1600:B1604 A1614:B1618 A1628:B1632 A1642:B1646 A1656:B1660 A1670:B1674 A1684:B1688 A1698:B1702 A1712:B1716 A1726:B1730 A1740:B1744 A1754:B1758 A1768:B1772 A1782:B1786 A1796:B1800 A1810:B1814 A1824:B1828 A1838:B1842 A1852:B1856 A1866:B1870 A1880:B1884 A1894:B1898 A1908:B1912 A1922:B1926 A1936:B1940 A1950:B1954 A1964:B1968 A1978:B1982 A1992:B1996 A2006:B2010 A2020:B2021 A28:B29 A42:B43 A56:B57 A70:B71 A84:B85 A98:B99 A112:B113 A126:B127 A140:B141 A154:B155 A168:B169 A182:B183 A196:B197 A210:B211 A224:B225 A238:B239 A252:B253 A266:B267 A280:B281 A294:B295 A308:B309 A322:B323 A336:B337 A350:B351 A364:B365 A378:B379 A392:B393 A406:B407 A420:B421 A434:B435 A448:B449 A462:B463 A476:B477 A490:B491 A504:B505 A518:B519 A532:B533 A546:B547 A560:B561 A574:B575 A588:B589 A602:B603 A616:B617 A630:B631 A644:B645 A658:B659 A672:B673 A686:B687 A700:B701 A714:B715 A728:B729 A742:B743 A756:B757 A770:B771 A784:B785 A798:B799 A812:B813 A826:B827 A840:B841 A854:B855 A868:B869 A882:B883 A896:B897 A910:B911 A924:B925 A938:B939 A952:B953 A966:B967 A980:B981 A994:B995 A1008:B1009 A1022:B1023 A1036:B1037 A1050:B1051 A1064:B1065 A1078:B1079 A1092:B1093 A1106:B1107 A1120:B1121 A1134:B1135 A1148:B1149 A1162:B1163 A1176:B1177 A1190:B1191 A1204:B1205 A1218:B1219 A1232:B1233 A1246:B1247 A1260:B1261 A1274:B1275 A1288:B1289 A1302:B1303 A1316:B1317 A1330:B1331 A1344:B1345 A1358:B1359 A1372:B1373 A1386:B1387 A1400:B1401 A1414:B1415 A1428:B1429 A1442:B1443 A1456:B1457 A1470:B1471 A1484:B1485 A1498:B1499 A1512:B1513 A1526:B1527 A1540:B1541 A1554:B1555 A1568:B1569 A1582:B1583 A1596:B1597 A1610:B1611 A1624:B1625 A1638:B1639 A1652:B1653 A1666:B1667 A1680:B1681 A1694:B1695 A1708:B1709 A1722:B1723 A1736:B1737 A1750:B1751 A1764:B1765 A1778:B1779 A1792:B1793 A1806:B1807 A1820:B1821 A1834:B1835 A1848:B1849 A1862:B1863 A1876:B1877 A1890:B1891 A1904:B1905 A1918:B1919 A1932:B1933 A1946:B1947 A1960:B1961 A1974:B1975 A1988:B1989 A2002:B2003 A2016:B2017 A24:A25 A38:A39 A52:A53 A66:A67 A80:A81 A94:A95 A108:A109 A122:A123 A136:A137 A150:A151 A164:A165 A178:A179 A192:A193 A206:A207 A220:A221 A234:A235 A248:A249 A262:A263 A276:A277 A290:A291 A304:A305 A318:A319 A332:A333 A346:A347 A360:A361 A374:A375 A388:A389 A402:A403 A416:A417 A430:A431 A444:A445 A458:A459 A472:A473 A486:A487 A500:A501 A514:A515 A528:A529 A542:A543 A556:A557 A570:A571 A584:A585 A598:A599 A612:A613 A626:A627 A640:A641 A654:A655 A668:A669 A682:A683 A696:A697 A710:A711 A724:A725 A738:A739 A752:A753 A766:A767 A780:A781 A794:A795 A808:A809 A822:A823 A836:A837 A850:A851 A864:A865 A878:A879 A892:A893 A906:A907 A920:A921 A934:A935 A948:A949 A962:A963 A976:A977 A990:A991 A1004:A1005 A1018:A1019 A1032:A1033 A1046:A1047 A1060:A1061 A1074:A1075 A1088:A1089 A1102:A1103 A1116:A1117 A1130:A1131 A1144:A1145 A1158:A1159 A1172:A1173 A1186:A1187 A1200:A1201 A1214:A1215 A1228:A1229 A1242:A1243 A1256:A1257 A1270:A1271 A1284:A1285 A1298:A1299 A1312:A1313 A1326:A1327 A1340:A1341 A1354:A1355 A1368:A1369 A1382:A1383 A1396:A1397 A1410:A1411 A1424:A1425 A1438:A1439 A1452:A1453 A1466:A1467 A1480:A1481 A1494:A1495 A1508:A1509 A1522:A1523 A1536:A1537 A1550:A1551 A1564:A1565 A1578:A1579 A1592:A1593 A1606:A1607 A1620:A1621 A1634:A1635 A1648:A1649 A1662:A1663 A1676:A1677 A1690:A1691 A1704:A1705 A1718:A1719 A1732:A1733 A1746:A1747 A1760:A1761 A1774:A1775 A1788:A1789 A1802:A1803 A1816:A1817 A1830:A1831 A1844:A1845 A1858:A1859 A1872:A1873 A1886:A1887 A1900:A1901 A1914:A1915 A1928:A1929 A1942:A1943 A1956:A1957 A1970:A1971 A1984:A1985 A1998:A1999 A2012:A2013">
-    <cfRule type="expression" dxfId="52" priority="2">
+    <cfRule type="expression" dxfId="56" priority="7">
       <formula>AND($L16&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:B25 A34:B39 A48:B53 A62:B67 A76:B81 A90:B95 A104:B109 A118:B123 A132:B137 A146:B151 A160:B165 A174:B179 A188:B193 A202:B207 A216:B221 A230:B235 A244:B249 A258:B263 A272:B277 A286:B291 A300:B305 A314:B319 A328:B333 A342:B347 A356:B361 A370:B375 A384:B389 A398:B403 A412:B417 A426:B431 A440:B445 A454:B459 A468:B473 A482:B487 A496:B501 A510:B515 A524:B529 A538:B543 A552:B557 A566:B571 A580:B585 A594:B599 A608:B613 A622:B627 A636:B641 A650:B655 A664:B669 A678:B683 A692:B697 A706:B711 A720:B725 A734:B739 A748:B753 A762:B767 A776:B781 A790:B795 A804:B809 A818:B823 A832:B837 A846:B851 A860:B865 A874:B879 A888:B893 A902:B907 A916:B921 A930:B935 A944:B949 A958:B963 A972:B977 A986:B991 A1000:B1005 A1014:B1019 A1028:B1033 A1042:B1047 A1056:B1061 A1070:B1075 A1084:B1089 A1098:B1103 A1112:B1117 A1126:B1131 A1140:B1145 A1154:B1159 A1168:B1173 A1182:B1187 A1196:B1201 A1210:B1215 A1224:B1229 A1238:B1243 A1252:B1257 A1266:B1271 A1280:B1285 A1294:B1299 A1308:B1313 A1322:B1327 A1336:B1341 A1350:B1355 A1364:B1369 A1378:B1383 A1392:B1397 A1406:B1411 A1420:B1425 A1434:B1439 A1448:B1453 A1462:B1467 A1476:B1481 A1490:B1495 A1504:B1509 A1518:B1523 A1532:B1537 A1546:B1551 A1560:B1565 A1574:B1579 A1588:B1593 A1602:B1607 A1616:B1621 A1630:B1635 A1644:B1649 A1658:B1663 A1672:B1677 A1686:B1691 A1700:B1705 A1714:B1719 A1728:B1733 A1742:B1747 A1756:B1761 A1770:B1775 A1784:B1789 A1798:B1803 A1812:B1817 A1826:B1831 A1840:B1845 A1854:B1859 A1868:B1873 A1882:B1887 A1896:B1901 A1910:B1915 A1924:B1929 A1938:B1943 A1952:B1957 A1966:B1971 A1980:B1985 A1994:B1999 A2008:B2013">
-    <cfRule type="expression" dxfId="51" priority="3">
+    <cfRule type="expression" dxfId="55" priority="8">
       <formula>AND($L16&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:B18 A32:B32 A46:B46 A60:B60 A74:B74 A88:B88 A102:B102 A116:B116 A130:B130 A144:B144 A158:B158 A172:B172 A186:B186 A200:B200 A214:B214 A228:B228 A242:B242 A256:B256 A270:B270 A284:B284 A298:B298 A312:B312 A326:B326 A340:B340 A354:B354 A368:B368 A382:B382 A396:B396 A410:B410 A424:B424 A438:B438 A452:B452 A466:B466 A480:B480 A494:B494 A508:B508 A522:B522 A536:B536 A550:B550 A564:B564 A578:B578 A592:B592 A606:B606 A620:B620 A634:B634 A648:B648 A662:B662 A676:B676 A690:B690 A704:B704 A718:B718 A732:B732 A746:B746 A760:B760 A774:B774 A788:B788 A802:B802 A816:B816 A830:B830 A844:B844 A858:B858 A872:B872 A886:B886 A900:B900 A914:B914 A928:B928 A942:B942 A956:B956 A970:B970 A984:B984 A998:B998 A1012:B1012 A1026:B1026 A1040:B1040 A1054:B1054 A1068:B1068 A1082:B1082 A1096:B1096 A1110:B1110 A1124:B1124 A1138:B1138 A1152:B1152 A1166:B1166 A1180:B1180 A1194:B1194 A1208:B1208 A1222:B1222 A1236:B1236 A1250:B1250 A1264:B1264 A1278:B1278 A1292:B1292 A1306:B1306 A1320:B1320 A1334:B1334 A1348:B1348 A1362:B1362 A1376:B1376 A1390:B1390 A1404:B1404 A1418:B1418 A1432:B1432 A1446:B1446 A1460:B1460 A1474:B1474 A1488:B1488 A1502:B1502 A1516:B1516 A1530:B1530 A1544:B1544 A1558:B1558 A1572:B1572 A1586:B1586 A1600:B1600 A1614:B1614 A1628:B1628 A1642:B1642 A1656:B1656 A1670:B1670 A1684:B1684 A1698:B1698 A1712:B1712 A1726:B1726 A1740:B1740 A1754:B1754 A1768:B1768 A1782:B1782 A1796:B1796 A1810:B1810 A1824:B1824 A1838:B1838 A1852:B1852 A1866:B1866 A1880:B1880 A1894:B1894 A1908:B1908 A1922:B1922 A1936:B1936 A1950:B1950 A1964:B1964 A1978:B1978 A1992:B1992 A2006:B2006 A2020:B2020 A28:B28 A42:B42 A56:B56 A70:B70 A84:B84 A98:B98 A112:B112 A126:B126 A140:B140 A154:B154 A168:B168 A182:B182 A196:B196 A210:B210 A224:B224 A238:B238 A252:B252 A266:B266 A280:B280 A294:B294 A308:B308 A322:B322 A336:B336 A350:B350 A364:B364 A378:B378 A392:B392 A406:B406 A420:B420 A434:B434 A448:B448 A462:B462 A476:B476 A490:B490 A504:B504 A518:B518 A532:B532 A546:B546 A560:B560 A574:B574 A588:B588 A602:B602 A616:B616 A630:B630 A644:B644 A658:B658 A672:B672 A686:B686 A700:B700 A714:B714 A728:B728 A742:B742 A756:B756 A770:B770 A784:B784 A798:B798 A812:B812 A826:B826 A840:B840 A854:B854 A868:B868 A882:B882 A896:B896 A910:B910 A924:B924 A938:B938 A952:B952 A966:B966 A980:B980 A994:B994 A1008:B1008 A1022:B1022 A1036:B1036 A1050:B1050 A1064:B1064 A1078:B1078 A1092:B1092 A1106:B1106 A1120:B1120 A1134:B1134 A1148:B1148 A1162:B1162 A1176:B1176 A1190:B1190 A1204:B1204 A1218:B1218 A1232:B1232 A1246:B1246 A1260:B1260 A1274:B1274 A1288:B1288 A1302:B1302 A1316:B1316 A1330:B1330 A1344:B1344 A1358:B1358 A1372:B1372 A1386:B1386 A1400:B1400 A1414:B1414 A1428:B1428 A1442:B1442 A1456:B1456 A1470:B1470 A1484:B1484 A1498:B1498 A1512:B1512 A1526:B1526 A1540:B1540 A1554:B1554 A1568:B1568 A1582:B1582 A1596:B1596 A1610:B1610 A1624:B1624 A1638:B1638 A1652:B1652 A1666:B1666 A1680:B1680 A1694:B1694 A1708:B1708 A1722:B1722 A1736:B1736 A1750:B1750 A1764:B1764 A1778:B1778 A1792:B1792 A1806:B1806 A1820:B1820 A1834:B1834 A1848:B1848 A1862:B1862 A1876:B1876 A1890:B1890 A1904:B1904 A1918:B1918 A1932:B1932 A1946:B1946 A1960:B1960 A1974:B1974 A1988:B1988 A2002:B2002 A2016:B2016 A16:B16 A30:B30 A44:B44 A58:B58 A72:B72 A86:B86 A100:B100 A114:B114 A128:B128 A142:B142 A156:B156 A170:B170 A184:B184 A198:B198 A212:B212 A226:B226 A240:B240 A254:B254 A268:B268 A282:B282 A296:B296 A310:B310 A324:B324 A338:B338 A352:B352 A366:B366 A380:B380 A394:B394 A408:B408 A422:B422 A436:B436 A450:B450 A464:B464 A478:B478 A492:B492 A506:B506 A520:B520 A534:B534 A548:B548 A562:B562 A576:B576 A590:B590 A604:B604 A618:B618 A632:B632 A646:B646 A660:B660 A674:B674 A688:B688 A702:B702 A716:B716 A730:B730 A744:B744 A758:B758 A772:B772 A786:B786 A800:B800 A814:B814 A828:B828 A842:B842 A856:B856 A870:B870 A884:B884 A898:B898 A912:B912 A926:B926 A940:B940 A954:B954 A968:B968 A982:B982 A996:B996 A1010:B1010 A1024:B1024 A1038:B1038 A1052:B1052 A1066:B1066 A1080:B1080 A1094:B1094 A1108:B1108 A1122:B1122 A1136:B1136 A1150:B1150 A1164:B1164 A1178:B1178 A1192:B1192 A1206:B1206 A1220:B1220 A1234:B1234 A1248:B1248 A1262:B1262 A1276:B1276 A1290:B1290 A1304:B1304 A1318:B1318 A1332:B1332 A1346:B1346 A1360:B1360 A1374:B1374 A1388:B1388 A1402:B1402 A1416:B1416 A1430:B1430 A1444:B1444 A1458:B1458 A1472:B1472 A1486:B1486 A1500:B1500 A1514:B1514 A1528:B1528 A1542:B1542 A1556:B1556 A1570:B1570 A1584:B1584 A1598:B1598 A1612:B1612 A1626:B1626 A1640:B1640 A1654:B1654 A1668:B1668 A1682:B1682 A1696:B1696 A1710:B1710 A1724:B1724 A1738:B1738 A1752:B1752 A1766:B1766 A1780:B1780 A1794:B1794 A1808:B1808 A1822:B1822 A1836:B1836 A1850:B1850 A1864:B1864 A1878:B1878 A1892:B1892 A1906:B1906 A1920:B1920 A1934:B1934 A1948:B1948 A1962:B1962 A1976:B1976 A1990:B1990 A2004:B2004 A2018:B2018 A26:B26 A40:B40 A54:B54 A68:B68 A82:B82 A96:B96 A110:B110 A124:B124 A138:B138 A152:B152 A166:B166 A180:B180 A194:B194 A208:B208 A222:B222 A236:B236 A250:B250 A264:B264 A278:B278 A292:B292 A306:B306 A320:B320 A334:B334 A348:B348 A362:B362 A376:B376 A390:B390 A404:B404 A418:B418 A432:B432 A446:B446 A460:B460 A474:B474 A488:B488 A502:B502 A516:B516 A530:B530 A544:B544 A558:B558 A572:B572 A586:B586 A600:B600 A614:B614 A628:B628 A642:B642 A656:B656 A670:B670 A684:B684 A698:B698 A712:B712 A726:B726 A740:B740 A754:B754 A768:B768 A782:B782 A796:B796 A810:B810 A824:B824 A838:B838 A852:B852 A866:B866 A880:B880 A894:B894 A908:B908 A922:B922 A936:B936 A950:B950 A964:B964 A978:B978 A992:B992 A1006:B1006 A1020:B1020 A1034:B1034 A1048:B1048 A1062:B1062 A1076:B1076 A1090:B1090 A1104:B1104 A1118:B1118 A1132:B1132 A1146:B1146 A1160:B1160 A1174:B1174 A1188:B1188 A1202:B1202 A1216:B1216 A1230:B1230 A1244:B1244 A1258:B1258 A1272:B1272 A1286:B1286 A1300:B1300 A1314:B1314 A1328:B1328 A1342:B1342 A1356:B1356 A1370:B1370 A1384:B1384 A1398:B1398 A1412:B1412 A1426:B1426 A1440:B1440 A1454:B1454 A1468:B1468 A1482:B1482 A1496:B1496 A1510:B1510 A1524:B1524 A1538:B1538 A1552:B1552 A1566:B1566 A1580:B1580 A1594:B1594 A1608:B1608 A1622:B1622 A1636:B1636 A1650:B1650 A1664:B1664 A1678:B1678 A1692:B1692 A1706:B1706 A1720:B1720 A1734:B1734 A1748:B1748 A1762:B1762 A1776:B1776 A1790:B1790 A1804:B1804 A1818:B1818 A1832:B1832 A1846:B1846 A1860:B1860 A1874:B1874 A1888:B1888 A1902:B1902 A1916:B1916 A1930:B1930 A1944:B1944 A1958:B1958 A1972:B1972 A1986:B1986 A2000:B2000 A2014:B2014 A24 A38 A52 A66 A80 A94 A108 A122 A136 A150 A164 A178 A192 A206 A220 A234 A248 A262 A276 A290 A304 A318 A332 A346 A360 A374 A388 A402 A416 A430 A444 A458 A472 A486 A500 A514 A528 A542 A556 A570 A584 A598 A612 A626 A640 A654 A668 A682 A696 A710 A724 A738 A752 A766 A780 A794 A808 A822 A836 A850 A864 A878 A892 A906 A920 A934 A948 A962 A976 A990 A1004 A1018 A1032 A1046 A1060 A1074 A1088 A1102 A1116 A1130 A1144 A1158 A1172 A1186 A1200 A1214 A1228 A1242 A1256 A1270 A1284 A1298 A1312 A1326 A1340 A1354 A1368 A1382 A1396 A1410 A1424 A1438 A1452 A1466 A1480 A1494 A1508 A1522 A1536 A1550 A1564 A1578 A1592 A1606 A1620 A1634 A1648 A1662 A1676 A1690 A1704 A1718 A1732 A1746 A1760 A1774 A1788 A1802 A1816 A1830 A1844 A1858 A1872 A1886 A1900 A1914 A1928 A1942 A1956 A1970 A1984 A1998 A2012 A21:B22 A35:B36 A49:B50 A63:B64 A77:B78 A91:B92 A105:B106 A119:B120 A133:B134 A147:B148 A161:B162 A175:B176 A189:B190 A203:B204 A217:B218 A231:B232 A245:B246 A259:B260 A273:B274 A287:B288 A301:B302 A315:B316 A329:B330 A343:B344 A357:B358 A371:B372 A385:B386 A399:B400 A413:B414 A427:B428 A441:B442 A455:B456 A469:B470 A483:B484 A497:B498 A511:B512 A525:B526 A539:B540 A553:B554 A567:B568 A581:B582 A595:B596 A609:B610 A623:B624 A637:B638 A651:B652 A665:B666 A679:B680 A693:B694 A707:B708 A721:B722 A735:B736 A749:B750 A763:B764 A777:B778 A791:B792 A805:B806 A819:B820 A833:B834 A847:B848 A861:B862 A875:B876 A889:B890 A903:B904 A917:B918 A931:B932 A945:B946 A959:B960 A973:B974 A987:B988 A1001:B1002 A1015:B1016 A1029:B1030 A1043:B1044 A1057:B1058 A1071:B1072 A1085:B1086 A1099:B1100 A1113:B1114 A1127:B1128 A1141:B1142 A1155:B1156 A1169:B1170 A1183:B1184 A1197:B1198 A1211:B1212 A1225:B1226 A1239:B1240 A1253:B1254 A1267:B1268 A1281:B1282 A1295:B1296 A1309:B1310 A1323:B1324 A1337:B1338 A1351:B1352 A1365:B1366 A1379:B1380 A1393:B1394 A1407:B1408 A1421:B1422 A1435:B1436 A1449:B1450 A1463:B1464 A1477:B1478 A1491:B1492 A1505:B1506 A1519:B1520 A1533:B1534 A1547:B1548 A1561:B1562 A1575:B1576 A1589:B1590 A1603:B1604 A1617:B1618 A1631:B1632 A1645:B1646 A1659:B1660 A1673:B1674 A1687:B1688 A1701:B1702 A1715:B1716 A1729:B1730 A1743:B1744 A1757:B1758 A1771:B1772 A1785:B1786 A1799:B1800 A1813:B1814 A1827:B1828 A1841:B1842 A1855:B1856 A1869:B1870 A1883:B1884 A1897:B1898 A1911:B1912 A1925:B1926 A1939:B1940 A1953:B1954 A1967:B1968 A1981:B1982 A1995:B1996 A2009:B2010">
-    <cfRule type="expression" dxfId="50" priority="1">
+    <cfRule type="expression" dxfId="54" priority="6">
       <formula>AND($L13&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:B17 A31:B31 A45:B45 A59:B59 A73:B73 A87:B87 A101:B101 A115:B115 A129:B129 A143:B143 A157:B157 A171:B171 A185:B185 A199:B199 A213:B213 A227:B227 A241:B241 A255:B255 A269:B269 A283:B283 A297:B297 A311:B311 A325:B325 A339:B339 A353:B353 A367:B367 A381:B381 A395:B395 A409:B409 A423:B423 A437:B437 A451:B451 A465:B465 A479:B479 A493:B493 A507:B507 A521:B521 A535:B535 A549:B549 A563:B563 A577:B577 A591:B591 A605:B605 A619:B619 A633:B633 A647:B647 A661:B661 A675:B675 A689:B689 A703:B703 A717:B717 A731:B731 A745:B745 A759:B759 A773:B773 A787:B787 A801:B801 A815:B815 A829:B829 A843:B843 A857:B857 A871:B871 A885:B885 A899:B899 A913:B913 A927:B927 A941:B941 A955:B955 A969:B969 A983:B983 A997:B997 A1011:B1011 A1025:B1025 A1039:B1039 A1053:B1053 A1067:B1067 A1081:B1081 A1095:B1095 A1109:B1109 A1123:B1123 A1137:B1137 A1151:B1151 A1165:B1165 A1179:B1179 A1193:B1193 A1207:B1207 A1221:B1221 A1235:B1235 A1249:B1249 A1263:B1263 A1277:B1277 A1291:B1291 A1305:B1305 A1319:B1319 A1333:B1333 A1347:B1347 A1361:B1361 A1375:B1375 A1389:B1389 A1403:B1403 A1417:B1417 A1431:B1431 A1445:B1445 A1459:B1459 A1473:B1473 A1487:B1487 A1501:B1501 A1515:B1515 A1529:B1529 A1543:B1543 A1557:B1557 A1571:B1571 A1585:B1585 A1599:B1599 A1613:B1613 A1627:B1627 A1641:B1641 A1655:B1655 A1669:B1669 A1683:B1683 A1697:B1697 A1711:B1711 A1725:B1725 A1739:B1739 A1753:B1753 A1767:B1767 A1781:B1781 A1795:B1795 A1809:B1809 A1823:B1823 A1837:B1837 A1851:B1851 A1865:B1865 A1879:B1879 A1893:B1893 A1907:B1907 A1921:B1921 A1935:B1935 A1949:B1949 A1963:B1963 A1977:B1977 A1991:B1991 A2005:B2005 A2019:B2019 A27:B27 A41:B41 A55:B55 A69:B69 A83:B83 A97:B97 A111:B111 A125:B125 A139:B139 A153:B153 A167:B167 A181:B181 A195:B195 A209:B209 A223:B223 A237:B237 A251:B251 A265:B265 A279:B279 A293:B293 A307:B307 A321:B321 A335:B335 A349:B349 A363:B363 A377:B377 A391:B391 A405:B405 A419:B419 A433:B433 A447:B447 A461:B461 A475:B475 A489:B489 A503:B503 A517:B517 A531:B531 A545:B545 A559:B559 A573:B573 A587:B587 A601:B601 A615:B615 A629:B629 A643:B643 A657:B657 A671:B671 A685:B685 A699:B699 A713:B713 A727:B727 A741:B741 A755:B755 A769:B769 A783:B783 A797:B797 A811:B811 A825:B825 A839:B839 A853:B853 A867:B867 A881:B881 A895:B895 A909:B909 A923:B923 A937:B937 A951:B951 A965:B965 A979:B979 A993:B993 A1007:B1007 A1021:B1021 A1035:B1035 A1049:B1049 A1063:B1063 A1077:B1077 A1091:B1091 A1105:B1105 A1119:B1119 A1133:B1133 A1147:B1147 A1161:B1161 A1175:B1175 A1189:B1189 A1203:B1203 A1217:B1217 A1231:B1231 A1245:B1245 A1259:B1259 A1273:B1273 A1287:B1287 A1301:B1301 A1315:B1315 A1329:B1329 A1343:B1343 A1357:B1357 A1371:B1371 A1385:B1385 A1399:B1399 A1413:B1413 A1427:B1427 A1441:B1441 A1455:B1455 A1469:B1469 A1483:B1483 A1497:B1497 A1511:B1511 A1525:B1525 A1539:B1539 A1553:B1553 A1567:B1567 A1581:B1581 A1595:B1595 A1609:B1609 A1623:B1623 A1637:B1637 A1651:B1651 A1665:B1665 A1679:B1679 A1693:B1693 A1707:B1707 A1721:B1721 A1735:B1735 A1749:B1749 A1763:B1763 A1777:B1777 A1791:B1791 A1805:B1805 A1819:B1819 A1833:B1833 A1847:B1847 A1861:B1861 A1875:B1875 A1889:B1889 A1903:B1903 A1917:B1917 A1931:B1931 A1945:B1945 A1959:B1959 A1973:B1973 A1987:B1987 A2001:B2001 A2015:B2015 A23 A37 A51 A65 A79 A93 A107 A121 A135 A149 A163 A177 A191 A205 A219 A233 A247 A261 A275 A289 A303 A317 A331 A345 A359 A373 A387 A401 A415 A429 A443 A457 A471 A485 A499 A513 A527 A541 A555 A569 A583 A597 A611 A625 A639 A653 A667 A681 A695 A709 A723 A737 A751 A765 A779 A793 A807 A821 A835 A849 A863 A877 A891 A905 A919 A933 A947 A961 A975 A989 A1003 A1017 A1031 A1045 A1059 A1073 A1087 A1101 A1115 A1129 A1143 A1157 A1171 A1185 A1199 A1213 A1227 A1241 A1255 A1269 A1283 A1297 A1311 A1325 A1339 A1353 A1367 A1381 A1395 A1409 A1423 A1437 A1451 A1465 A1479 A1493 A1507 A1521 A1535 A1549 A1563 A1577 A1591 A1605 A1619 A1633 A1647 A1661 A1675 A1689 A1703 A1717 A1731 A1745 A1759 A1773 A1787 A1801 A1815 A1829 A1843 A1857 A1871 A1885 A1899 A1913 A1927 A1941 A1955 A1969 A1983 A1997 A2011">
-    <cfRule type="expression" dxfId="49" priority="4">
+    <cfRule type="expression" dxfId="53" priority="9">
       <formula>AND(#REF!&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:B16 A30:B30 A44:B44 A58:B58 A72:B72 A86:B86 A100:B100 A114:B114 A128:B128 A142:B142 A156:B156 A170:B170 A184:B184 A198:B198 A212:B212 A226:B226 A240:B240 A254:B254 A268:B268 A282:B282 A296:B296 A310:B310 A324:B324 A338:B338 A352:B352 A366:B366 A380:B380 A394:B394 A408:B408 A422:B422 A436:B436 A450:B450 A464:B464 A478:B478 A492:B492 A506:B506 A520:B520 A534:B534 A548:B548 A562:B562 A576:B576 A590:B590 A604:B604 A618:B618 A632:B632 A646:B646 A660:B660 A674:B674 A688:B688 A702:B702 A716:B716 A730:B730 A744:B744 A758:B758 A772:B772 A786:B786 A800:B800 A814:B814 A828:B828 A842:B842 A856:B856 A870:B870 A884:B884 A898:B898 A912:B912 A926:B926 A940:B940 A954:B954 A968:B968 A982:B982 A996:B996 A1010:B1010 A1024:B1024 A1038:B1038 A1052:B1052 A1066:B1066 A1080:B1080 A1094:B1094 A1108:B1108 A1122:B1122 A1136:B1136 A1150:B1150 A1164:B1164 A1178:B1178 A1192:B1192 A1206:B1206 A1220:B1220 A1234:B1234 A1248:B1248 A1262:B1262 A1276:B1276 A1290:B1290 A1304:B1304 A1318:B1318 A1332:B1332 A1346:B1346 A1360:B1360 A1374:B1374 A1388:B1388 A1402:B1402 A1416:B1416 A1430:B1430 A1444:B1444 A1458:B1458 A1472:B1472 A1486:B1486 A1500:B1500 A1514:B1514 A1528:B1528 A1542:B1542 A1556:B1556 A1570:B1570 A1584:B1584 A1598:B1598 A1612:B1612 A1626:B1626 A1640:B1640 A1654:B1654 A1668:B1668 A1682:B1682 A1696:B1696 A1710:B1710 A1724:B1724 A1738:B1738 A1752:B1752 A1766:B1766 A1780:B1780 A1794:B1794 A1808:B1808 A1822:B1822 A1836:B1836 A1850:B1850 A1864:B1864 A1878:B1878 A1892:B1892 A1906:B1906 A1920:B1920 A1934:B1934 A1948:B1948 A1962:B1962 A1976:B1976 A1990:B1990 A2004:B2004 A2018:B2018 A26:B26 A40:B40 A54:B54 A68:B68 A82:B82 A96:B96 A110:B110 A124:B124 A138:B138 A152:B152 A166:B166 A180:B180 A194:B194 A208:B208 A222:B222 A236:B236 A250:B250 A264:B264 A278:B278 A292:B292 A306:B306 A320:B320 A334:B334 A348:B348 A362:B362 A376:B376 A390:B390 A404:B404 A418:B418 A432:B432 A446:B446 A460:B460 A474:B474 A488:B488 A502:B502 A516:B516 A530:B530 A544:B544 A558:B558 A572:B572 A586:B586 A600:B600 A614:B614 A628:B628 A642:B642 A656:B656 A670:B670 A684:B684 A698:B698 A712:B712 A726:B726 A740:B740 A754:B754 A768:B768 A782:B782 A796:B796 A810:B810 A824:B824 A838:B838 A852:B852 A866:B866 A880:B880 A894:B894 A908:B908 A922:B922 A936:B936 A950:B950 A964:B964 A978:B978 A992:B992 A1006:B1006 A1020:B1020 A1034:B1034 A1048:B1048 A1062:B1062 A1076:B1076 A1090:B1090 A1104:B1104 A1118:B1118 A1132:B1132 A1146:B1146 A1160:B1160 A1174:B1174 A1188:B1188 A1202:B1202 A1216:B1216 A1230:B1230 A1244:B1244 A1258:B1258 A1272:B1272 A1286:B1286 A1300:B1300 A1314:B1314 A1328:B1328 A1342:B1342 A1356:B1356 A1370:B1370 A1384:B1384 A1398:B1398 A1412:B1412 A1426:B1426 A1440:B1440 A1454:B1454 A1468:B1468 A1482:B1482 A1496:B1496 A1510:B1510 A1524:B1524 A1538:B1538 A1552:B1552 A1566:B1566 A1580:B1580 A1594:B1594 A1608:B1608 A1622:B1622 A1636:B1636 A1650:B1650 A1664:B1664 A1678:B1678 A1692:B1692 A1706:B1706 A1720:B1720 A1734:B1734 A1748:B1748 A1762:B1762 A1776:B1776 A1790:B1790 A1804:B1804 A1818:B1818 A1832:B1832 A1846:B1846 A1860:B1860 A1874:B1874 A1888:B1888 A1902:B1902 A1916:B1916 A1930:B1930 A1944:B1944 A1958:B1958 A1972:B1972 A1986:B1986 A2000:B2000 A2014:B2014 A22 A36 A50 A64 A78 A92 A106 A120 A134 A148 A162 A176 A190 A204 A218 A232 A246 A260 A274 A288 A302 A316 A330 A344 A358 A372 A386 A400 A414 A428 A442 A456 A470 A484 A498 A512 A526 A540 A554 A568 A582 A596 A610 A624 A638 A652 A666 A680 A694 A708 A722 A736 A750 A764 A778 A792 A806 A820 A834 A848 A862 A876 A890 A904 A918 A932 A946 A960 A974 A988 A1002 A1016 A1030 A1044 A1058 A1072 A1086 A1100 A1114 A1128 A1142 A1156 A1170 A1184 A1198 A1212 A1226 A1240 A1254 A1268 A1282 A1296 A1310 A1324 A1338 A1352 A1366 A1380 A1394 A1408 A1422 A1436 A1450 A1464 A1478 A1492 A1506 A1520 A1534 A1548 A1562 A1576 A1590 A1604 A1618 A1632 A1646 A1660 A1674 A1688 A1702 A1716 A1730 A1744 A1758 A1772 A1786 A1800 A1814 A1828 A1842 A1856 A1870 A1884 A1898 A1912 A1926 A1940 A1954 A1968 A1982 A1996 A2010">
-    <cfRule type="expression" dxfId="48" priority="5">
+    <cfRule type="expression" dxfId="52" priority="10">
       <formula>AND($L15&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:B17 A31:B31 A45:B45 A59:B59 A73:B73 A87:B87 A101:B101 A115:B115 A129:B129 A143:B143 A157:B157 A171:B171 A185:B185 A199:B199 A213:B213 A227:B227 A241:B241 A255:B255 A269:B269 A283:B283 A297:B297 A311:B311 A325:B325 A339:B339 A353:B353 A367:B367 A381:B381 A395:B395 A409:B409 A423:B423 A437:B437 A451:B451 A465:B465 A479:B479 A493:B493 A507:B507 A521:B521 A535:B535 A549:B549 A563:B563 A577:B577 A591:B591 A605:B605 A619:B619 A633:B633 A647:B647 A661:B661 A675:B675 A689:B689 A703:B703 A717:B717 A731:B731 A745:B745 A759:B759 A773:B773 A787:B787 A801:B801 A815:B815 A829:B829 A843:B843 A857:B857 A871:B871 A885:B885 A899:B899 A913:B913 A927:B927 A941:B941 A955:B955 A969:B969 A983:B983 A997:B997 A1011:B1011 A1025:B1025 A1039:B1039 A1053:B1053 A1067:B1067 A1081:B1081 A1095:B1095 A1109:B1109 A1123:B1123 A1137:B1137 A1151:B1151 A1165:B1165 A1179:B1179 A1193:B1193 A1207:B1207 A1221:B1221 A1235:B1235 A1249:B1249 A1263:B1263 A1277:B1277 A1291:B1291 A1305:B1305 A1319:B1319 A1333:B1333 A1347:B1347 A1361:B1361 A1375:B1375 A1389:B1389 A1403:B1403 A1417:B1417 A1431:B1431 A1445:B1445 A1459:B1459 A1473:B1473 A1487:B1487 A1501:B1501 A1515:B1515 A1529:B1529 A1543:B1543 A1557:B1557 A1571:B1571 A1585:B1585 A1599:B1599 A1613:B1613 A1627:B1627 A1641:B1641 A1655:B1655 A1669:B1669 A1683:B1683 A1697:B1697 A1711:B1711 A1725:B1725 A1739:B1739 A1753:B1753 A1767:B1767 A1781:B1781 A1795:B1795 A1809:B1809 A1823:B1823 A1837:B1837 A1851:B1851 A1865:B1865 A1879:B1879 A1893:B1893 A1907:B1907 A1921:B1921 A1935:B1935 A1949:B1949 A1963:B1963 A1977:B1977 A1991:B1991 A2005:B2005 A2019:B2019 A27:B27 A41:B41 A55:B55 A69:B69 A83:B83 A97:B97 A111:B111 A125:B125 A139:B139 A153:B153 A167:B167 A181:B181 A195:B195 A209:B209 A223:B223 A237:B237 A251:B251 A265:B265 A279:B279 A293:B293 A307:B307 A321:B321 A335:B335 A349:B349 A363:B363 A377:B377 A391:B391 A405:B405 A419:B419 A433:B433 A447:B447 A461:B461 A475:B475 A489:B489 A503:B503 A517:B517 A531:B531 A545:B545 A559:B559 A573:B573 A587:B587 A601:B601 A615:B615 A629:B629 A643:B643 A657:B657 A671:B671 A685:B685 A699:B699 A713:B713 A727:B727 A741:B741 A755:B755 A769:B769 A783:B783 A797:B797 A811:B811 A825:B825 A839:B839 A853:B853 A867:B867 A881:B881 A895:B895 A909:B909 A923:B923 A937:B937 A951:B951 A965:B965 A979:B979 A993:B993 A1007:B1007 A1021:B1021 A1035:B1035 A1049:B1049 A1063:B1063 A1077:B1077 A1091:B1091 A1105:B1105 A1119:B1119 A1133:B1133 A1147:B1147 A1161:B1161 A1175:B1175 A1189:B1189 A1203:B1203 A1217:B1217 A1231:B1231 A1245:B1245 A1259:B1259 A1273:B1273 A1287:B1287 A1301:B1301 A1315:B1315 A1329:B1329 A1343:B1343 A1357:B1357 A1371:B1371 A1385:B1385 A1399:B1399 A1413:B1413 A1427:B1427 A1441:B1441 A1455:B1455 A1469:B1469 A1483:B1483 A1497:B1497 A1511:B1511 A1525:B1525 A1539:B1539 A1553:B1553 A1567:B1567 A1581:B1581 A1595:B1595 A1609:B1609 A1623:B1623 A1637:B1637 A1651:B1651 A1665:B1665 A1679:B1679 A1693:B1693 A1707:B1707 A1721:B1721 A1735:B1735 A1749:B1749 A1763:B1763 A1777:B1777 A1791:B1791 A1805:B1805 A1819:B1819 A1833:B1833 A1847:B1847 A1861:B1861 A1875:B1875 A1889:B1889 A1903:B1903 A1917:B1917 A1931:B1931 A1945:B1945 A1959:B1959 A1973:B1973 A1987:B1987 A2001:B2001 A2015:B2015 A23 A37 A51 A65 A79 A93 A107 A121 A135 A149 A163 A177 A191 A205 A219 A233 A247 A261 A275 A289 A303 A317 A331 A345 A359 A373 A387 A401 A415 A429 A443 A457 A471 A485 A499 A513 A527 A541 A555 A569 A583 A597 A611 A625 A639 A653 A667 A681 A695 A709 A723 A737 A751 A765 A779 A793 A807 A821 A835 A849 A863 A877 A891 A905 A919 A933 A947 A961 A975 A989 A1003 A1017 A1031 A1045 A1059 A1073 A1087 A1101 A1115 A1129 A1143 A1157 A1171 A1185 A1199 A1213 A1227 A1241 A1255 A1269 A1283 A1297 A1311 A1325 A1339 A1353 A1367 A1381 A1395 A1409 A1423 A1437 A1451 A1465 A1479 A1493 A1507 A1521 A1535 A1549 A1563 A1577 A1591 A1605 A1619 A1633 A1647 A1661 A1675 A1689 A1703 A1717 A1731 A1745 A1759 A1773 A1787 A1801 A1815 A1829 A1843 A1857 A1871 A1885 A1899 A1913 A1927 A1941 A1955 A1969 A1983 A1997 A2011">
-    <cfRule type="expression" dxfId="47" priority="6">
+    <cfRule type="expression" dxfId="51" priority="11">
       <formula>AND(#REF!&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:B19 A33:B33 A47:B47 A61:B61 A75:B75 A89:B89 A103:B103 A117:B117 A131:B131 A145:B145 A159:B159 A173:B173 A187:B187 A201:B201 A215:B215 A229:B229 A243:B243 A257:B257 A271:B271 A285:B285 A299:B299 A313:B313 A327:B327 A341:B341 A355:B355 A369:B369 A383:B383 A397:B397 A411:B411 A425:B425 A439:B439 A453:B453 A467:B467 A481:B481 A495:B495 A509:B509 A523:B523 A537:B537 A551:B551 A565:B565 A579:B579 A593:B593 A607:B607 A621:B621 A635:B635 A649:B649 A663:B663 A677:B677 A691:B691 A705:B705 A719:B719 A733:B733 A747:B747 A761:B761 A775:B775 A789:B789 A803:B803 A817:B817 A831:B831 A845:B845 A859:B859 A873:B873 A887:B887 A901:B901 A915:B915 A929:B929 A943:B943 A957:B957 A971:B971 A985:B985 A999:B999 A1013:B1013 A1027:B1027 A1041:B1041 A1055:B1055 A1069:B1069 A1083:B1083 A1097:B1097 A1111:B1111 A1125:B1125 A1139:B1139 A1153:B1153 A1167:B1167 A1181:B1181 A1195:B1195 A1209:B1209 A1223:B1223 A1237:B1237 A1251:B1251 A1265:B1265 A1279:B1279 A1293:B1293 A1307:B1307 A1321:B1321 A1335:B1335 A1349:B1349 A1363:B1363 A1377:B1377 A1391:B1391 A1405:B1405 A1419:B1419 A1433:B1433 A1447:B1447 A1461:B1461 A1475:B1475 A1489:B1489 A1503:B1503 A1517:B1517 A1531:B1531 A1545:B1545 A1559:B1559 A1573:B1573 A1587:B1587 A1601:B1601 A1615:B1615 A1629:B1629 A1643:B1643 A1657:B1657 A1671:B1671 A1685:B1685 A1699:B1699 A1713:B1713 A1727:B1727 A1741:B1741 A1755:B1755 A1769:B1769 A1783:B1783 A1797:B1797 A1811:B1811 A1825:B1825 A1839:B1839 A1853:B1853 A1867:B1867 A1881:B1881 A1895:B1895 A1909:B1909 A1923:B1923 A1937:B1937 A1951:B1951 A1965:B1965 A1979:B1979 A1993:B1993 A2007:B2007 A2021:B2021 A29:B29 A43:B43 A57:B57 A71:B71 A85:B85 A99:B99 A113:B113 A127:B127 A141:B141 A155:B155 A169:B169 A183:B183 A197:B197 A211:B211 A225:B225 A239:B239 A253:B253 A267:B267 A281:B281 A295:B295 A309:B309 A323:B323 A337:B337 A351:B351 A365:B365 A379:B379 A393:B393 A407:B407 A421:B421 A435:B435 A449:B449 A463:B463 A477:B477 A491:B491 A505:B505 A519:B519 A533:B533 A547:B547 A561:B561 A575:B575 A589:B589 A603:B603 A617:B617 A631:B631 A645:B645 A659:B659 A673:B673 A687:B687 A701:B701 A715:B715 A729:B729 A743:B743 A757:B757 A771:B771 A785:B785 A799:B799 A813:B813 A827:B827 A841:B841 A855:B855 A869:B869 A883:B883 A897:B897 A911:B911 A925:B925 A939:B939 A953:B953 A967:B967 A981:B981 A995:B995 A1009:B1009 A1023:B1023 A1037:B1037 A1051:B1051 A1065:B1065 A1079:B1079 A1093:B1093 A1107:B1107 A1121:B1121 A1135:B1135 A1149:B1149 A1163:B1163 A1177:B1177 A1191:B1191 A1205:B1205 A1219:B1219 A1233:B1233 A1247:B1247 A1261:B1261 A1275:B1275 A1289:B1289 A1303:B1303 A1317:B1317 A1331:B1331 A1345:B1345 A1359:B1359 A1373:B1373 A1387:B1387 A1401:B1401 A1415:B1415 A1429:B1429 A1443:B1443 A1457:B1457 A1471:B1471 A1485:B1485 A1499:B1499 A1513:B1513 A1527:B1527 A1541:B1541 A1555:B1555 A1569:B1569 A1583:B1583 A1597:B1597 A1611:B1611 A1625:B1625 A1639:B1639 A1653:B1653 A1667:B1667 A1681:B1681 A1695:B1695 A1709:B1709 A1723:B1723 A1737:B1737 A1751:B1751 A1765:B1765 A1779:B1779 A1793:B1793 A1807:B1807 A1821:B1821 A1835:B1835 A1849:B1849 A1863:B1863 A1877:B1877 A1891:B1891 A1905:B1905 A1919:B1919 A1933:B1933 A1947:B1947 A1961:B1961 A1975:B1975 A1989:B1989 A2003:B2003 A2017:B2017 A25 A39 A53 A67 A81 A95 A109 A123 A137 A151 A165 A179 A193 A207 A221 A235 A249 A263 A277 A291 A305 A319 A333 A347 A361 A375 A389 A403 A417 A431 A445 A459 A473 A487 A501 A515 A529 A543 A557 A571 A585 A599 A613 A627 A641 A655 A669 A683 A697 A711 A725 A739 A753 A767 A781 A795 A809 A823 A837 A851 A865 A879 A893 A907 A921 A935 A949 A963 A977 A991 A1005 A1019 A1033 A1047 A1061 A1075 A1089 A1103 A1117 A1131 A1145 A1159 A1173 A1187 A1201 A1215 A1229 A1243 A1257 A1271 A1285 A1299 A1313 A1327 A1341 A1355 A1369 A1383 A1397 A1411 A1425 A1439 A1453 A1467 A1481 A1495 A1509 A1523 A1537 A1551 A1565 A1579 A1593 A1607 A1621 A1635 A1649 A1663 A1677 A1691 A1705 A1719 A1733 A1747 A1761 A1775 A1789 A1803 A1817 A1831 A1845 A1859 A1873 A1887 A1901 A1915 A1929 A1943 A1957 A1971 A1985 A1999 A2013">
-    <cfRule type="expression" dxfId="46" priority="7">
+    <cfRule type="expression" dxfId="50" priority="12">
       <formula>AND(#REF!&lt;&gt;"",MOD(ROW(),2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2022:B2022">
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>#REF!=ROW()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2022:B2022">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2022:B2022">
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>AND($L2007&lt;&gt;"",MOD(ROW(),2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2022:B2022">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>AND($L2020&lt;&gt;"",MOD(ROW(),2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2022:B2022">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND($L2019&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23933,19 +24031,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A690538-64CC-4629-ABCB-DDD9EB61421C}">
-  <sheetPr codeName="Feuil4"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DDC857-10E7-4C20-A5AB-56FF0B802DF5}">
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:D5"/>
@@ -24035,55 +24120,54 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:C5">
-    <cfRule type="expression" dxfId="45" priority="16">
+    <cfRule type="expression" dxfId="49" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="17">
-      <formula>#REF!=ROW()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="20">
+    <cfRule type="expression" dxfId="48" priority="20">
       <formula>AND($M1048563&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:D2">
-    <cfRule type="expression" dxfId="42" priority="22">
+    <cfRule type="expression" dxfId="47" priority="22">
       <formula>AND($M1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="32">
+    <cfRule type="expression" dxfId="46" priority="32">
       <formula>AND($M1046559&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A2:D5">
+    <cfRule type="expression" dxfId="45" priority="4">
+      <formula>#REF!=ROW()</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A3:D3">
-    <cfRule type="expression" dxfId="40" priority="21">
+    <cfRule type="expression" dxfId="44" priority="21">
       <formula>AND(#REF!&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="23">
+    <cfRule type="expression" dxfId="43" priority="23">
       <formula>AND(#REF!&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:D4">
-    <cfRule type="expression" dxfId="38" priority="15">
+    <cfRule type="expression" dxfId="42" priority="15">
       <formula>AND($M1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:D5">
-    <cfRule type="expression" dxfId="37" priority="18">
+    <cfRule type="expression" dxfId="41" priority="18">
       <formula>AND($M2&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:D5">
-    <cfRule type="expression" dxfId="36" priority="24">
+    <cfRule type="expression" dxfId="40" priority="24">
       <formula>AND(#REF!&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D5">
-    <cfRule type="expression" dxfId="35" priority="3">
+    <cfRule type="expression" dxfId="39" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="4">
-      <formula>#REF!=ROW()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="7">
+    <cfRule type="expression" dxfId="38" priority="7">
       <formula>AND($L1048563&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24091,7 +24175,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E737781B-436D-488E-AD45-0F19C0E292DB}">
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:C10"/>
@@ -24221,29 +24305,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:C2 A4:C4 A6:C6 A8:C8 A10:C10">
-    <cfRule type="expression" dxfId="32" priority="13">
+    <cfRule type="expression" dxfId="37" priority="13">
       <formula>AND($L1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="16">
+    <cfRule type="expression" dxfId="36" priority="16">
       <formula>AND($L1046559&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:C10">
-    <cfRule type="expression" dxfId="30" priority="1">
+    <cfRule type="expression" dxfId="35" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="2">
+    <cfRule type="expression" dxfId="34" priority="2">
       <formula>#REF!=ROW()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="3">
+    <cfRule type="expression" dxfId="33" priority="3">
       <formula>AND($K1048563&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:C3 A5:C5 A7:C7 A9:C9">
-    <cfRule type="expression" dxfId="27" priority="12">
+    <cfRule type="expression" dxfId="32" priority="12">
       <formula>AND(#REF!&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="14">
+    <cfRule type="expression" dxfId="31" priority="14">
       <formula>AND(#REF!&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24251,13 +24335,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07C88F7-C961-4594-AD1B-F2D5F8D5E029}">
   <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:M2018"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31013,128 +31097,128 @@
     <sortCondition ref="C2:C62"/>
   </sortState>
   <conditionalFormatting sqref="A2:B52 A8:A62">
-    <cfRule type="expression" dxfId="25" priority="8">
+    <cfRule type="expression" dxfId="30" priority="8">
       <formula>AND($L1048563&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52:B62">
-    <cfRule type="expression" dxfId="24" priority="21">
+    <cfRule type="expression" dxfId="29" priority="21">
       <formula>AND($M36&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:D2 A8 A14 A20 A26 A32 A38 A44 A50 A56 A62">
-    <cfRule type="expression" dxfId="23" priority="24">
+    <cfRule type="expression" dxfId="28" priority="24">
       <formula>AND($L1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:D2 A4:D4 A7:D8 A10 A13:A14 A16 A19:A20 A22 A25:A26 A28 A31:A32 A34 A37:A38 A40 A43:A44 A46 A49:A50 A52 A55:A56 A58 A61:A62">
-    <cfRule type="expression" dxfId="22" priority="3">
+    <cfRule type="expression" dxfId="27" priority="3">
       <formula>AND($L1048575&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:D21 A8:A62">
-    <cfRule type="expression" dxfId="21" priority="5">
+    <cfRule type="expression" dxfId="26" priority="5">
       <formula>#REF!=ROW()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:D62">
-    <cfRule type="expression" dxfId="20" priority="4">
+    <cfRule type="expression" dxfId="25" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:D3 A9 A15 A21 A27 A33 A39 A45 A51 A57">
-    <cfRule type="expression" dxfId="19" priority="15">
+    <cfRule type="expression" dxfId="24" priority="15">
       <formula>AND(#REF!&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="26">
+    <cfRule type="expression" dxfId="23" priority="26">
       <formula>AND(#REF!&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:D8 A10:A13 A16:A19 A22:A25 A28:A31 A34:A37 A40:A43 A46:A49 A52:A55 A58:A61">
-    <cfRule type="expression" dxfId="17" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>AND($L2&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:D5 A11 A17 A23 A29 A35 A41 A47 A53 A59">
-    <cfRule type="expression" dxfId="16" priority="30">
+    <cfRule type="expression" dxfId="21" priority="30">
       <formula>AND(#REF!&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:D41 A42:A43 A48:A49 A54:A55 A60:A61">
-    <cfRule type="expression" dxfId="15" priority="7">
+    <cfRule type="expression" dxfId="20" priority="7">
       <formula>AND($L2&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:D42">
-    <cfRule type="expression" dxfId="14" priority="17">
+    <cfRule type="expression" dxfId="19" priority="17">
       <formula>AND($L49&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43:D44">
-    <cfRule type="expression" dxfId="13" priority="19">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>AND($L51&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45:D45">
-    <cfRule type="expression" dxfId="12" priority="9">
+    <cfRule type="expression" dxfId="17" priority="9">
       <formula>AND(#REF!&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46:D48">
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="16" priority="13">
       <formula>AND($L78&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:D52">
-    <cfRule type="expression" dxfId="10" priority="10">
+    <cfRule type="expression" dxfId="15" priority="10">
       <formula>AND($L83&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:D52">
-    <cfRule type="expression" dxfId="9" priority="16">
+    <cfRule type="expression" dxfId="14" priority="16">
       <formula>AND($L35&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52:D52">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>AND($L85&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>AND($L35&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:D54">
-    <cfRule type="expression" dxfId="6" priority="23">
+    <cfRule type="expression" dxfId="11" priority="23">
       <formula>AND($L36&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:D62">
-    <cfRule type="expression" dxfId="5" priority="22">
+    <cfRule type="expression" dxfId="10" priority="22">
       <formula>AND($L86&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55:D55">
-    <cfRule type="expression" dxfId="4" priority="18">
+    <cfRule type="expression" dxfId="9" priority="18">
       <formula>AND($L49&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:D57">
-    <cfRule type="expression" dxfId="3" priority="20">
+    <cfRule type="expression" dxfId="8" priority="20">
       <formula>AND($L51&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:D58">
-    <cfRule type="expression" dxfId="2" priority="11">
+    <cfRule type="expression" dxfId="7" priority="11">
       <formula>AND(#REF!&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:D61">
-    <cfRule type="expression" dxfId="1" priority="14">
+    <cfRule type="expression" dxfId="6" priority="14">
       <formula>AND($L78&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:D62">
-    <cfRule type="expression" dxfId="0" priority="12">
+    <cfRule type="expression" dxfId="5" priority="12">
       <formula>AND($L83&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
2024-10-03 @ 12:48 - v4.J.2
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250D73FC-9244-4981-8511-4B39A4983D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D004EE-D414-4BF2-B864-271B6D1A1637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11897" uniqueCount="6998">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11923" uniqueCount="7011">
   <si>
     <t>Client_ID</t>
   </si>
@@ -21044,6 +21044,45 @@
   </si>
   <si>
     <t>H1W 2W9</t>
+  </si>
+  <si>
+    <t>Construction Nelson Inc. [Nelson Massicotte]</t>
+  </si>
+  <si>
+    <t>1803</t>
+  </si>
+  <si>
+    <t>Nelson Massicotte</t>
+  </si>
+  <si>
+    <t>106-742 Notre-Dame</t>
+  </si>
+  <si>
+    <t>J5W 3W7</t>
+  </si>
+  <si>
+    <t>Nicholas Boulard</t>
+  </si>
+  <si>
+    <t>9327-2193 Québec Inc. [Suzanne Harel]</t>
+  </si>
+  <si>
+    <t>1804</t>
+  </si>
+  <si>
+    <t>Suzanne Harel</t>
+  </si>
+  <si>
+    <t>suharel@me.com</t>
+  </si>
+  <si>
+    <t>1045 place Joseph-Tassé</t>
+  </si>
+  <si>
+    <t>H7X 3L4</t>
+  </si>
+  <si>
+    <t>Inconnues</t>
   </si>
 </sst>
 </file>
@@ -22111,31 +22150,31 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
   <sheetPr codeName="wshClients"/>
-  <dimension ref="A1:O1093"/>
+  <dimension ref="A1:O1095"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A585" activePane="bottomLeft"/>
+      <pane ySplit="612" topLeftCell="A585" activePane="bottomLeft"/>
       <selection activeCell="M1" sqref="M1:M1048576"/>
       <selection pane="bottomLeft" activeCell="A594" sqref="A594:XFD594"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="55.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="33.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.85546875" style="21" customWidth="1"/>
+    <col min="1" max="1" width="55.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.109375" style="21" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.88671875" style="21" customWidth="1"/>
     <col min="6" max="6" width="32" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="42.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.28515625" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42.44140625" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" style="47" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -22204,6 +22243,9 @@
       <c r="F2" s="3" t="s">
         <v>179</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>7010</v>
+      </c>
       <c r="H2" s="3" t="s">
         <v>180</v>
       </c>
@@ -61528,6 +61570,85 @@
       </c>
       <c r="O1093" t="s">
         <v>1479</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:15">
+      <c r="A1094" s="3" t="s">
+        <v>6998</v>
+      </c>
+      <c r="B1094" s="24" t="s">
+        <v>6999</v>
+      </c>
+      <c r="C1094" s="21" t="s">
+        <v>7000</v>
+      </c>
+      <c r="D1094" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1094" s="3" t="s">
+        <v>7001</v>
+      </c>
+      <c r="H1094" s="3" t="s">
+        <v>1545</v>
+      </c>
+      <c r="I1094" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="J1094" s="22" t="s">
+        <v>7002</v>
+      </c>
+      <c r="K1094" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="L1094" t="s">
+        <v>7003</v>
+      </c>
+      <c r="M1094" s="47" t="s">
+        <v>5818</v>
+      </c>
+      <c r="N1094" t="s">
+        <v>7003</v>
+      </c>
+      <c r="O1094" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:15">
+      <c r="A1095" s="3" t="s">
+        <v>7004</v>
+      </c>
+      <c r="B1095" s="24" t="s">
+        <v>7005</v>
+      </c>
+      <c r="C1095" s="21" t="s">
+        <v>7006</v>
+      </c>
+      <c r="D1095" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1095" s="21" t="s">
+        <v>7007</v>
+      </c>
+      <c r="F1095" s="3" t="s">
+        <v>7008</v>
+      </c>
+      <c r="H1095" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I1095" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="J1095" s="22" t="s">
+        <v>7009</v>
+      </c>
+      <c r="K1095" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="L1095" t="s">
+        <v>279</v>
+      </c>
+      <c r="N1095" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -61823,26 +61944,26 @@
   <dimension ref="A1:O63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="615"/>
+      <pane ySplit="612"/>
       <selection sqref="A1:XFD1048576"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="56.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" style="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="11.5703125" style="1"/>
+    <col min="11" max="11" width="17.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -63714,18 +63835,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" style="2" customWidth="1"/>
-    <col min="10" max="13" width="11.5703125" style="1"/>
+    <col min="1" max="1" width="33.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="17" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" style="2" customWidth="1"/>
+    <col min="10" max="13" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -64661,7 +64782,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15.75" thickBot="1">
+    <row r="67" spans="1:4" ht="15" thickBot="1">
       <c r="A67" s="12" t="s">
         <v>128</v>
       </c>

</xml_diff>

<commit_message>
2024-10-04 @ 00:44 - v4.J.3.xlsb
Ajustements aux trois principaux log
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D004EE-D414-4BF2-B864-271B6D1A1637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93311A1-5D36-4E40-A224-5AA4F83E3C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11923" uniqueCount="7011">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11922" uniqueCount="7010">
   <si>
     <t>Client_ID</t>
   </si>
@@ -21080,9 +21080,6 @@
   </si>
   <si>
     <t>H7X 3L4</t>
-  </si>
-  <si>
-    <t>Inconnues</t>
   </si>
 </sst>
 </file>
@@ -22153,28 +22150,28 @@
   <dimension ref="A1:O1095"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="612" topLeftCell="A585" activePane="bottomLeft"/>
+      <pane ySplit="615" topLeftCell="A585" activePane="bottomLeft"/>
       <selection activeCell="M1" sqref="M1:M1048576"/>
       <selection pane="bottomLeft" activeCell="A594" sqref="A594:XFD594"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.109375" style="21" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.88671875" style="21" customWidth="1"/>
+    <col min="1" max="1" width="55.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.85546875" style="21" customWidth="1"/>
     <col min="6" max="6" width="32" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="42.44140625" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" style="47" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.33203125" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -22242,9 +22239,6 @@
       </c>
       <c r="F2" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>7010</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>180</v>
@@ -61944,26 +61938,26 @@
   <dimension ref="A1:O63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="612"/>
+      <pane ySplit="615"/>
       <selection sqref="A1:XFD1048576"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.44140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="11.5546875" style="1"/>
+    <col min="11" max="11" width="17.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -63835,18 +63829,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.6640625" style="2" customWidth="1"/>
-    <col min="10" max="13" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="33.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" style="2" customWidth="1"/>
+    <col min="10" max="13" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -64782,7 +64776,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" thickBot="1">
+    <row r="67" spans="1:4" ht="15.75" thickBot="1">
       <c r="A67" s="12" t="s">
         <v>128</v>
       </c>

</xml_diff>

<commit_message>
2024-10-11 @ 17:17 - v4.K.2.xlsb
* modFAC_Brouillon
   - Prendre la date du jour comme date par défaut, et non celle du projet de facture
   - Traitement des paires multiples de crochets dans le nom de client
   - Traitement particulier pour les charges postérieures au projet de facture (case non cochée + Message)
* modStatsHeures
   - Beaucoup de travail pour créer des Pivot Tables (semaine, mois, trimestre & année)
*modTEC_Saisie
   - Pousser les nouvelles charges dans TEC_TDB_Data pour avoir des Pivot Tables à jour
   - Nouveaux sous-totaux (4) pour montrer les Hres/FACT & Hres/NonFACT pour le jour et la semaine
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9670F60D-2B76-4816-B1A7-52E05107E01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E4E0D3-D172-4E25-BE9D-B646B1ED814D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="30960" windowHeight="12204" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11949" uniqueCount="7023">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11974" uniqueCount="7037">
   <si>
     <t>Client_ID</t>
   </si>
@@ -21043,12 +21043,6 @@
     <t>suharel@me.com</t>
   </si>
   <si>
-    <t>1045 place Joseph-Tassé</t>
-  </si>
-  <si>
-    <t>H7X 3L4</t>
-  </si>
-  <si>
     <t>Agence Code Communications Inc. [Mme France Daniel]</t>
   </si>
   <si>
@@ -21119,6 +21113,54 @@
   </si>
   <si>
     <t>Iberville</t>
+  </si>
+  <si>
+    <t>9259-5362 Québec Inc. (Parler Plus) [Rosalie G. Hogue]</t>
+  </si>
+  <si>
+    <t>2053</t>
+  </si>
+  <si>
+    <t>Rosalie G. Hogue</t>
+  </si>
+  <si>
+    <t>rosalie@parlerplus.ca</t>
+  </si>
+  <si>
+    <t>105-3195 Boul. de la pinière</t>
+  </si>
+  <si>
+    <t>J6X4P7</t>
+  </si>
+  <si>
+    <t>Immeubles Marklin C2 Inc. [Caroline Chaput]</t>
+  </si>
+  <si>
+    <t>2054</t>
+  </si>
+  <si>
+    <t>Caroline Chaput</t>
+  </si>
+  <si>
+    <t>info@immeublesmarklin.com</t>
+  </si>
+  <si>
+    <t>9 rue Saint-Pierre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Québec </t>
+  </si>
+  <si>
+    <t>J5A 1A1</t>
+  </si>
+  <si>
+    <t>Leblanc Notaires</t>
+  </si>
+  <si>
+    <t>574 rue Principale</t>
+  </si>
+  <si>
+    <t>H7X 1C9</t>
   </si>
 </sst>
 </file>
@@ -22192,31 +22234,31 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
   <sheetPr codeName="wshClients"/>
-  <dimension ref="A1:O1097"/>
+  <dimension ref="A1:O1099"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <pane ySplit="612" topLeftCell="A26" activePane="bottomLeft"/>
+      <pane ySplit="615" topLeftCell="A26" activePane="bottomLeft"/>
       <selection activeCell="B41" sqref="B1:B1048576"/>
       <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.109375" style="21" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.88671875" style="21" customWidth="1"/>
+    <col min="1" max="1" width="55.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.85546875" style="21" customWidth="1"/>
     <col min="6" max="6" width="32" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="42.44140625" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" style="46" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" style="46" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -22304,7 +22346,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="3" t="s">
-        <v>7018</v>
+        <v>7016</v>
       </c>
       <c r="B6" s="49" t="s">
         <v>2350</v>
@@ -33340,7 +33382,7 @@
     </row>
     <row r="340" spans="1:15">
       <c r="A340" s="3" t="s">
-        <v>7010</v>
+        <v>7008</v>
       </c>
       <c r="B340" s="49" t="s">
         <v>5338</v>
@@ -37842,7 +37884,7 @@
     </row>
     <row r="460" spans="1:15">
       <c r="A460" s="3" t="s">
-        <v>7001</v>
+        <v>6999</v>
       </c>
       <c r="B460" s="49" t="s">
         <v>5516</v>
@@ -60550,7 +60592,7 @@
         <v>6996</v>
       </c>
       <c r="F1069" s="3" t="s">
-        <v>6997</v>
+        <v>7035</v>
       </c>
       <c r="H1069" s="3" t="s">
         <v>180</v>
@@ -60559,7 +60601,7 @@
         <v>575</v>
       </c>
       <c r="J1069" s="22" t="s">
-        <v>6998</v>
+        <v>7036</v>
       </c>
       <c r="K1069" s="22" t="s">
         <v>156</v>
@@ -60573,22 +60615,22 @@
     </row>
     <row r="1070" spans="1:15">
       <c r="A1070" s="3" t="s">
+        <v>7009</v>
+      </c>
+      <c r="B1070" s="49" t="s">
+        <v>7010</v>
+      </c>
+      <c r="C1070" s="21" t="s">
         <v>7011</v>
-      </c>
-      <c r="B1070" s="49" t="s">
-        <v>7012</v>
-      </c>
-      <c r="C1070" s="21" t="s">
-        <v>7013</v>
       </c>
       <c r="D1070" s="23" t="s">
         <v>835</v>
       </c>
       <c r="E1070" s="21" t="s">
-        <v>7014</v>
+        <v>7012</v>
       </c>
       <c r="F1070" s="3" t="s">
-        <v>7015</v>
+        <v>7013</v>
       </c>
       <c r="H1070" s="3" t="s">
         <v>2257</v>
@@ -60597,13 +60639,13 @@
         <v>575</v>
       </c>
       <c r="J1070" s="22" t="s">
-        <v>7016</v>
+        <v>7014</v>
       </c>
       <c r="K1070" s="22" t="s">
         <v>156</v>
       </c>
       <c r="L1070" t="s">
-        <v>7017</v>
+        <v>7015</v>
       </c>
       <c r="M1070" s="46" t="s">
         <v>2761</v>
@@ -60658,13 +60700,13 @@
     </row>
     <row r="1072" spans="1:15">
       <c r="A1072" s="3" t="s">
-        <v>7002</v>
+        <v>7000</v>
       </c>
       <c r="B1072" s="49" t="s">
         <v>5815</v>
       </c>
       <c r="C1072" s="21" t="s">
-        <v>7005</v>
+        <v>7003</v>
       </c>
       <c r="D1072" s="23" t="s">
         <v>171</v>
@@ -60700,13 +60742,13 @@
     </row>
     <row r="1073" spans="1:15">
       <c r="A1073" s="3" t="s">
-        <v>6999</v>
+        <v>6997</v>
       </c>
       <c r="B1073" s="49" t="s">
         <v>5816</v>
       </c>
       <c r="C1073" s="21" t="s">
-        <v>7006</v>
+        <v>7004</v>
       </c>
       <c r="D1073" s="23" t="s">
         <v>175</v>
@@ -60742,13 +60784,13 @@
     </row>
     <row r="1074" spans="1:15">
       <c r="A1074" s="3" t="s">
-        <v>7003</v>
+        <v>7001</v>
       </c>
       <c r="B1074" s="49" t="s">
         <v>5817</v>
       </c>
       <c r="C1074" s="21" t="s">
-        <v>7007</v>
+        <v>7005</v>
       </c>
       <c r="D1074" s="23" t="s">
         <v>171</v>
@@ -60914,13 +60956,13 @@
     </row>
     <row r="1078" spans="1:15">
       <c r="A1078" s="3" t="s">
-        <v>7004</v>
+        <v>7002</v>
       </c>
       <c r="B1078" s="49" t="s">
         <v>5820</v>
       </c>
       <c r="C1078" s="21" t="s">
-        <v>7008</v>
+        <v>7006</v>
       </c>
       <c r="D1078" s="23" t="s">
         <v>2283</v>
@@ -61302,13 +61344,13 @@
     </row>
     <row r="1087" spans="1:15">
       <c r="A1087" s="3" t="s">
-        <v>7000</v>
+        <v>6998</v>
       </c>
       <c r="B1087" s="49" t="s">
         <v>5831</v>
       </c>
       <c r="C1087" s="21" t="s">
-        <v>7009</v>
+        <v>7007</v>
       </c>
       <c r="D1087" s="23" t="s">
         <v>858</v>
@@ -61733,13 +61775,13 @@
     </row>
     <row r="1097" spans="1:15">
       <c r="A1097" s="3" t="s">
+        <v>7017</v>
+      </c>
+      <c r="B1097" s="49" t="s">
+        <v>7018</v>
+      </c>
+      <c r="C1097" s="21" t="s">
         <v>7019</v>
-      </c>
-      <c r="B1097" s="49" t="s">
-        <v>7020</v>
-      </c>
-      <c r="C1097" s="21" t="s">
-        <v>7021</v>
       </c>
       <c r="D1097" s="23" t="s">
         <v>172</v>
@@ -61751,7 +61793,7 @@
         <v>2887</v>
       </c>
       <c r="H1097" s="3" t="s">
-        <v>7022</v>
+        <v>7020</v>
       </c>
       <c r="I1097" s="22" t="s">
         <v>575</v>
@@ -61773,6 +61815,85 @@
       </c>
       <c r="O1097" t="s">
         <v>5354</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:15">
+      <c r="A1098" s="3" t="s">
+        <v>7021</v>
+      </c>
+      <c r="B1098" s="49" t="s">
+        <v>7022</v>
+      </c>
+      <c r="C1098" s="21" t="s">
+        <v>7023</v>
+      </c>
+      <c r="E1098" s="21" t="s">
+        <v>7024</v>
+      </c>
+      <c r="F1098" s="3" t="s">
+        <v>7025</v>
+      </c>
+      <c r="H1098" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1098" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="J1098" s="22" t="s">
+        <v>7026</v>
+      </c>
+      <c r="K1098" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="L1098" t="s">
+        <v>2760</v>
+      </c>
+      <c r="M1098" s="46" t="s">
+        <v>2761</v>
+      </c>
+      <c r="N1098" t="s">
+        <v>2760</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:15">
+      <c r="A1099" s="3" t="s">
+        <v>7027</v>
+      </c>
+      <c r="B1099" s="49" t="s">
+        <v>7028</v>
+      </c>
+      <c r="C1099" s="21" t="s">
+        <v>7029</v>
+      </c>
+      <c r="E1099" s="21" t="s">
+        <v>7030</v>
+      </c>
+      <c r="F1099" s="3" t="s">
+        <v>7031</v>
+      </c>
+      <c r="H1099" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="I1099" s="22" t="s">
+        <v>7032</v>
+      </c>
+      <c r="J1099" s="22" t="s">
+        <v>7033</v>
+      </c>
+      <c r="K1099" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="L1099" t="s">
+        <v>816</v>
+      </c>
+      <c r="M1099" s="46" t="s">
+        <v>5633</v>
+      </c>
+      <c r="N1099" t="s">
+        <v>816</v>
+      </c>
+      <c r="O1099" t="s">
+        <v>7034</v>
       </c>
     </row>
   </sheetData>
@@ -62073,26 +62194,26 @@
   <dimension ref="A1:O63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="612"/>
+      <pane ySplit="615"/>
       <selection sqref="A1:XFD1048576"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.44140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="11.5546875" style="1"/>
+    <col min="11" max="11" width="17.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -63964,18 +64085,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.6640625" style="2" customWidth="1"/>
-    <col min="10" max="13" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="33.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" style="2" customWidth="1"/>
+    <col min="10" max="13" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -64911,7 +65032,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" thickBot="1">
+    <row r="67" spans="1:4" ht="15.75" thickBot="1">
       <c r="A67" s="12" t="s">
         <v>128</v>
       </c>

</xml_diff>

<commit_message>
2024-10-12 @ 19:34 - v4.K.2.xlsb
* modAppli.bas
   - Nouvelle procédure pour mettre à jour (update) les 4 pivot tables (stats heures)
* modFunctions.bas
   - Nouvelle fonction pour valider les fractions d'heures
* modStatsHeures.bas
   - Mise en commentaire d'une procedure 'CreatePivotWithSoecificSorting'
   - Routine pour retourner au ufSaisieHeures (X)
* ufSaisieHeures.frm
   - Déplacer du code de AfterUpdate vers Exit pour txtHeures
   - Validation de la partie fractionnaire des heures
   - Possibilité d'accéder aux 4 pivot tables pour les statistiques d'heures à partir d'une nouvelle image
* wshStatsHeuresPivotTables.doccls
   - Worksheet_Activate
   - Worksheet Change
* wshTEC_Analyse.doccls
   - Ajout des lignes 258 & 259
* wshTEC_TDB_Data.doccls
   - Déplacer la procédure 'UpdatePivotTables' vers ...
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E4E0D3-D172-4E25-BE9D-B646B1ED814D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70BC032-239E-45E6-AFA2-668E84A63C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Clients!$A$1:$O$1096</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Clients!$A$1:$O$1098</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Fournisseurs!$A$1:$K$20</definedName>
     <definedName name="dnrClients" localSheetId="0">OFFSET(Clients!#REF!,1,0,COUNTA(Clients!$A:$A)-1,2)</definedName>
     <definedName name="dnrClients" localSheetId="1">OFFSET(Fournisseurs!$A$1,1,0,COUNTA(Fournisseurs!$A:$A)-1,2)</definedName>
@@ -21118,9 +21118,6 @@
     <t>9259-5362 Québec Inc. (Parler Plus) [Rosalie G. Hogue]</t>
   </si>
   <si>
-    <t>2053</t>
-  </si>
-  <si>
     <t>Rosalie G. Hogue</t>
   </si>
   <si>
@@ -21136,9 +21133,6 @@
     <t>Immeubles Marklin C2 Inc. [Caroline Chaput]</t>
   </si>
   <si>
-    <t>2054</t>
-  </si>
-  <si>
     <t>Caroline Chaput</t>
   </si>
   <si>
@@ -21161,6 +21155,12 @@
   </si>
   <si>
     <t>H7X 1C9</t>
+  </si>
+  <si>
+    <t>1806</t>
+  </si>
+  <si>
+    <t>1807</t>
   </si>
 </sst>
 </file>
@@ -22237,9 +22237,9 @@
   <dimension ref="A1:O1099"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A26" activePane="bottomLeft"/>
+      <pane ySplit="615" topLeftCell="A1066" activePane="bottomLeft"/>
       <selection activeCell="B41" sqref="B1:B1048576"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+      <selection pane="bottomLeft" activeCell="A1078" sqref="A1078"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -60592,7 +60592,7 @@
         <v>6996</v>
       </c>
       <c r="F1069" s="3" t="s">
-        <v>7035</v>
+        <v>7033</v>
       </c>
       <c r="H1069" s="3" t="s">
         <v>180</v>
@@ -60601,7 +60601,7 @@
         <v>575</v>
       </c>
       <c r="J1069" s="22" t="s">
-        <v>7036</v>
+        <v>7034</v>
       </c>
       <c r="K1069" s="22" t="s">
         <v>156</v>
@@ -60656,117 +60656,110 @@
     </row>
     <row r="1071" spans="1:15">
       <c r="A1071" s="3" t="s">
-        <v>6579</v>
+        <v>7021</v>
       </c>
       <c r="B1071" s="49" t="s">
-        <v>46</v>
+        <v>7035</v>
       </c>
       <c r="C1071" s="21" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D1071" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="E1071" s="32" t="s">
-        <v>2268</v>
+        <v>7022</v>
+      </c>
+      <c r="E1071" s="21" t="s">
+        <v>7023</v>
       </c>
       <c r="F1071" s="3" t="s">
-        <v>2269</v>
+        <v>7024</v>
       </c>
       <c r="H1071" s="3" t="s">
-        <v>2248</v>
+        <v>224</v>
       </c>
       <c r="I1071" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1071" s="22" t="s">
-        <v>2270</v>
+        <v>7025</v>
       </c>
       <c r="K1071" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="L1071" s="25" t="s">
-        <v>323</v>
-      </c>
-      <c r="M1071" s="24" t="s">
-        <v>5814</v>
-      </c>
-      <c r="N1071" s="25" t="s">
-        <v>323</v>
-      </c>
-      <c r="O1071" s="25" t="s">
-        <v>5354</v>
+      <c r="L1071" t="s">
+        <v>2760</v>
+      </c>
+      <c r="M1071" s="46" t="s">
+        <v>2761</v>
+      </c>
+      <c r="N1071" t="s">
+        <v>2760</v>
       </c>
     </row>
     <row r="1072" spans="1:15">
       <c r="A1072" s="3" t="s">
-        <v>7000</v>
+        <v>7026</v>
       </c>
       <c r="B1072" s="49" t="s">
-        <v>5815</v>
+        <v>7036</v>
       </c>
       <c r="C1072" s="21" t="s">
-        <v>7003</v>
-      </c>
-      <c r="D1072" s="23" t="s">
-        <v>171</v>
+        <v>7027</v>
       </c>
       <c r="E1072" s="21" t="s">
-        <v>5845</v>
+        <v>7028</v>
       </c>
       <c r="F1072" s="3" t="s">
-        <v>2271</v>
+        <v>7029</v>
       </c>
       <c r="H1072" s="3" t="s">
-        <v>2248</v>
+        <v>283</v>
       </c>
       <c r="I1072" s="22" t="s">
-        <v>575</v>
+        <v>7030</v>
       </c>
       <c r="J1072" s="22" t="s">
-        <v>2272</v>
+        <v>7031</v>
       </c>
       <c r="K1072" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="L1072" s="25" t="s">
-        <v>323</v>
-      </c>
-      <c r="M1072" s="24" t="s">
-        <v>2761</v>
-      </c>
-      <c r="N1072" s="25" t="s">
-        <v>323</v>
-      </c>
-      <c r="O1072" s="25"/>
+      <c r="L1072" t="s">
+        <v>816</v>
+      </c>
+      <c r="M1072" s="46" t="s">
+        <v>5633</v>
+      </c>
+      <c r="N1072" t="s">
+        <v>816</v>
+      </c>
+      <c r="O1072" t="s">
+        <v>7032</v>
+      </c>
     </row>
     <row r="1073" spans="1:15">
       <c r="A1073" s="3" t="s">
-        <v>6997</v>
+        <v>6579</v>
       </c>
       <c r="B1073" s="49" t="s">
-        <v>5816</v>
+        <v>46</v>
       </c>
       <c r="C1073" s="21" t="s">
-        <v>7004</v>
+        <v>2267</v>
       </c>
       <c r="D1073" s="23" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E1073" s="32" t="s">
-        <v>2273</v>
+        <v>2268</v>
       </c>
       <c r="F1073" s="3" t="s">
-        <v>2274</v>
+        <v>2269</v>
       </c>
       <c r="H1073" s="3" t="s">
-        <v>254</v>
+        <v>2248</v>
       </c>
       <c r="I1073" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1073" s="22" t="s">
-        <v>2275</v>
+        <v>2270</v>
       </c>
       <c r="K1073" s="22" t="s">
         <v>156</v>
@@ -60775,40 +60768,42 @@
         <v>323</v>
       </c>
       <c r="M1073" s="24" t="s">
-        <v>5633</v>
+        <v>5814</v>
       </c>
       <c r="N1073" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="O1073" s="25"/>
+      <c r="O1073" s="25" t="s">
+        <v>5354</v>
+      </c>
     </row>
     <row r="1074" spans="1:15">
       <c r="A1074" s="3" t="s">
-        <v>7001</v>
+        <v>7000</v>
       </c>
       <c r="B1074" s="49" t="s">
-        <v>5817</v>
+        <v>5815</v>
       </c>
       <c r="C1074" s="21" t="s">
-        <v>7005</v>
+        <v>7003</v>
       </c>
       <c r="D1074" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="E1074" s="32" t="s">
-        <v>1585</v>
+      <c r="E1074" s="21" t="s">
+        <v>5845</v>
       </c>
       <c r="F1074" s="3" t="s">
-        <v>2276</v>
+        <v>2271</v>
       </c>
       <c r="H1074" s="3" t="s">
-        <v>157</v>
+        <v>2248</v>
       </c>
       <c r="I1074" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1074" s="22" t="s">
-        <v>1587</v>
+        <v>2272</v>
       </c>
       <c r="K1074" s="22" t="s">
         <v>156</v>
@@ -60822,37 +60817,35 @@
       <c r="N1074" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="O1074" s="25" t="s">
-        <v>5354</v>
-      </c>
+      <c r="O1074" s="25"/>
     </row>
     <row r="1075" spans="1:15">
       <c r="A1075" s="3" t="s">
-        <v>6580</v>
+        <v>6997</v>
       </c>
       <c r="B1075" s="49" t="s">
-        <v>5818</v>
+        <v>5816</v>
       </c>
       <c r="C1075" s="21" t="s">
-        <v>2277</v>
+        <v>7004</v>
       </c>
       <c r="D1075" s="23" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E1075" s="32" t="s">
-        <v>2278</v>
+        <v>2273</v>
       </c>
       <c r="F1075" s="3" t="s">
-        <v>2279</v>
+        <v>2274</v>
       </c>
       <c r="H1075" s="3" t="s">
-        <v>2280</v>
+        <v>254</v>
       </c>
       <c r="I1075" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1075" s="22" t="s">
-        <v>2281</v>
+        <v>2275</v>
       </c>
       <c r="K1075" s="22" t="s">
         <v>156</v>
@@ -60861,7 +60854,7 @@
         <v>323</v>
       </c>
       <c r="M1075" s="24" t="s">
-        <v>2761</v>
+        <v>5633</v>
       </c>
       <c r="N1075" s="25" t="s">
         <v>323</v>
@@ -60870,31 +60863,31 @@
     </row>
     <row r="1076" spans="1:15">
       <c r="A1076" s="3" t="s">
-        <v>6581</v>
+        <v>7001</v>
       </c>
       <c r="B1076" s="49" t="s">
-        <v>48</v>
+        <v>5817</v>
       </c>
       <c r="C1076" s="21" t="s">
-        <v>2282</v>
+        <v>7005</v>
       </c>
       <c r="D1076" s="23" t="s">
-        <v>2283</v>
+        <v>171</v>
       </c>
       <c r="E1076" s="32" t="s">
-        <v>718</v>
+        <v>1585</v>
       </c>
       <c r="F1076" s="3" t="s">
-        <v>2284</v>
+        <v>2276</v>
       </c>
       <c r="H1076" s="3" t="s">
-        <v>1171</v>
+        <v>157</v>
       </c>
       <c r="I1076" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1076" s="22" t="s">
-        <v>721</v>
+        <v>1587</v>
       </c>
       <c r="K1076" s="22" t="s">
         <v>156</v>
@@ -60909,36 +60902,36 @@
         <v>323</v>
       </c>
       <c r="O1076" s="25" t="s">
-        <v>5827</v>
+        <v>5354</v>
       </c>
     </row>
     <row r="1077" spans="1:15">
       <c r="A1077" s="3" t="s">
-        <v>6582</v>
+        <v>6580</v>
       </c>
       <c r="B1077" s="49" t="s">
-        <v>5819</v>
+        <v>5818</v>
       </c>
       <c r="C1077" s="21" t="s">
-        <v>2285</v>
+        <v>2277</v>
       </c>
       <c r="D1077" s="23" t="s">
-        <v>2283</v>
+        <v>172</v>
       </c>
       <c r="E1077" s="32" t="s">
-        <v>2286</v>
+        <v>2278</v>
       </c>
       <c r="F1077" s="3" t="s">
-        <v>2287</v>
+        <v>2279</v>
       </c>
       <c r="H1077" s="3" t="s">
-        <v>2288</v>
+        <v>2280</v>
       </c>
       <c r="I1077" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1077" s="22" t="s">
-        <v>2289</v>
+        <v>2281</v>
       </c>
       <c r="K1077" s="22" t="s">
         <v>156</v>
@@ -60956,31 +60949,31 @@
     </row>
     <row r="1078" spans="1:15">
       <c r="A1078" s="3" t="s">
-        <v>7002</v>
+        <v>6581</v>
       </c>
       <c r="B1078" s="49" t="s">
-        <v>5820</v>
+        <v>48</v>
       </c>
       <c r="C1078" s="21" t="s">
-        <v>7006</v>
+        <v>2282</v>
       </c>
       <c r="D1078" s="23" t="s">
         <v>2283</v>
       </c>
       <c r="E1078" s="32" t="s">
-        <v>2291</v>
+        <v>718</v>
       </c>
       <c r="F1078" s="3" t="s">
-        <v>2292</v>
+        <v>2284</v>
       </c>
       <c r="H1078" s="3" t="s">
-        <v>423</v>
+        <v>1171</v>
       </c>
       <c r="I1078" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1078" s="22" t="s">
-        <v>2293</v>
+        <v>721</v>
       </c>
       <c r="K1078" s="22" t="s">
         <v>156</v>
@@ -60995,36 +60988,36 @@
         <v>323</v>
       </c>
       <c r="O1078" s="25" t="s">
-        <v>5354</v>
+        <v>5827</v>
       </c>
     </row>
     <row r="1079" spans="1:15">
       <c r="A1079" s="3" t="s">
-        <v>6583</v>
+        <v>6582</v>
       </c>
       <c r="B1079" s="49" t="s">
-        <v>5821</v>
+        <v>5819</v>
       </c>
       <c r="C1079" s="21" t="s">
-        <v>2294</v>
+        <v>2285</v>
       </c>
       <c r="D1079" s="23" t="s">
-        <v>172</v>
+        <v>2283</v>
       </c>
       <c r="E1079" s="32" t="s">
-        <v>2295</v>
+        <v>2286</v>
       </c>
       <c r="F1079" s="3" t="s">
-        <v>2296</v>
+        <v>2287</v>
       </c>
       <c r="H1079" s="3" t="s">
-        <v>248</v>
+        <v>2288</v>
       </c>
       <c r="I1079" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1079" s="22" t="s">
-        <v>2297</v>
+        <v>2289</v>
       </c>
       <c r="K1079" s="22" t="s">
         <v>156</v>
@@ -61038,37 +61031,35 @@
       <c r="N1079" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="O1079" s="25" t="s">
-        <v>5354</v>
-      </c>
+      <c r="O1079" s="25"/>
     </row>
     <row r="1080" spans="1:15">
       <c r="A1080" s="3" t="s">
-        <v>6584</v>
+        <v>7002</v>
       </c>
       <c r="B1080" s="49" t="s">
-        <v>5822</v>
+        <v>5820</v>
       </c>
       <c r="C1080" s="21" t="s">
-        <v>2298</v>
+        <v>7006</v>
       </c>
       <c r="D1080" s="23" t="s">
-        <v>172</v>
+        <v>2283</v>
       </c>
       <c r="E1080" s="32" t="s">
-        <v>2299</v>
+        <v>2291</v>
       </c>
       <c r="F1080" s="3" t="s">
-        <v>2300</v>
+        <v>2292</v>
       </c>
       <c r="H1080" s="3" t="s">
-        <v>2301</v>
+        <v>423</v>
       </c>
       <c r="I1080" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1080" s="22" t="s">
-        <v>2302</v>
+        <v>2293</v>
       </c>
       <c r="K1080" s="22" t="s">
         <v>156</v>
@@ -61077,40 +61068,42 @@
         <v>323</v>
       </c>
       <c r="M1080" s="24" t="s">
-        <v>5823</v>
+        <v>2761</v>
       </c>
       <c r="N1080" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="O1080" s="25"/>
+      <c r="O1080" s="25" t="s">
+        <v>5354</v>
+      </c>
     </row>
     <row r="1081" spans="1:15">
       <c r="A1081" s="3" t="s">
-        <v>6585</v>
+        <v>6583</v>
       </c>
       <c r="B1081" s="49" t="s">
-        <v>5824</v>
+        <v>5821</v>
       </c>
       <c r="C1081" s="21" t="s">
-        <v>2303</v>
+        <v>2294</v>
       </c>
       <c r="D1081" s="23" t="s">
-        <v>2304</v>
+        <v>172</v>
       </c>
       <c r="E1081" s="32" t="s">
-        <v>2305</v>
+        <v>2295</v>
       </c>
       <c r="F1081" s="3" t="s">
-        <v>2306</v>
+        <v>2296</v>
       </c>
       <c r="H1081" s="3" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="I1081" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1081" s="22" t="s">
-        <v>2307</v>
+        <v>2297</v>
       </c>
       <c r="K1081" s="22" t="s">
         <v>156</v>
@@ -61124,35 +61117,37 @@
       <c r="N1081" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="O1081" s="25"/>
+      <c r="O1081" s="25" t="s">
+        <v>5354</v>
+      </c>
     </row>
     <row r="1082" spans="1:15">
       <c r="A1082" s="3" t="s">
-        <v>6586</v>
+        <v>6584</v>
       </c>
       <c r="B1082" s="49" t="s">
-        <v>5825</v>
+        <v>5822</v>
       </c>
       <c r="C1082" s="21" t="s">
-        <v>2308</v>
+        <v>2298</v>
       </c>
       <c r="D1082" s="23" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E1082" s="32" t="s">
-        <v>2309</v>
+        <v>2299</v>
       </c>
       <c r="F1082" s="3" t="s">
-        <v>2310</v>
+        <v>2300</v>
       </c>
       <c r="H1082" s="3" t="s">
-        <v>1537</v>
+        <v>2301</v>
       </c>
       <c r="I1082" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1082" s="22" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
       <c r="K1082" s="22" t="s">
         <v>156</v>
@@ -61161,7 +61156,7 @@
         <v>323</v>
       </c>
       <c r="M1082" s="24" t="s">
-        <v>5382</v>
+        <v>5823</v>
       </c>
       <c r="N1082" s="25" t="s">
         <v>323</v>
@@ -61170,31 +61165,31 @@
     </row>
     <row r="1083" spans="1:15">
       <c r="A1083" s="3" t="s">
-        <v>6587</v>
+        <v>6585</v>
       </c>
       <c r="B1083" s="49" t="s">
-        <v>5826</v>
+        <v>5824</v>
       </c>
       <c r="C1083" s="21" t="s">
-        <v>2308</v>
+        <v>2303</v>
       </c>
       <c r="D1083" s="23" t="s">
-        <v>171</v>
+        <v>2304</v>
       </c>
       <c r="E1083" s="32" t="s">
-        <v>2309</v>
+        <v>2305</v>
       </c>
       <c r="F1083" s="3" t="s">
-        <v>2310</v>
+        <v>2306</v>
       </c>
       <c r="H1083" s="3" t="s">
-        <v>1537</v>
+        <v>254</v>
       </c>
       <c r="I1083" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1083" s="22" t="s">
-        <v>2311</v>
+        <v>2307</v>
       </c>
       <c r="K1083" s="22" t="s">
         <v>156</v>
@@ -61203,7 +61198,7 @@
         <v>323</v>
       </c>
       <c r="M1083" s="24" t="s">
-        <v>5382</v>
+        <v>2761</v>
       </c>
       <c r="N1083" s="25" t="s">
         <v>323</v>
@@ -61212,31 +61207,31 @@
     </row>
     <row r="1084" spans="1:15">
       <c r="A1084" s="3" t="s">
-        <v>5893</v>
+        <v>6586</v>
       </c>
       <c r="B1084" s="49" t="s">
-        <v>5353</v>
+        <v>5825</v>
       </c>
       <c r="C1084" s="21" t="s">
-        <v>2282</v>
+        <v>2308</v>
       </c>
       <c r="D1084" s="23" t="s">
-        <v>835</v>
+        <v>171</v>
       </c>
       <c r="E1084" s="32" t="s">
-        <v>718</v>
+        <v>2309</v>
       </c>
       <c r="F1084" s="3" t="s">
-        <v>2284</v>
+        <v>2310</v>
       </c>
       <c r="H1084" s="3" t="s">
-        <v>1171</v>
+        <v>1537</v>
       </c>
       <c r="I1084" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1084" s="22" t="s">
-        <v>721</v>
+        <v>2311</v>
       </c>
       <c r="K1084" s="22" t="s">
         <v>156</v>
@@ -61245,42 +61240,40 @@
         <v>323</v>
       </c>
       <c r="M1084" s="24" t="s">
-        <v>5823</v>
+        <v>5382</v>
       </c>
       <c r="N1084" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="O1084" s="25" t="s">
-        <v>5354</v>
-      </c>
+      <c r="O1084" s="25"/>
     </row>
     <row r="1085" spans="1:15">
       <c r="A1085" s="3" t="s">
-        <v>6588</v>
+        <v>6587</v>
       </c>
       <c r="B1085" s="49" t="s">
-        <v>5828</v>
+        <v>5826</v>
       </c>
       <c r="C1085" s="21" t="s">
-        <v>2290</v>
+        <v>2308</v>
       </c>
       <c r="D1085" s="23" t="s">
-        <v>858</v>
+        <v>171</v>
       </c>
       <c r="E1085" s="32" t="s">
-        <v>2291</v>
+        <v>2309</v>
       </c>
       <c r="F1085" s="3" t="s">
-        <v>2292</v>
+        <v>2310</v>
       </c>
       <c r="H1085" s="3" t="s">
-        <v>423</v>
+        <v>1537</v>
       </c>
       <c r="I1085" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1085" s="22" t="s">
-        <v>2293</v>
+        <v>2311</v>
       </c>
       <c r="K1085" s="22" t="s">
         <v>156</v>
@@ -61289,42 +61282,40 @@
         <v>323</v>
       </c>
       <c r="M1085" s="24" t="s">
-        <v>5829</v>
+        <v>5382</v>
       </c>
       <c r="N1085" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="O1085" s="25" t="s">
-        <v>5354</v>
-      </c>
+      <c r="O1085" s="25"/>
     </row>
     <row r="1086" spans="1:15">
       <c r="A1086" s="3" t="s">
-        <v>6589</v>
+        <v>5893</v>
       </c>
       <c r="B1086" s="49" t="s">
-        <v>5830</v>
+        <v>5353</v>
       </c>
       <c r="C1086" s="21" t="s">
-        <v>2290</v>
+        <v>2282</v>
       </c>
       <c r="D1086" s="23" t="s">
-        <v>858</v>
+        <v>835</v>
       </c>
       <c r="E1086" s="32" t="s">
-        <v>2291</v>
+        <v>718</v>
       </c>
       <c r="F1086" s="3" t="s">
-        <v>2292</v>
+        <v>2284</v>
       </c>
       <c r="H1086" s="3" t="s">
-        <v>423</v>
+        <v>1171</v>
       </c>
       <c r="I1086" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1086" s="22" t="s">
-        <v>2293</v>
+        <v>721</v>
       </c>
       <c r="K1086" s="22" t="s">
         <v>156</v>
@@ -61333,7 +61324,7 @@
         <v>323</v>
       </c>
       <c r="M1086" s="24" t="s">
-        <v>5829</v>
+        <v>5823</v>
       </c>
       <c r="N1086" s="25" t="s">
         <v>323</v>
@@ -61344,31 +61335,31 @@
     </row>
     <row r="1087" spans="1:15">
       <c r="A1087" s="3" t="s">
-        <v>6998</v>
+        <v>6588</v>
       </c>
       <c r="B1087" s="49" t="s">
-        <v>5831</v>
+        <v>5828</v>
       </c>
       <c r="C1087" s="21" t="s">
-        <v>7007</v>
+        <v>2290</v>
       </c>
       <c r="D1087" s="23" t="s">
         <v>858</v>
       </c>
       <c r="E1087" s="32" t="s">
-        <v>2312</v>
+        <v>2291</v>
       </c>
       <c r="F1087" s="3" t="s">
-        <v>2313</v>
+        <v>2292</v>
       </c>
       <c r="H1087" s="3" t="s">
-        <v>2314</v>
+        <v>423</v>
       </c>
       <c r="I1087" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1087" s="22" t="s">
-        <v>2315</v>
+        <v>2293</v>
       </c>
       <c r="K1087" s="22" t="s">
         <v>156</v>
@@ -61377,40 +61368,42 @@
         <v>323</v>
       </c>
       <c r="M1087" s="24" t="s">
-        <v>2761</v>
+        <v>5829</v>
       </c>
       <c r="N1087" s="25" t="s">
-        <v>2316</v>
-      </c>
-      <c r="O1087" s="25"/>
+        <v>323</v>
+      </c>
+      <c r="O1087" s="25" t="s">
+        <v>5354</v>
+      </c>
     </row>
     <row r="1088" spans="1:15">
       <c r="A1088" s="3" t="s">
-        <v>6590</v>
+        <v>6589</v>
       </c>
       <c r="B1088" s="49" t="s">
-        <v>5832</v>
+        <v>5830</v>
       </c>
       <c r="C1088" s="21" t="s">
-        <v>2317</v>
+        <v>2290</v>
       </c>
       <c r="D1088" s="23" t="s">
-        <v>172</v>
+        <v>858</v>
       </c>
       <c r="E1088" s="32" t="s">
-        <v>2318</v>
+        <v>2291</v>
       </c>
       <c r="F1088" s="3" t="s">
-        <v>2319</v>
+        <v>2292</v>
       </c>
       <c r="H1088" s="3" t="s">
-        <v>168</v>
+        <v>423</v>
       </c>
       <c r="I1088" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1088" s="22" t="s">
-        <v>2164</v>
+        <v>2293</v>
       </c>
       <c r="K1088" s="22" t="s">
         <v>156</v>
@@ -61419,43 +61412,42 @@
         <v>323</v>
       </c>
       <c r="M1088" s="24" t="s">
-        <v>5796</v>
+        <v>5829</v>
       </c>
       <c r="N1088" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="O1088" s="25"/>
+      <c r="O1088" s="25" t="s">
+        <v>5354</v>
+      </c>
     </row>
     <row r="1089" spans="1:15">
       <c r="A1089" s="3" t="s">
-        <v>6591</v>
+        <v>6998</v>
       </c>
       <c r="B1089" s="49" t="s">
-        <v>5833</v>
+        <v>5831</v>
       </c>
       <c r="C1089" s="21" t="s">
-        <v>2317</v>
+        <v>7007</v>
       </c>
       <c r="D1089" s="23" t="s">
-        <v>172</v>
+        <v>858</v>
       </c>
       <c r="E1089" s="32" t="s">
-        <v>2320</v>
+        <v>2312</v>
       </c>
       <c r="F1089" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="G1089" s="3" t="s">
-        <v>2321</v>
+        <v>2313</v>
       </c>
       <c r="H1089" s="3" t="s">
-        <v>254</v>
+        <v>2314</v>
       </c>
       <c r="I1089" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1089" s="22" t="s">
-        <v>255</v>
+        <v>2315</v>
       </c>
       <c r="K1089" s="22" t="s">
         <v>156</v>
@@ -61467,39 +61459,37 @@
         <v>2761</v>
       </c>
       <c r="N1089" s="25" t="s">
-        <v>323</v>
-      </c>
-      <c r="O1089" s="25" t="s">
-        <v>2322</v>
-      </c>
+        <v>2316</v>
+      </c>
+      <c r="O1089" s="25"/>
     </row>
     <row r="1090" spans="1:15">
       <c r="A1090" s="3" t="s">
-        <v>6592</v>
+        <v>6590</v>
       </c>
       <c r="B1090" s="49" t="s">
-        <v>5834</v>
+        <v>5832</v>
       </c>
       <c r="C1090" s="21" t="s">
-        <v>2323</v>
+        <v>2317</v>
       </c>
       <c r="D1090" s="23" t="s">
         <v>172</v>
       </c>
       <c r="E1090" s="32" t="s">
-        <v>2324</v>
+        <v>2318</v>
       </c>
       <c r="F1090" s="3" t="s">
-        <v>2325</v>
+        <v>2319</v>
       </c>
       <c r="H1090" s="3" t="s">
-        <v>1652</v>
+        <v>168</v>
       </c>
       <c r="I1090" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1090" s="22" t="s">
-        <v>2326</v>
+        <v>2164</v>
       </c>
       <c r="K1090" s="22" t="s">
         <v>156</v>
@@ -61508,7 +61498,7 @@
         <v>323</v>
       </c>
       <c r="M1090" s="24" t="s">
-        <v>5814</v>
+        <v>5796</v>
       </c>
       <c r="N1090" s="25" t="s">
         <v>323</v>
@@ -61517,31 +61507,34 @@
     </row>
     <row r="1091" spans="1:15">
       <c r="A1091" s="3" t="s">
-        <v>6593</v>
+        <v>6591</v>
       </c>
       <c r="B1091" s="49" t="s">
-        <v>5355</v>
+        <v>5833</v>
       </c>
       <c r="C1091" s="21" t="s">
-        <v>2327</v>
+        <v>2317</v>
       </c>
       <c r="D1091" s="23" t="s">
         <v>172</v>
       </c>
       <c r="E1091" s="32" t="s">
-        <v>2328</v>
+        <v>2320</v>
       </c>
       <c r="F1091" s="3" t="s">
-        <v>2329</v>
+        <v>253</v>
+      </c>
+      <c r="G1091" s="3" t="s">
+        <v>2321</v>
       </c>
       <c r="H1091" s="3" t="s">
-        <v>2330</v>
+        <v>254</v>
       </c>
       <c r="I1091" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1091" s="22" t="s">
-        <v>2331</v>
+        <v>255</v>
       </c>
       <c r="K1091" s="22" t="s">
         <v>156</v>
@@ -61555,35 +61548,37 @@
       <c r="N1091" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="O1091" s="25"/>
+      <c r="O1091" s="25" t="s">
+        <v>2322</v>
+      </c>
     </row>
     <row r="1092" spans="1:15">
       <c r="A1092" s="3" t="s">
-        <v>6594</v>
+        <v>6592</v>
       </c>
       <c r="B1092" s="49" t="s">
-        <v>5835</v>
+        <v>5834</v>
       </c>
       <c r="C1092" s="21" t="s">
-        <v>2332</v>
+        <v>2323</v>
       </c>
       <c r="D1092" s="23" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E1092" s="32" t="s">
-        <v>2333</v>
+        <v>2324</v>
       </c>
       <c r="F1092" s="3" t="s">
-        <v>2310</v>
+        <v>2325</v>
       </c>
       <c r="H1092" s="3" t="s">
-        <v>1537</v>
+        <v>1652</v>
       </c>
       <c r="I1092" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1092" s="22" t="s">
-        <v>2311</v>
+        <v>2326</v>
       </c>
       <c r="K1092" s="22" t="s">
         <v>156</v>
@@ -61592,7 +61587,7 @@
         <v>323</v>
       </c>
       <c r="M1092" s="24" t="s">
-        <v>5382</v>
+        <v>5814</v>
       </c>
       <c r="N1092" s="25" t="s">
         <v>323</v>
@@ -61601,34 +61596,31 @@
     </row>
     <row r="1093" spans="1:15">
       <c r="A1093" s="3" t="s">
-        <v>6595</v>
+        <v>6593</v>
       </c>
       <c r="B1093" s="49" t="s">
-        <v>5836</v>
+        <v>5355</v>
       </c>
       <c r="C1093" s="21" t="s">
-        <v>2303</v>
+        <v>2327</v>
       </c>
       <c r="D1093" s="23" t="s">
         <v>172</v>
       </c>
       <c r="E1093" s="32" t="s">
-        <v>2305</v>
+        <v>2328</v>
       </c>
       <c r="F1093" s="3" t="s">
-        <v>2334</v>
-      </c>
-      <c r="G1093" s="3" t="s">
-        <v>2335</v>
+        <v>2329</v>
       </c>
       <c r="H1093" s="3" t="s">
-        <v>249</v>
+        <v>2330</v>
       </c>
       <c r="I1093" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1093" s="22" t="s">
-        <v>2336</v>
+        <v>2331</v>
       </c>
       <c r="K1093" s="22" t="s">
         <v>156</v>
@@ -61637,7 +61629,7 @@
         <v>323</v>
       </c>
       <c r="M1093" s="24" t="s">
-        <v>5814</v>
+        <v>2761</v>
       </c>
       <c r="N1093" s="25" t="s">
         <v>323</v>
@@ -61646,34 +61638,31 @@
     </row>
     <row r="1094" spans="1:15">
       <c r="A1094" s="3" t="s">
-        <v>6596</v>
+        <v>6594</v>
       </c>
       <c r="B1094" s="49" t="s">
-        <v>5837</v>
+        <v>5835</v>
       </c>
       <c r="C1094" s="21" t="s">
-        <v>2337</v>
+        <v>2332</v>
       </c>
       <c r="D1094" s="23" t="s">
         <v>171</v>
       </c>
       <c r="E1094" s="32" t="s">
-        <v>2338</v>
+        <v>2333</v>
       </c>
       <c r="F1094" s="3" t="s">
-        <v>2339</v>
-      </c>
-      <c r="G1094" s="3" t="s">
-        <v>2340</v>
+        <v>2310</v>
       </c>
       <c r="H1094" s="3" t="s">
-        <v>254</v>
+        <v>1537</v>
       </c>
       <c r="I1094" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1094" s="22" t="s">
-        <v>2341</v>
+        <v>2311</v>
       </c>
       <c r="K1094" s="22" t="s">
         <v>156</v>
@@ -61682,7 +61671,7 @@
         <v>323</v>
       </c>
       <c r="M1094" s="24" t="s">
-        <v>5805</v>
+        <v>5382</v>
       </c>
       <c r="N1094" s="25" t="s">
         <v>323</v>
@@ -61691,31 +61680,34 @@
     </row>
     <row r="1095" spans="1:15">
       <c r="A1095" s="3" t="s">
-        <v>6597</v>
+        <v>6595</v>
       </c>
       <c r="B1095" s="49" t="s">
-        <v>5838</v>
+        <v>5836</v>
       </c>
       <c r="C1095" s="21" t="s">
-        <v>2342</v>
+        <v>2303</v>
       </c>
       <c r="D1095" s="23" t="s">
         <v>172</v>
       </c>
       <c r="E1095" s="32" t="s">
-        <v>2343</v>
+        <v>2305</v>
       </c>
       <c r="F1095" s="3" t="s">
-        <v>2344</v>
+        <v>2334</v>
+      </c>
+      <c r="G1095" s="3" t="s">
+        <v>2335</v>
       </c>
       <c r="H1095" s="3" t="s">
-        <v>2345</v>
+        <v>249</v>
       </c>
       <c r="I1095" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1095" s="22" t="s">
-        <v>2346</v>
+        <v>2336</v>
       </c>
       <c r="K1095" s="22" t="s">
         <v>156</v>
@@ -61724,7 +61716,7 @@
         <v>323</v>
       </c>
       <c r="M1095" s="24" t="s">
-        <v>5805</v>
+        <v>5814</v>
       </c>
       <c r="N1095" s="25" t="s">
         <v>323</v>
@@ -61733,31 +61725,34 @@
     </row>
     <row r="1096" spans="1:15">
       <c r="A1096" s="3" t="s">
-        <v>6598</v>
+        <v>6596</v>
       </c>
       <c r="B1096" s="49" t="s">
-        <v>5839</v>
+        <v>5837</v>
       </c>
       <c r="C1096" s="21" t="s">
-        <v>2285</v>
+        <v>2337</v>
       </c>
       <c r="D1096" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E1096" s="32" t="s">
-        <v>2286</v>
+        <v>2338</v>
       </c>
       <c r="F1096" s="3" t="s">
-        <v>2287</v>
+        <v>2339</v>
+      </c>
+      <c r="G1096" s="3" t="s">
+        <v>2340</v>
       </c>
       <c r="H1096" s="3" t="s">
-        <v>2288</v>
+        <v>254</v>
       </c>
       <c r="I1096" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1096" s="22" t="s">
-        <v>2289</v>
+        <v>2341</v>
       </c>
       <c r="K1096" s="22" t="s">
         <v>156</v>
@@ -61766,7 +61761,7 @@
         <v>323</v>
       </c>
       <c r="M1096" s="24" t="s">
-        <v>2761</v>
+        <v>5805</v>
       </c>
       <c r="N1096" s="25" t="s">
         <v>323</v>
@@ -61775,165 +61770,170 @@
     </row>
     <row r="1097" spans="1:15">
       <c r="A1097" s="3" t="s">
-        <v>7017</v>
+        <v>6597</v>
       </c>
       <c r="B1097" s="49" t="s">
-        <v>7018</v>
+        <v>5838</v>
       </c>
       <c r="C1097" s="21" t="s">
-        <v>7019</v>
+        <v>2342</v>
       </c>
       <c r="D1097" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="E1097" s="21" t="s">
-        <v>2886</v>
+      <c r="E1097" s="32" t="s">
+        <v>2343</v>
       </c>
       <c r="F1097" s="3" t="s">
-        <v>2887</v>
+        <v>2344</v>
       </c>
       <c r="H1097" s="3" t="s">
-        <v>7020</v>
+        <v>2345</v>
       </c>
       <c r="I1097" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1097" s="22" t="s">
-        <v>2888</v>
+        <v>2346</v>
       </c>
       <c r="K1097" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="L1097" t="s">
+      <c r="L1097" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="M1097" s="46" t="s">
-        <v>5633</v>
-      </c>
-      <c r="N1097" t="s">
+      <c r="M1097" s="24" t="s">
+        <v>5805</v>
+      </c>
+      <c r="N1097" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="O1097" t="s">
-        <v>5354</v>
-      </c>
+      <c r="O1097" s="25"/>
     </row>
     <row r="1098" spans="1:15">
       <c r="A1098" s="3" t="s">
-        <v>7021</v>
+        <v>6598</v>
       </c>
       <c r="B1098" s="49" t="s">
-        <v>7022</v>
+        <v>5839</v>
       </c>
       <c r="C1098" s="21" t="s">
-        <v>7023</v>
-      </c>
-      <c r="E1098" s="21" t="s">
-        <v>7024</v>
+        <v>2285</v>
+      </c>
+      <c r="D1098" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1098" s="32" t="s">
+        <v>2286</v>
       </c>
       <c r="F1098" s="3" t="s">
-        <v>7025</v>
+        <v>2287</v>
       </c>
       <c r="H1098" s="3" t="s">
-        <v>224</v>
+        <v>2288</v>
       </c>
       <c r="I1098" s="22" t="s">
         <v>575</v>
       </c>
       <c r="J1098" s="22" t="s">
-        <v>7026</v>
+        <v>2289</v>
       </c>
       <c r="K1098" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="L1098" t="s">
-        <v>2760</v>
-      </c>
-      <c r="M1098" s="46" t="s">
+      <c r="L1098" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="M1098" s="24" t="s">
         <v>2761</v>
       </c>
-      <c r="N1098" t="s">
-        <v>2760</v>
-      </c>
+      <c r="N1098" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="O1098" s="25"/>
     </row>
     <row r="1099" spans="1:15">
       <c r="A1099" s="3" t="s">
-        <v>7027</v>
+        <v>7017</v>
       </c>
       <c r="B1099" s="49" t="s">
-        <v>7028</v>
+        <v>7018</v>
       </c>
       <c r="C1099" s="21" t="s">
-        <v>7029</v>
+        <v>7019</v>
+      </c>
+      <c r="D1099" s="23" t="s">
+        <v>172</v>
       </c>
       <c r="E1099" s="21" t="s">
-        <v>7030</v>
+        <v>2886</v>
       </c>
       <c r="F1099" s="3" t="s">
-        <v>7031</v>
+        <v>2887</v>
       </c>
       <c r="H1099" s="3" t="s">
-        <v>283</v>
+        <v>7020</v>
       </c>
       <c r="I1099" s="22" t="s">
-        <v>7032</v>
+        <v>575</v>
       </c>
       <c r="J1099" s="22" t="s">
-        <v>7033</v>
+        <v>2888</v>
       </c>
       <c r="K1099" s="22" t="s">
         <v>156</v>
       </c>
       <c r="L1099" t="s">
-        <v>816</v>
+        <v>323</v>
       </c>
       <c r="M1099" s="46" t="s">
         <v>5633</v>
       </c>
       <c r="N1099" t="s">
-        <v>816</v>
+        <v>323</v>
       </c>
       <c r="O1099" t="s">
-        <v>7034</v>
+        <v>5354</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O1096" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O1096">
-      <sortCondition ref="B2:B1096"/>
-      <sortCondition ref="A2:A1096"/>
+  <autoFilter ref="A1:O1098" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O1098">
+      <sortCondition ref="B2:B1098"/>
+      <sortCondition ref="A2:A1098"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A2:O9804">
+  <conditionalFormatting sqref="A2:O9802">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND($A2&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E1096" r:id="rId1" xr:uid="{F456DE86-0DC4-459B-8786-AEB12C0F36B0}"/>
-    <hyperlink ref="E1095" r:id="rId2" xr:uid="{A987B60B-629E-450A-AFE5-A7284329CD96}"/>
-    <hyperlink ref="E1094" r:id="rId3" xr:uid="{BDA96C0A-370D-46F7-82B7-86D5AE155E9F}"/>
-    <hyperlink ref="E1093" r:id="rId4" xr:uid="{E0EF30A2-FEE8-48F7-905E-3DCEE9D90336}"/>
-    <hyperlink ref="E1092" r:id="rId5" xr:uid="{F5EE9F94-288C-4D35-98F2-B7DF314331DE}"/>
-    <hyperlink ref="E1091" r:id="rId6" xr:uid="{A71B48CB-C499-456A-8FFD-47EFE60A828E}"/>
-    <hyperlink ref="E1090" r:id="rId7" xr:uid="{AF04FF5C-ADCA-44DC-B3B2-A425FC0DCFD9}"/>
-    <hyperlink ref="E1089" r:id="rId8" xr:uid="{F55EAFC5-5519-4A1F-80D4-95B4D202FE38}"/>
-    <hyperlink ref="E1088" r:id="rId9" xr:uid="{5FE20200-FB86-452E-8BE1-863A3C65BD07}"/>
-    <hyperlink ref="E1087" r:id="rId10" xr:uid="{8F88B4B6-197E-4940-B572-1769D2C402A3}"/>
-    <hyperlink ref="E1086" r:id="rId11" xr:uid="{DACEA89F-4573-408A-AA3D-AAFC4DF8DB2E}"/>
-    <hyperlink ref="E1085" r:id="rId12" xr:uid="{BF25E2D2-8541-4371-99B7-17A8B86CC8F6}"/>
-    <hyperlink ref="E1084" r:id="rId13" xr:uid="{57CD897B-E530-431D-A4B5-59D9C0F63217}"/>
-    <hyperlink ref="E1083" r:id="rId14" xr:uid="{CEEE77DB-0464-4890-9DA6-629F365AAC93}"/>
-    <hyperlink ref="E1082" r:id="rId15" xr:uid="{D183A8CF-2618-4DDD-8523-A347B0789735}"/>
-    <hyperlink ref="E1081" r:id="rId16" xr:uid="{B44DC245-3939-4FC4-B86F-7F55F80E20F1}"/>
-    <hyperlink ref="E1080" r:id="rId17" xr:uid="{77BEB31C-67F9-4892-974A-C42D173ACEC7}"/>
-    <hyperlink ref="E1079" r:id="rId18" xr:uid="{802015E0-18C1-4D8F-BD48-60606EF00558}"/>
-    <hyperlink ref="E1078" r:id="rId19" xr:uid="{185AA3D8-0081-42DB-B36C-3B1B4DF6AE78}"/>
-    <hyperlink ref="E1077" r:id="rId20" xr:uid="{C92F0FF0-F014-47C6-8A1D-37500F8CB37C}"/>
-    <hyperlink ref="E1076" r:id="rId21" xr:uid="{A79E531F-E421-48DC-B313-0C433AA33C66}"/>
-    <hyperlink ref="E1075" r:id="rId22" xr:uid="{CF6C1299-30F9-427A-9C11-CDEF3096DB13}"/>
-    <hyperlink ref="E1074" r:id="rId23" xr:uid="{B0ED86D2-3643-405A-B6A7-581D3F444E88}"/>
-    <hyperlink ref="E1073" r:id="rId24" xr:uid="{3643C6A3-6F1E-403F-B5BD-A7251D505F5B}"/>
-    <hyperlink ref="E1071" r:id="rId25" xr:uid="{0E92FFCB-F966-4697-91BE-A3130C1CAE25}"/>
+    <hyperlink ref="E1098" r:id="rId1" xr:uid="{F456DE86-0DC4-459B-8786-AEB12C0F36B0}"/>
+    <hyperlink ref="E1097" r:id="rId2" xr:uid="{A987B60B-629E-450A-AFE5-A7284329CD96}"/>
+    <hyperlink ref="E1096" r:id="rId3" xr:uid="{BDA96C0A-370D-46F7-82B7-86D5AE155E9F}"/>
+    <hyperlink ref="E1095" r:id="rId4" xr:uid="{E0EF30A2-FEE8-48F7-905E-3DCEE9D90336}"/>
+    <hyperlink ref="E1094" r:id="rId5" xr:uid="{F5EE9F94-288C-4D35-98F2-B7DF314331DE}"/>
+    <hyperlink ref="E1093" r:id="rId6" xr:uid="{A71B48CB-C499-456A-8FFD-47EFE60A828E}"/>
+    <hyperlink ref="E1092" r:id="rId7" xr:uid="{AF04FF5C-ADCA-44DC-B3B2-A425FC0DCFD9}"/>
+    <hyperlink ref="E1091" r:id="rId8" xr:uid="{F55EAFC5-5519-4A1F-80D4-95B4D202FE38}"/>
+    <hyperlink ref="E1090" r:id="rId9" xr:uid="{5FE20200-FB86-452E-8BE1-863A3C65BD07}"/>
+    <hyperlink ref="E1089" r:id="rId10" xr:uid="{8F88B4B6-197E-4940-B572-1769D2C402A3}"/>
+    <hyperlink ref="E1088" r:id="rId11" xr:uid="{DACEA89F-4573-408A-AA3D-AAFC4DF8DB2E}"/>
+    <hyperlink ref="E1087" r:id="rId12" xr:uid="{BF25E2D2-8541-4371-99B7-17A8B86CC8F6}"/>
+    <hyperlink ref="E1086" r:id="rId13" xr:uid="{57CD897B-E530-431D-A4B5-59D9C0F63217}"/>
+    <hyperlink ref="E1085" r:id="rId14" xr:uid="{CEEE77DB-0464-4890-9DA6-629F365AAC93}"/>
+    <hyperlink ref="E1084" r:id="rId15" xr:uid="{D183A8CF-2618-4DDD-8523-A347B0789735}"/>
+    <hyperlink ref="E1083" r:id="rId16" xr:uid="{B44DC245-3939-4FC4-B86F-7F55F80E20F1}"/>
+    <hyperlink ref="E1082" r:id="rId17" xr:uid="{77BEB31C-67F9-4892-974A-C42D173ACEC7}"/>
+    <hyperlink ref="E1081" r:id="rId18" xr:uid="{802015E0-18C1-4D8F-BD48-60606EF00558}"/>
+    <hyperlink ref="E1080" r:id="rId19" xr:uid="{185AA3D8-0081-42DB-B36C-3B1B4DF6AE78}"/>
+    <hyperlink ref="E1079" r:id="rId20" xr:uid="{C92F0FF0-F014-47C6-8A1D-37500F8CB37C}"/>
+    <hyperlink ref="E1078" r:id="rId21" xr:uid="{A79E531F-E421-48DC-B313-0C433AA33C66}"/>
+    <hyperlink ref="E1077" r:id="rId22" xr:uid="{CF6C1299-30F9-427A-9C11-CDEF3096DB13}"/>
+    <hyperlink ref="E1076" r:id="rId23" xr:uid="{B0ED86D2-3643-405A-B6A7-581D3F444E88}"/>
+    <hyperlink ref="E1075" r:id="rId24" xr:uid="{3643C6A3-6F1E-403F-B5BD-A7251D505F5B}"/>
+    <hyperlink ref="E1073" r:id="rId25" xr:uid="{0E92FFCB-F966-4697-91BE-A3130C1CAE25}"/>
     <hyperlink ref="E373" r:id="rId26" xr:uid="{B4AE46D0-0113-43B5-920F-41BAD7FB12F3}"/>
     <hyperlink ref="E360" r:id="rId27" xr:uid="{6A53CFF1-B4AE-4894-AF74-B4B080E1676D}"/>
     <hyperlink ref="E357" r:id="rId28" xr:uid="{FC91B321-7F3C-4B7C-978D-FF322BE215D6}"/>

</xml_diff>

<commit_message>
2024-10-17 @ 21:41 - v5.A.0.xlsb
* modAppli_Utils.bas
   - Agrandir le masque des montants et ajouter un espace avant le $
   - Convertir Inv_No en String dans FAC_Détails
   - Vérifier que les dates sont à 10 caractères (pas d'heure, de minute et de seconde)
   - Nouvelle procédure pour lire le fichier LogSaisieHeures.txt
   - Procédure pour corriger les dates trop longues... date <> int(date)
* modFAC_Finale.bas
   - Convertir le numéro de facture en String dans la création de FAC_Détails
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3A3D9A-C727-4636-BE41-95911697A0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA0750A-8DF9-4DD6-BF9A-40DDF31F9AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
@@ -20773,9 +20773,6 @@
     <t>4695 Route 125</t>
   </si>
   <si>
-    <t>9514-1149 Québec Inc. [Alexandre Paris]</t>
-  </si>
-  <si>
     <t>1770</t>
   </si>
   <si>
@@ -21194,6 +21191,9 @@
   </si>
   <si>
     <t>J5V 2B4</t>
+  </si>
+  <si>
+    <t>9514-1149 Québec Inc. [Bélanger Sauvé] [Alexandre Paris]</t>
   </si>
 </sst>
 </file>
@@ -22380,7 +22380,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="3" t="s">
-        <v>7012</v>
+        <v>7011</v>
       </c>
       <c r="B6" s="49" t="s">
         <v>2350</v>
@@ -23234,7 +23234,7 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="3" t="s">
-        <v>6945</v>
+        <v>6944</v>
       </c>
       <c r="B30" s="49" t="s">
         <v>2765</v>
@@ -23339,7 +23339,7 @@
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="3" t="s">
-        <v>6944</v>
+        <v>6943</v>
       </c>
       <c r="B33" s="49" t="s">
         <v>5905</v>
@@ -23625,7 +23625,7 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="3" t="s">
-        <v>6957</v>
+        <v>6956</v>
       </c>
       <c r="B41" s="49" t="s">
         <v>5908</v>
@@ -23661,7 +23661,7 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="3" t="s">
-        <v>6946</v>
+        <v>6945</v>
       </c>
       <c r="B42" s="49" t="s">
         <v>2768</v>
@@ -30632,7 +30632,7 @@
     </row>
     <row r="254" spans="1:15">
       <c r="A254" s="3" t="s">
-        <v>6940</v>
+        <v>6939</v>
       </c>
       <c r="B254" s="49" t="s">
         <v>5301</v>
@@ -33416,7 +33416,7 @@
     </row>
     <row r="340" spans="1:15">
       <c r="A340" s="3" t="s">
-        <v>7004</v>
+        <v>7003</v>
       </c>
       <c r="B340" s="49" t="s">
         <v>5335</v>
@@ -34647,19 +34647,19 @@
     </row>
     <row r="377" spans="1:15">
       <c r="A377" s="3" t="s">
+        <v>6974</v>
+      </c>
+      <c r="B377" s="49" t="s">
         <v>6975</v>
       </c>
-      <c r="B377" s="49" t="s">
-        <v>6976</v>
-      </c>
       <c r="C377" s="21" t="s">
-        <v>6975</v>
+        <v>6974</v>
       </c>
       <c r="E377" s="21" t="s">
+        <v>6979</v>
+      </c>
+      <c r="F377" s="3" t="s">
         <v>6980</v>
-      </c>
-      <c r="F377" s="3" t="s">
-        <v>6981</v>
       </c>
       <c r="H377" s="3" t="s">
         <v>254</v>
@@ -34668,7 +34668,7 @@
         <v>575</v>
       </c>
       <c r="J377" s="22" t="s">
-        <v>6982</v>
+        <v>6981</v>
       </c>
       <c r="K377" s="22" t="s">
         <v>156</v>
@@ -35144,7 +35144,7 @@
     </row>
     <row r="390" spans="1:15">
       <c r="A390" s="3" t="s">
-        <v>6943</v>
+        <v>6942</v>
       </c>
       <c r="B390" s="49" t="s">
         <v>465</v>
@@ -35684,7 +35684,7 @@
     </row>
     <row r="403" spans="1:15">
       <c r="A403" s="3" t="s">
-        <v>6956</v>
+        <v>6955</v>
       </c>
       <c r="B403" s="49" t="s">
         <v>5494</v>
@@ -35696,7 +35696,7 @@
         <v>1070</v>
       </c>
       <c r="E403" s="50" t="s">
-        <v>7037</v>
+        <v>7036</v>
       </c>
       <c r="F403" s="3" t="s">
         <v>489</v>
@@ -37688,7 +37688,7 @@
     </row>
     <row r="454" spans="1:15">
       <c r="A454" s="3" t="s">
-        <v>6942</v>
+        <v>6941</v>
       </c>
       <c r="B454" s="49" t="s">
         <v>2783</v>
@@ -37918,7 +37918,7 @@
     </row>
     <row r="460" spans="1:15">
       <c r="A460" s="3" t="s">
-        <v>6995</v>
+        <v>6994</v>
       </c>
       <c r="B460" s="49" t="s">
         <v>5513</v>
@@ -39994,7 +39994,7 @@
     </row>
     <row r="516" spans="1:15">
       <c r="A516" s="3" t="s">
-        <v>6961</v>
+        <v>6960</v>
       </c>
       <c r="B516" s="49" t="s">
         <v>3008</v>
@@ -40557,7 +40557,7 @@
     </row>
     <row r="531" spans="1:15">
       <c r="A531" s="3" t="s">
-        <v>6963</v>
+        <v>6962</v>
       </c>
       <c r="B531" s="49" t="s">
         <v>3082</v>
@@ -40592,7 +40592,7 @@
     </row>
     <row r="532" spans="1:15">
       <c r="A532" s="3" t="s">
-        <v>6958</v>
+        <v>6957</v>
       </c>
       <c r="B532" s="49" t="s">
         <v>3087</v>
@@ -40773,7 +40773,7 @@
     </row>
     <row r="537" spans="1:15">
       <c r="A537" s="3" t="s">
-        <v>6964</v>
+        <v>6963</v>
       </c>
       <c r="B537" s="49" t="s">
         <v>13</v>
@@ -41061,7 +41061,7 @@
     </row>
     <row r="545" spans="1:15">
       <c r="A545" s="3" t="s">
-        <v>6968</v>
+        <v>6967</v>
       </c>
       <c r="B545" s="49" t="s">
         <v>3142</v>
@@ -41168,7 +41168,7 @@
     </row>
     <row r="548" spans="1:15">
       <c r="A548" s="3" t="s">
-        <v>6959</v>
+        <v>6958</v>
       </c>
       <c r="B548" s="49" t="s">
         <v>3157</v>
@@ -42910,7 +42910,7 @@
     </row>
     <row r="595" spans="1:15">
       <c r="A595" s="3" t="s">
-        <v>6962</v>
+        <v>6961</v>
       </c>
       <c r="B595" s="49" t="s">
         <v>3366</v>
@@ -44221,7 +44221,7 @@
     </row>
     <row r="631" spans="1:15">
       <c r="A631" s="3" t="s">
-        <v>6941</v>
+        <v>6940</v>
       </c>
       <c r="B631" s="49" t="s">
         <v>3531</v>
@@ -45165,10 +45165,10 @@
         <v>3648</v>
       </c>
       <c r="C656" s="37" t="s">
+        <v>7037</v>
+      </c>
+      <c r="E656" s="37" t="s">
         <v>7038</v>
-      </c>
-      <c r="E656" s="37" t="s">
-        <v>7039</v>
       </c>
       <c r="F656" s="37" t="s">
         <v>3649</v>
@@ -45667,7 +45667,7 @@
     </row>
     <row r="670" spans="1:15">
       <c r="A670" s="3" t="s">
-        <v>6965</v>
+        <v>6964</v>
       </c>
       <c r="B670" s="49" t="s">
         <v>3704</v>
@@ -47169,7 +47169,7 @@
     </row>
     <row r="711" spans="1:15">
       <c r="A711" s="3" t="s">
-        <v>6960</v>
+        <v>6959</v>
       </c>
       <c r="B711" s="49" t="s">
         <v>3873</v>
@@ -47728,7 +47728,7 @@
     </row>
     <row r="726" spans="1:15">
       <c r="A726" s="3" t="s">
-        <v>6952</v>
+        <v>6951</v>
       </c>
       <c r="B726" s="49" t="s">
         <v>3948</v>
@@ -47763,7 +47763,7 @@
     </row>
     <row r="727" spans="1:15">
       <c r="A727" s="3" t="s">
-        <v>6967</v>
+        <v>6966</v>
       </c>
       <c r="B727" s="49" t="s">
         <v>3953</v>
@@ -49527,7 +49527,7 @@
     </row>
     <row r="774" spans="1:15">
       <c r="A774" s="3" t="s">
-        <v>6966</v>
+        <v>6965</v>
       </c>
       <c r="B774" s="49" t="s">
         <v>4193</v>
@@ -50131,7 +50131,7 @@
     </row>
     <row r="790" spans="1:15">
       <c r="A790" s="3" t="s">
-        <v>6934</v>
+        <v>6933</v>
       </c>
       <c r="B790" s="49" t="s">
         <v>4274</v>
@@ -50727,7 +50727,7 @@
     </row>
     <row r="806" spans="1:15">
       <c r="A806" s="3" t="s">
-        <v>6950</v>
+        <v>6949</v>
       </c>
       <c r="B806" s="49" t="s">
         <v>4355</v>
@@ -51059,7 +51059,7 @@
     </row>
     <row r="815" spans="1:15">
       <c r="A815" s="3" t="s">
-        <v>6935</v>
+        <v>6934</v>
       </c>
       <c r="B815" s="49" t="s">
         <v>4395</v>
@@ -51139,7 +51139,7 @@
         <v>4404</v>
       </c>
       <c r="E817" s="37" t="s">
-        <v>7040</v>
+        <v>7039</v>
       </c>
       <c r="F817" s="37" t="s">
         <v>6723</v>
@@ -51833,7 +51833,7 @@
     </row>
     <row r="836" spans="1:15">
       <c r="A836" s="3" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="B836" s="49" t="s">
         <v>4493</v>
@@ -53400,7 +53400,7 @@
     </row>
     <row r="878" spans="1:15">
       <c r="A878" s="3" t="s">
-        <v>6948</v>
+        <v>6947</v>
       </c>
       <c r="B878" s="49" t="s">
         <v>4673</v>
@@ -53847,7 +53847,7 @@
     </row>
     <row r="890" spans="1:15">
       <c r="A890" s="3" t="s">
-        <v>6951</v>
+        <v>6950</v>
       </c>
       <c r="B890" s="49" t="s">
         <v>4732</v>
@@ -54639,7 +54639,7 @@
     </row>
     <row r="911" spans="1:15">
       <c r="A911" s="3" t="s">
-        <v>6937</v>
+        <v>6936</v>
       </c>
       <c r="B911" s="49" t="s">
         <v>4832</v>
@@ -55708,7 +55708,7 @@
     </row>
     <row r="940" spans="1:15">
       <c r="A940" s="3" t="s">
-        <v>6938</v>
+        <v>6937</v>
       </c>
       <c r="B940" s="49" t="s">
         <v>4961</v>
@@ -56040,7 +56040,7 @@
     </row>
     <row r="949" spans="1:15">
       <c r="A949" s="3" t="s">
-        <v>6947</v>
+        <v>6946</v>
       </c>
       <c r="B949" s="49" t="s">
         <v>5002</v>
@@ -56193,7 +56193,7 @@
     </row>
     <row r="953" spans="1:15">
       <c r="A953" s="3" t="s">
-        <v>6949</v>
+        <v>6948</v>
       </c>
       <c r="B953" s="49" t="s">
         <v>5027</v>
@@ -56719,7 +56719,7 @@
     </row>
     <row r="967" spans="1:15">
       <c r="A967" s="3" t="s">
-        <v>6953</v>
+        <v>6952</v>
       </c>
       <c r="B967" s="49" t="s">
         <v>5104</v>
@@ -56761,10 +56761,10 @@
     </row>
     <row r="968" spans="1:15">
       <c r="A968" s="3" t="s">
-        <v>6954</v>
+        <v>6953</v>
       </c>
       <c r="B968" s="49" t="s">
-        <v>6933</v>
+        <v>6932</v>
       </c>
       <c r="C968" s="3" t="s">
         <v>774</v>
@@ -56898,7 +56898,7 @@
         <v>794</v>
       </c>
       <c r="F971" s="3" t="s">
-        <v>6939</v>
+        <v>6938</v>
       </c>
       <c r="G971" s="3" t="s">
         <v>3967</v>
@@ -59242,7 +59242,7 @@
     </row>
     <row r="1032" spans="1:15">
       <c r="A1032" s="3" t="s">
-        <v>6907</v>
+        <v>7047</v>
       </c>
       <c r="B1032" s="49" t="s">
         <v>5133</v>
@@ -59343,7 +59343,7 @@
         <v>2690</v>
       </c>
       <c r="B1035" s="49" t="s">
-        <v>6908</v>
+        <v>6907</v>
       </c>
       <c r="C1035" s="3" t="s">
         <v>1069</v>
@@ -59382,10 +59382,10 @@
     </row>
     <row r="1036" spans="1:15">
       <c r="A1036" s="3" t="s">
-        <v>6955</v>
+        <v>6954</v>
       </c>
       <c r="B1036" s="49" t="s">
-        <v>6909</v>
+        <v>6908</v>
       </c>
       <c r="C1036" s="3" t="s">
         <v>1076</v>
@@ -59421,10 +59421,10 @@
     </row>
     <row r="1037" spans="1:15">
       <c r="A1037" s="3" t="s">
+        <v>6909</v>
+      </c>
+      <c r="B1037" s="49" t="s">
         <v>6910</v>
-      </c>
-      <c r="B1037" s="49" t="s">
-        <v>6911</v>
       </c>
       <c r="C1037" s="3" t="s">
         <v>1082</v>
@@ -59462,7 +59462,7 @@
     </row>
     <row r="1038" spans="1:15">
       <c r="A1038" s="31" t="s">
-        <v>6913</v>
+        <v>6912</v>
       </c>
       <c r="B1038" s="49" t="s">
         <v>5891</v>
@@ -59477,7 +59477,7 @@
         <v>1089</v>
       </c>
       <c r="F1038" s="3" t="s">
-        <v>6912</v>
+        <v>6911</v>
       </c>
       <c r="H1038" s="3" t="s">
         <v>1054</v>
@@ -59503,7 +59503,7 @@
         <v>2691</v>
       </c>
       <c r="B1039" s="49" t="s">
-        <v>6914</v>
+        <v>6913</v>
       </c>
       <c r="C1039" s="3" t="s">
         <v>1091</v>
@@ -59541,7 +59541,7 @@
         <v>2692</v>
       </c>
       <c r="B1040" s="49" t="s">
-        <v>6915</v>
+        <v>6914</v>
       </c>
       <c r="C1040" s="3" t="s">
         <v>1096</v>
@@ -59576,7 +59576,7 @@
     </row>
     <row r="1041" spans="1:15">
       <c r="A1041" s="3" t="s">
-        <v>6916</v>
+        <v>6915</v>
       </c>
       <c r="B1041" s="49" t="s">
         <v>6133</v>
@@ -59665,7 +59665,7 @@
         <v>5137</v>
       </c>
       <c r="F1043" s="3" t="s">
-        <v>6917</v>
+        <v>6916</v>
       </c>
       <c r="G1043" s="3" t="s">
         <v>4460</v>
@@ -59692,7 +59692,7 @@
         <v>2693</v>
       </c>
       <c r="B1044" s="49" t="s">
-        <v>6918</v>
+        <v>6917</v>
       </c>
       <c r="C1044" s="3" t="s">
         <v>1109</v>
@@ -59731,7 +59731,7 @@
     </row>
     <row r="1045" spans="1:15">
       <c r="A1045" s="3" t="s">
-        <v>6919</v>
+        <v>6918</v>
       </c>
       <c r="B1045" s="49" t="s">
         <v>5138</v>
@@ -59769,7 +59769,7 @@
     </row>
     <row r="1046" spans="1:15">
       <c r="A1046" s="3" t="s">
-        <v>6920</v>
+        <v>6919</v>
       </c>
       <c r="B1046" s="49" t="s">
         <v>5139</v>
@@ -59784,7 +59784,7 @@
         <v>5853</v>
       </c>
       <c r="F1046" s="3" t="s">
-        <v>6921</v>
+        <v>6920</v>
       </c>
       <c r="H1046" s="3" t="s">
         <v>254</v>
@@ -59820,7 +59820,7 @@
         <v>6130</v>
       </c>
       <c r="F1047" s="3" t="s">
-        <v>6922</v>
+        <v>6921</v>
       </c>
       <c r="H1047" s="3" t="s">
         <v>6131</v>
@@ -59847,7 +59847,7 @@
     </row>
     <row r="1048" spans="1:15">
       <c r="A1048" s="3" t="s">
-        <v>6923</v>
+        <v>6922</v>
       </c>
       <c r="B1048" s="49" t="s">
         <v>6137</v>
@@ -59862,7 +59862,7 @@
         <v>1120</v>
       </c>
       <c r="F1048" s="3" t="s">
-        <v>6924</v>
+        <v>6923</v>
       </c>
       <c r="H1048" s="3" t="s">
         <v>6139</v>
@@ -59888,7 +59888,7 @@
         <v>2694</v>
       </c>
       <c r="B1049" s="49" t="s">
-        <v>6925</v>
+        <v>6924</v>
       </c>
       <c r="C1049" s="3" t="s">
         <v>1121</v>
@@ -59926,10 +59926,10 @@
     </row>
     <row r="1050" spans="1:15">
       <c r="A1050" s="3" t="s">
+        <v>6925</v>
+      </c>
+      <c r="B1050" s="49" t="s">
         <v>6926</v>
-      </c>
-      <c r="B1050" s="49" t="s">
-        <v>6927</v>
       </c>
       <c r="C1050" s="3" t="s">
         <v>1127</v>
@@ -59968,10 +59968,10 @@
     </row>
     <row r="1051" spans="1:15">
       <c r="A1051" s="3" t="s">
+        <v>6927</v>
+      </c>
+      <c r="B1051" s="49" t="s">
         <v>6928</v>
-      </c>
-      <c r="B1051" s="49" t="s">
-        <v>6929</v>
       </c>
       <c r="C1051" s="3" t="s">
         <v>1134</v>
@@ -60047,7 +60047,7 @@
         <v>1142</v>
       </c>
       <c r="B1053" s="49" t="s">
-        <v>6930</v>
+        <v>6929</v>
       </c>
       <c r="C1053" s="3" t="s">
         <v>1143</v>
@@ -60080,10 +60080,10 @@
     </row>
     <row r="1054" spans="1:15">
       <c r="A1054" s="3" t="s">
+        <v>6930</v>
+      </c>
+      <c r="B1054" s="49" t="s">
         <v>6931</v>
-      </c>
-      <c r="B1054" s="49" t="s">
-        <v>6932</v>
       </c>
       <c r="C1054" s="3" t="s">
         <v>1147</v>
@@ -60220,7 +60220,7 @@
         <v>6596</v>
       </c>
       <c r="B1058" s="47" t="s">
-        <v>7033</v>
+        <v>7032</v>
       </c>
       <c r="C1058" s="37" t="s">
         <v>5353</v>
@@ -60229,10 +60229,10 @@
         <v>171</v>
       </c>
       <c r="E1058" s="21" t="s">
+        <v>7033</v>
+      </c>
+      <c r="F1058" s="3" t="s">
         <v>7034</v>
-      </c>
-      <c r="F1058" s="3" t="s">
-        <v>7035</v>
       </c>
       <c r="H1058" s="3" t="s">
         <v>4205</v>
@@ -60241,7 +60241,7 @@
         <v>575</v>
       </c>
       <c r="J1058" s="22" t="s">
-        <v>7036</v>
+        <v>7035</v>
       </c>
       <c r="K1058" s="22" t="s">
         <v>156</v>
@@ -60530,19 +60530,19 @@
     </row>
     <row r="1066" spans="1:15">
       <c r="A1066" s="3" t="s">
+        <v>6968</v>
+      </c>
+      <c r="B1066" s="49" t="s">
         <v>6969</v>
       </c>
-      <c r="B1066" s="49" t="s">
+      <c r="C1066" s="21" t="s">
         <v>6970</v>
       </c>
-      <c r="C1066" s="21" t="s">
+      <c r="E1066" s="21" t="s">
         <v>6971</v>
       </c>
-      <c r="E1066" s="21" t="s">
+      <c r="F1066" s="3" t="s">
         <v>6972</v>
-      </c>
-      <c r="F1066" s="3" t="s">
-        <v>6973</v>
       </c>
       <c r="H1066" s="3" t="s">
         <v>168</v>
@@ -60551,7 +60551,7 @@
         <v>2380</v>
       </c>
       <c r="J1066" s="22" t="s">
-        <v>6974</v>
+        <v>6973</v>
       </c>
       <c r="K1066" s="22" t="s">
         <v>156</v>
@@ -60568,13 +60568,13 @@
     </row>
     <row r="1067" spans="1:15">
       <c r="A1067" s="3" t="s">
+        <v>6976</v>
+      </c>
+      <c r="B1067" s="49" t="s">
         <v>6977</v>
       </c>
-      <c r="B1067" s="49" t="s">
+      <c r="L1067" t="s">
         <v>6978</v>
-      </c>
-      <c r="L1067" t="s">
-        <v>6979</v>
       </c>
       <c r="O1067" t="s">
         <v>1479</v>
@@ -60582,19 +60582,19 @@
     </row>
     <row r="1068" spans="1:15">
       <c r="A1068" s="3" t="s">
+        <v>6982</v>
+      </c>
+      <c r="B1068" s="49" t="s">
         <v>6983</v>
       </c>
-      <c r="B1068" s="49" t="s">
+      <c r="C1068" s="21" t="s">
         <v>6984</v>
-      </c>
-      <c r="C1068" s="21" t="s">
-        <v>6985</v>
       </c>
       <c r="D1068" s="23" t="s">
         <v>172</v>
       </c>
       <c r="F1068" s="3" t="s">
-        <v>6986</v>
+        <v>6985</v>
       </c>
       <c r="H1068" s="3" t="s">
         <v>1545</v>
@@ -60603,19 +60603,19 @@
         <v>575</v>
       </c>
       <c r="J1068" s="22" t="s">
+        <v>6986</v>
+      </c>
+      <c r="K1068" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="L1068" t="s">
         <v>6987</v>
-      </c>
-      <c r="K1068" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="L1068" t="s">
-        <v>6988</v>
       </c>
       <c r="M1068" s="46" t="s">
         <v>5811</v>
       </c>
       <c r="N1068" t="s">
-        <v>6988</v>
+        <v>6987</v>
       </c>
       <c r="O1068" t="s">
         <v>997</v>
@@ -60623,22 +60623,22 @@
     </row>
     <row r="1069" spans="1:15">
       <c r="A1069" s="3" t="s">
+        <v>6988</v>
+      </c>
+      <c r="B1069" s="49" t="s">
         <v>6989</v>
       </c>
-      <c r="B1069" s="49" t="s">
+      <c r="C1069" s="21" t="s">
         <v>6990</v>
-      </c>
-      <c r="C1069" s="21" t="s">
-        <v>6991</v>
       </c>
       <c r="D1069" s="23" t="s">
         <v>171</v>
       </c>
       <c r="E1069" s="21" t="s">
-        <v>6992</v>
+        <v>6991</v>
       </c>
       <c r="F1069" s="3" t="s">
-        <v>7029</v>
+        <v>7028</v>
       </c>
       <c r="H1069" s="3" t="s">
         <v>180</v>
@@ -60647,7 +60647,7 @@
         <v>575</v>
       </c>
       <c r="J1069" s="22" t="s">
-        <v>7030</v>
+        <v>7029</v>
       </c>
       <c r="K1069" s="22" t="s">
         <v>156</v>
@@ -60661,22 +60661,22 @@
     </row>
     <row r="1070" spans="1:15">
       <c r="A1070" s="3" t="s">
+        <v>7004</v>
+      </c>
+      <c r="B1070" s="49" t="s">
         <v>7005</v>
       </c>
-      <c r="B1070" s="49" t="s">
+      <c r="C1070" s="21" t="s">
         <v>7006</v>
-      </c>
-      <c r="C1070" s="21" t="s">
-        <v>7007</v>
       </c>
       <c r="D1070" s="23" t="s">
         <v>835</v>
       </c>
       <c r="E1070" s="21" t="s">
+        <v>7007</v>
+      </c>
+      <c r="F1070" s="3" t="s">
         <v>7008</v>
-      </c>
-      <c r="F1070" s="3" t="s">
-        <v>7009</v>
       </c>
       <c r="H1070" s="3" t="s">
         <v>2257</v>
@@ -60685,13 +60685,13 @@
         <v>575</v>
       </c>
       <c r="J1070" s="22" t="s">
+        <v>7009</v>
+      </c>
+      <c r="K1070" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="L1070" t="s">
         <v>7010</v>
-      </c>
-      <c r="K1070" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="L1070" t="s">
-        <v>7011</v>
       </c>
       <c r="M1070" s="46" t="s">
         <v>2761</v>
@@ -60702,19 +60702,19 @@
     </row>
     <row r="1071" spans="1:15">
       <c r="A1071" s="3" t="s">
+        <v>7016</v>
+      </c>
+      <c r="B1071" s="49" t="s">
+        <v>7030</v>
+      </c>
+      <c r="C1071" s="21" t="s">
         <v>7017</v>
       </c>
-      <c r="B1071" s="49" t="s">
-        <v>7031</v>
-      </c>
-      <c r="C1071" s="21" t="s">
+      <c r="E1071" s="21" t="s">
         <v>7018</v>
       </c>
-      <c r="E1071" s="21" t="s">
+      <c r="F1071" s="3" t="s">
         <v>7019</v>
-      </c>
-      <c r="F1071" s="3" t="s">
-        <v>7020</v>
       </c>
       <c r="H1071" s="3" t="s">
         <v>224</v>
@@ -60723,7 +60723,7 @@
         <v>575</v>
       </c>
       <c r="J1071" s="22" t="s">
-        <v>7021</v>
+        <v>7020</v>
       </c>
       <c r="K1071" s="22" t="s">
         <v>156</v>
@@ -60740,28 +60740,28 @@
     </row>
     <row r="1072" spans="1:15">
       <c r="A1072" s="3" t="s">
+        <v>7021</v>
+      </c>
+      <c r="B1072" s="49" t="s">
+        <v>7031</v>
+      </c>
+      <c r="C1072" s="21" t="s">
         <v>7022</v>
       </c>
-      <c r="B1072" s="49" t="s">
-        <v>7032</v>
-      </c>
-      <c r="C1072" s="21" t="s">
+      <c r="E1072" s="21" t="s">
         <v>7023</v>
       </c>
-      <c r="E1072" s="21" t="s">
+      <c r="F1072" s="3" t="s">
         <v>7024</v>
-      </c>
-      <c r="F1072" s="3" t="s">
-        <v>7025</v>
       </c>
       <c r="H1072" s="3" t="s">
         <v>283</v>
       </c>
       <c r="I1072" s="22" t="s">
+        <v>7025</v>
+      </c>
+      <c r="J1072" s="22" t="s">
         <v>7026</v>
-      </c>
-      <c r="J1072" s="22" t="s">
-        <v>7027</v>
       </c>
       <c r="K1072" s="22" t="s">
         <v>156</v>
@@ -60776,7 +60776,7 @@
         <v>816</v>
       </c>
       <c r="O1072" t="s">
-        <v>7028</v>
+        <v>7027</v>
       </c>
     </row>
     <row r="1073" spans="1:15">
@@ -60825,13 +60825,13 @@
     </row>
     <row r="1074" spans="1:15">
       <c r="A1074" s="3" t="s">
-        <v>6996</v>
+        <v>6995</v>
       </c>
       <c r="B1074" s="49" t="s">
         <v>5812</v>
       </c>
       <c r="C1074" s="21" t="s">
-        <v>6999</v>
+        <v>6998</v>
       </c>
       <c r="D1074" s="23" t="s">
         <v>171</v>
@@ -60867,13 +60867,13 @@
     </row>
     <row r="1075" spans="1:15">
       <c r="A1075" s="3" t="s">
-        <v>6993</v>
+        <v>6992</v>
       </c>
       <c r="B1075" s="49" t="s">
         <v>5813</v>
       </c>
       <c r="C1075" s="21" t="s">
-        <v>7000</v>
+        <v>6999</v>
       </c>
       <c r="D1075" s="23" t="s">
         <v>175</v>
@@ -60909,13 +60909,13 @@
     </row>
     <row r="1076" spans="1:15">
       <c r="A1076" s="3" t="s">
-        <v>6997</v>
+        <v>6996</v>
       </c>
       <c r="B1076" s="49" t="s">
         <v>5814</v>
       </c>
       <c r="C1076" s="21" t="s">
-        <v>7001</v>
+        <v>7000</v>
       </c>
       <c r="D1076" s="23" t="s">
         <v>171</v>
@@ -61081,13 +61081,13 @@
     </row>
     <row r="1080" spans="1:15">
       <c r="A1080" s="3" t="s">
-        <v>6998</v>
+        <v>6997</v>
       </c>
       <c r="B1080" s="49" t="s">
         <v>5817</v>
       </c>
       <c r="C1080" s="21" t="s">
-        <v>7002</v>
+        <v>7001</v>
       </c>
       <c r="D1080" s="23" t="s">
         <v>2283</v>
@@ -61469,13 +61469,13 @@
     </row>
     <row r="1089" spans="1:15">
       <c r="A1089" s="3" t="s">
-        <v>6994</v>
+        <v>6993</v>
       </c>
       <c r="B1089" s="49" t="s">
         <v>5828</v>
       </c>
       <c r="C1089" s="21" t="s">
-        <v>7003</v>
+        <v>7002</v>
       </c>
       <c r="D1089" s="23" t="s">
         <v>858</v>
@@ -61900,13 +61900,13 @@
     </row>
     <row r="1099" spans="1:15">
       <c r="A1099" s="3" t="s">
+        <v>7012</v>
+      </c>
+      <c r="B1099" s="49" t="s">
         <v>7013</v>
       </c>
-      <c r="B1099" s="49" t="s">
+      <c r="C1099" s="21" t="s">
         <v>7014</v>
-      </c>
-      <c r="C1099" s="21" t="s">
-        <v>7015</v>
       </c>
       <c r="D1099" s="23" t="s">
         <v>172</v>
@@ -61918,7 +61918,7 @@
         <v>2887</v>
       </c>
       <c r="H1099" s="3" t="s">
-        <v>7016</v>
+        <v>7015</v>
       </c>
       <c r="I1099" s="22" t="s">
         <v>575</v>
@@ -61944,22 +61944,22 @@
     </row>
     <row r="1100" spans="1:15">
       <c r="A1100" s="3" t="s">
+        <v>7040</v>
+      </c>
+      <c r="B1100" s="49" t="s">
         <v>7041</v>
       </c>
-      <c r="B1100" s="49" t="s">
+      <c r="C1100" s="21" t="s">
         <v>7042</v>
       </c>
-      <c r="C1100" s="21" t="s">
+      <c r="D1100" s="23" t="s">
         <v>7043</v>
       </c>
-      <c r="D1100" s="23" t="s">
+      <c r="E1100" s="21" t="s">
         <v>7044</v>
       </c>
-      <c r="E1100" s="21" t="s">
+      <c r="F1100" s="3" t="s">
         <v>7045</v>
-      </c>
-      <c r="F1100" s="3" t="s">
-        <v>7046</v>
       </c>
       <c r="H1100" s="3" t="s">
         <v>281</v>
@@ -61968,7 +61968,7 @@
         <v>575</v>
       </c>
       <c r="J1100" s="22" t="s">
-        <v>7047</v>
+        <v>7046</v>
       </c>
       <c r="K1100" s="22" t="s">
         <v>156</v>

</xml_diff>

<commit_message>
2024-10-26 @ 11:16 - v5.B.1.xlsb - 20 321 lignes - Compile - OK
* modAppli_Utils.bas
   - Changer l'ordre de vérification (Entête & Détails) pour FAC_Projets_*
* modCAR_Liste_Agée.bas
   - Éliminer du code en commentaires (mort)
* modFAC_Finale.bas
   - Éliminer du code en commentaires (mort)
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C492D92C-15EF-4667-BCDF-9E77BB13B872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87F4C5B-16CF-44C7-AEED-1D7393DD391E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39540" yWindow="-15030" windowWidth="21600" windowHeight="11385" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12023" uniqueCount="7059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12030" uniqueCount="7062">
   <si>
     <t>Client_ID</t>
   </si>
@@ -21227,6 +21227,15 @@
   </si>
   <si>
     <t>Gestion GMCB Inc. [Louis Parker][Giovanni Cinquino]</t>
+  </si>
+  <si>
+    <t>François-Pierre Laforest</t>
+  </si>
+  <si>
+    <t>1809</t>
+  </si>
+  <si>
+    <t>francoisplaforest@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -22301,7 +22310,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
   <sheetPr codeName="wshClients"/>
-  <dimension ref="A1:O1102"/>
+  <dimension ref="A1:O1103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
       <pane ySplit="615" topLeftCell="A380" activePane="bottomLeft"/>
@@ -62103,6 +62112,29 @@
       </c>
       <c r="O1102" t="s">
         <v>713</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:15">
+      <c r="A1103" s="3" t="s">
+        <v>7059</v>
+      </c>
+      <c r="B1103" s="49" t="s">
+        <v>7060</v>
+      </c>
+      <c r="C1103" s="21" t="s">
+        <v>7059</v>
+      </c>
+      <c r="D1103" s="23" t="s">
+        <v>5981</v>
+      </c>
+      <c r="E1103" s="21" t="s">
+        <v>7061</v>
+      </c>
+      <c r="L1103" t="s">
+        <v>3683</v>
+      </c>
+      <c r="M1103" s="46" t="s">
+        <v>2761</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2024-10-27 @ 14:58 - v4.1.xlsm
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C413A2-309A-4085-9B2D-BE365A497E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB94CBB0-19B9-4742-ACA0-6219DA7D3BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12049" uniqueCount="7069">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12065" uniqueCount="7077">
   <si>
     <t>Client_ID</t>
   </si>
@@ -21257,6 +21257,30 @@
   </si>
   <si>
     <t>15 chemin des Mésanges</t>
+  </si>
+  <si>
+    <t>Marie Guay</t>
+  </si>
+  <si>
+    <t>1811</t>
+  </si>
+  <si>
+    <t>Gestion MARIE GUAY</t>
+  </si>
+  <si>
+    <t>marie.guay@outlook.com</t>
+  </si>
+  <si>
+    <t>3467 rue de la Noraye</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Michel Lemieux</t>
+  </si>
+  <si>
+    <t>Pas d'appartement, donc pas de 's'</t>
   </si>
 </sst>
 </file>
@@ -22340,7 +22364,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
   <sheetPr codeName="wshClients"/>
-  <dimension ref="A1:Q1104"/>
+  <dimension ref="A1:Q1105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="615" topLeftCell="A2" activePane="bottomLeft"/>
@@ -24462,7 +24486,7 @@
       </c>
       <c r="P56" s="25"/>
       <c r="Q56" s="52">
-        <v>45591.535173611112</v>
+        <v>45592.351817129631</v>
       </c>
     </row>
     <row r="57" spans="1:17">
@@ -65541,6 +65565,59 @@
       </c>
       <c r="Q1104" s="52">
         <v>45591.537442129629</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:17">
+      <c r="A1105" s="3" t="s">
+        <v>7069</v>
+      </c>
+      <c r="B1105" s="49" t="s">
+        <v>7070</v>
+      </c>
+      <c r="C1105" s="49" t="s">
+        <v>7071</v>
+      </c>
+      <c r="D1105" s="21" t="s">
+        <v>7069</v>
+      </c>
+      <c r="E1105" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1105" s="21" t="s">
+        <v>7072</v>
+      </c>
+      <c r="G1105" s="3" t="s">
+        <v>7073</v>
+      </c>
+      <c r="H1105" s="3" t="s">
+        <v>7076</v>
+      </c>
+      <c r="I1105" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1105" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="K1105" s="22" t="s">
+        <v>2904</v>
+      </c>
+      <c r="L1105" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1105" t="s">
+        <v>7074</v>
+      </c>
+      <c r="N1105" s="46" t="s">
+        <v>5787</v>
+      </c>
+      <c r="O1105" t="s">
+        <v>4829</v>
+      </c>
+      <c r="P1105" t="s">
+        <v>7075</v>
+      </c>
+      <c r="Q1105" s="52">
+        <v>45591.804178240738</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2024-11-28 2 13:49 - v.5.F.2.xlsb - 21 806 lignes - Compile OK
* Changement de casse
   - .add ---> .Add
   - .list ---> .List
* modDev_Utils.bas
   - Travail sur une procédure pour identifier les procédures non-utilisées - Abandon
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8AC478-7EA9-45B5-AFA1-687FF85A2D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1694C779-F0D5-4537-9A9C-D6F6FAA2912F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13124" uniqueCount="7824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13143" uniqueCount="7842">
   <si>
     <t>Client_ID</t>
   </si>
@@ -23522,6 +23522,60 @@
   </si>
   <si>
     <t>&lt;Yves Beauchamps&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Robert Grégoire&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Mikael Dallaire&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Sci-Tek (Sylvain Pelletier)&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Compresseurs Gagnon&gt;</t>
+  </si>
+  <si>
+    <t>&lt;SVGO&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Groupe Privilège&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Gina Dubée Inc.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Manon Coulombe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Richard Provencher&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Accès Habitation&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Yanick Favreau&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Gestenv&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Gilbert Tanguay&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Éric L'Archvêque&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Stéphane et Serge Gariépy&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Sphère DI Inc.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bullseye AI&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Prospection&gt;</t>
   </si>
 </sst>
 </file>
@@ -24607,7 +24661,7 @@
   <sheetPr codeName="wshClients"/>
   <dimension ref="A1:Q1107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A381" workbookViewId="0">
       <pane ySplit="615" activePane="bottomLeft"/>
       <selection activeCell="Q1" sqref="Q1:Q1048576"/>
       <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
@@ -39311,6 +39365,9 @@
       <c r="B381" s="49" t="s">
         <v>2765</v>
       </c>
+      <c r="C381" s="49" t="s">
+        <v>7824</v>
+      </c>
       <c r="D381" s="21" t="s">
         <v>435</v>
       </c>
@@ -40335,6 +40392,9 @@
       <c r="B403" s="49" t="s">
         <v>5476</v>
       </c>
+      <c r="C403" s="49" t="s">
+        <v>7825</v>
+      </c>
       <c r="D403" s="21" t="s">
         <v>488</v>
       </c>
@@ -40592,6 +40652,9 @@
       <c r="B409" s="49" t="s">
         <v>2771</v>
       </c>
+      <c r="C409" s="49" t="s">
+        <v>7826</v>
+      </c>
       <c r="D409" s="21" t="s">
         <v>512</v>
       </c>
@@ -41964,6 +42027,9 @@
       <c r="B439" s="49" t="s">
         <v>6233</v>
       </c>
+      <c r="C439" s="49" t="s">
+        <v>7827</v>
+      </c>
       <c r="D439" s="21" t="s">
         <v>643</v>
       </c>
@@ -42458,6 +42524,9 @@
       <c r="B450" s="49" t="s">
         <v>6006</v>
       </c>
+      <c r="C450" s="49" t="s">
+        <v>7828</v>
+      </c>
       <c r="D450" s="21" t="s">
         <v>678</v>
       </c>
@@ -44551,6 +44620,9 @@
       <c r="B498" s="49" t="s">
         <v>2919</v>
       </c>
+      <c r="C498" s="49" t="s">
+        <v>7829</v>
+      </c>
       <c r="D498" s="37" t="s">
         <v>2920</v>
       </c>
@@ -45304,6 +45376,9 @@
       </c>
       <c r="B516" s="49" t="s">
         <v>2999</v>
+      </c>
+      <c r="C516" s="49" t="s">
+        <v>7830</v>
       </c>
       <c r="D516" s="37" t="s">
         <v>3000</v>
@@ -51003,6 +51078,9 @@
       <c r="B649" s="49" t="s">
         <v>3603</v>
       </c>
+      <c r="C649" s="49" t="s">
+        <v>7831</v>
+      </c>
       <c r="D649" s="37" t="s">
         <v>3604</v>
       </c>
@@ -51630,6 +51708,9 @@
       <c r="B664" s="49" t="s">
         <v>3666</v>
       </c>
+      <c r="C664" s="49" t="s">
+        <v>7832</v>
+      </c>
       <c r="D664" s="37" t="s">
         <v>3667</v>
       </c>
@@ -52667,6 +52748,9 @@
       <c r="B688" s="49" t="s">
         <v>3767</v>
       </c>
+      <c r="C688" s="49" t="s">
+        <v>7833</v>
+      </c>
       <c r="D688" s="37" t="s">
         <v>3768</v>
       </c>
@@ -53507,6 +53591,9 @@
       <c r="B708" s="49" t="s">
         <v>3856</v>
       </c>
+      <c r="C708" s="49" t="s">
+        <v>7834</v>
+      </c>
       <c r="D708" s="37" t="s">
         <v>3857</v>
       </c>
@@ -53674,6 +53761,9 @@
       <c r="B712" s="49" t="s">
         <v>3869</v>
       </c>
+      <c r="C712" s="49" t="s">
+        <v>7835</v>
+      </c>
       <c r="D712" s="37" t="s">
         <v>3870</v>
       </c>
@@ -54287,6 +54377,9 @@
       </c>
       <c r="B726" s="49" t="s">
         <v>3932</v>
+      </c>
+      <c r="C726" s="49" t="s">
+        <v>7836</v>
       </c>
       <c r="D726" s="37" t="s">
         <v>3933</v>
@@ -57244,6 +57337,9 @@
       <c r="B794" s="49" t="s">
         <v>4270</v>
       </c>
+      <c r="C794" s="49" t="s">
+        <v>7837</v>
+      </c>
       <c r="D794" s="37" t="s">
         <v>4271</v>
       </c>
@@ -57284,6 +57380,9 @@
       </c>
       <c r="B795" s="49" t="s">
         <v>4276</v>
+      </c>
+      <c r="C795" s="49" t="s">
+        <v>7831</v>
       </c>
       <c r="D795" s="37" t="s">
         <v>4277</v>
@@ -58403,6 +58502,9 @@
       <c r="B821" s="49" t="s">
         <v>4396</v>
       </c>
+      <c r="C821" s="49" t="s">
+        <v>7838</v>
+      </c>
       <c r="D821" s="37" t="s">
         <v>4397</v>
       </c>
@@ -62669,6 +62771,9 @@
       <c r="B920" s="49" t="s">
         <v>4842</v>
       </c>
+      <c r="C920" s="49" t="s">
+        <v>7839</v>
+      </c>
       <c r="D920" s="37" t="s">
         <v>4843</v>
       </c>
@@ -65378,6 +65483,9 @@
       <c r="B982" s="49" t="s">
         <v>5089</v>
       </c>
+      <c r="C982" s="49" t="s">
+        <v>7840</v>
+      </c>
       <c r="D982" s="3" t="s">
         <v>834</v>
       </c>
@@ -65760,6 +65868,9 @@
       </c>
       <c r="B991" s="49" t="s">
         <v>6814</v>
+      </c>
+      <c r="C991" s="49" t="s">
+        <v>7841</v>
       </c>
       <c r="D991" s="3"/>
       <c r="G991" s="3" t="s">

</xml_diff>

<commit_message>
2024-12-04 @ 13:25 - v5.G.0.xlsb - 22 031 lignes - Compile OK
* Problème de casse
   - x ---> X
   - valeur ---> Valeur
* modStatsHeures.bas
   - Dans wshTEC_TDB_Data, déplacer les 4 blocs d'information vers le haut (AF)
* ufStatsHeures.frm
   - Déplacer la procédure 'UserForm_Initialize' au début du module
   - Permettre le simple clic ou le double clic pour voir une semaine spécifique
   - Toujours avoir la semaine couverte dans le libellé (Total de la semaine)
   - Ajout du log dans les procédures du module
* wshENC_Saisie.doccls
   - Modifier l'approche pour 'colorer' les cellules qui auraient pu perdre leurs couleurs
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79E4E02-C033-405C-B07A-19C7A14C6D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE6FB81-B02A-47E3-894B-3E6BE6624DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="30960" windowHeight="12204" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="348" yWindow="348" windowWidth="20640" windowHeight="8340" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13172" uniqueCount="7850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13158" uniqueCount="7848">
   <si>
     <t>Client_ID</t>
   </si>
@@ -23573,12 +23573,6 @@
   </si>
   <si>
     <t>&lt;Prospection&gt;</t>
-  </si>
-  <si>
-    <t>1812</t>
-  </si>
-  <si>
-    <t>4445970 Canada Inc.</t>
   </si>
   <si>
     <t>Constructions Gilles Garry Inc. [Gilles Garry]</t>
@@ -24683,7 +24677,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
   <sheetPr codeName="wshClients"/>
-  <dimension ref="A1:Q1109"/>
+  <dimension ref="A1:Q1108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A381" workbookViewId="0">
       <pane ySplit="612" activePane="bottomLeft"/>
@@ -70217,7 +70211,7 @@
     </row>
     <row r="1088" spans="1:17">
       <c r="A1088" s="3" t="s">
-        <v>7843</v>
+        <v>7841</v>
       </c>
       <c r="B1088" s="49" t="s">
         <v>5798</v>
@@ -71176,34 +71170,34 @@
     </row>
     <row r="1108" spans="1:17">
       <c r="A1108" s="3" t="s">
-        <v>6568</v>
+        <v>7842</v>
       </c>
       <c r="B1108" s="49" t="s">
-        <v>7841</v>
+        <v>7843</v>
       </c>
       <c r="C1108" s="49" t="s">
-        <v>7842</v>
+        <v>7844</v>
       </c>
       <c r="D1108" s="21" t="s">
-        <v>2336</v>
+        <v>7845</v>
       </c>
       <c r="E1108" s="23" t="s">
-        <v>172</v>
+        <v>7846</v>
       </c>
       <c r="F1108" s="21" t="s">
-        <v>2337</v>
+        <v>2264</v>
       </c>
       <c r="G1108" s="3" t="s">
-        <v>2338</v>
+        <v>7847</v>
       </c>
       <c r="I1108" s="3" t="s">
-        <v>2339</v>
+        <v>2244</v>
       </c>
       <c r="J1108" s="22" t="s">
         <v>575</v>
       </c>
       <c r="K1108" s="22" t="s">
-        <v>2340</v>
+        <v>2266</v>
       </c>
       <c r="L1108" s="22" t="s">
         <v>156</v>
@@ -71212,62 +71206,15 @@
         <v>323</v>
       </c>
       <c r="N1108" s="46" t="s">
-        <v>5781</v>
+        <v>5790</v>
       </c>
       <c r="O1108" t="s">
         <v>323</v>
       </c>
+      <c r="P1108" t="s">
+        <v>5333</v>
+      </c>
       <c r="Q1108" s="52">
-        <v>45626.353472222225</v>
-      </c>
-    </row>
-    <row r="1109" spans="1:17">
-      <c r="A1109" s="3" t="s">
-        <v>7844</v>
-      </c>
-      <c r="B1109" s="49" t="s">
-        <v>7845</v>
-      </c>
-      <c r="C1109" s="49" t="s">
-        <v>7846</v>
-      </c>
-      <c r="D1109" s="21" t="s">
-        <v>7847</v>
-      </c>
-      <c r="E1109" s="23" t="s">
-        <v>7848</v>
-      </c>
-      <c r="F1109" s="21" t="s">
-        <v>2264</v>
-      </c>
-      <c r="G1109" s="3" t="s">
-        <v>7849</v>
-      </c>
-      <c r="I1109" s="3" t="s">
-        <v>2244</v>
-      </c>
-      <c r="J1109" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="K1109" s="22" t="s">
-        <v>2266</v>
-      </c>
-      <c r="L1109" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="M1109" t="s">
-        <v>323</v>
-      </c>
-      <c r="N1109" s="46" t="s">
-        <v>5790</v>
-      </c>
-      <c r="O1109" t="s">
-        <v>323</v>
-      </c>
-      <c r="P1109" t="s">
-        <v>5333</v>
-      </c>
-      <c r="Q1109" s="52">
         <v>45626.360127314816</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2024-12-12 @ 07:58 - Clients_v4.3.xlsm - 1 553 lignes - Compile OK
* Changement de nom
   - 'CM_Log_Record' ---> 'CM_Log_Activities'
* modUtils.bas
   - "yyyy-mm-dd_hh:mm:ss" ---> "yyyy-mm-dd hh:mm:ss") & "." & ms
   - "LogClientsApp.txt" ---> "LogClientsApp.log"
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CC73F3-5EA7-4D82-9D10-2EF121F38E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDCEE9D-9BA0-4017-BA23-34BAA7EAB45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="38280" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13172" uniqueCount="7855">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13186" uniqueCount="7863">
   <si>
     <t>Client_ID</t>
   </si>
@@ -23615,6 +23615,30 @@
   </si>
   <si>
     <t>j.boutin@pareassurances.com</t>
+  </si>
+  <si>
+    <t>DCP Dermoscience Inc. [Maude St-Pierre]</t>
+  </si>
+  <si>
+    <t>1812</t>
+  </si>
+  <si>
+    <t>DCP Dermoscience Inc.</t>
+  </si>
+  <si>
+    <t>maude@dcpdermoscience.com</t>
+  </si>
+  <si>
+    <t>102-1275 rue Gay-Lussac</t>
+  </si>
+  <si>
+    <t>J4B 7K1</t>
+  </si>
+  <si>
+    <t>Sauvageau Hanley</t>
+  </si>
+  <si>
+    <t>Maude Saint-Pierre</t>
   </si>
 </sst>
 </file>
@@ -24680,7 +24704,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
   <sheetPr codeName="wshClients"/>
-  <dimension ref="A1:Q1109"/>
+  <dimension ref="A1:Q1110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A381" workbookViewId="0">
       <pane ySplit="615" topLeftCell="A1077" activePane="bottomLeft"/>
@@ -71323,6 +71347,53 @@
       <c r="P1109" s="25"/>
       <c r="Q1109" s="48">
         <v>45602.422002314815</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:17">
+      <c r="A1110" s="3" t="s">
+        <v>7855</v>
+      </c>
+      <c r="B1110" s="45" t="s">
+        <v>7856</v>
+      </c>
+      <c r="C1110" s="45" t="s">
+        <v>7857</v>
+      </c>
+      <c r="D1110" s="21" t="s">
+        <v>7862</v>
+      </c>
+      <c r="E1110" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1110" s="21" t="s">
+        <v>7858</v>
+      </c>
+      <c r="G1110" s="3" t="s">
+        <v>7859</v>
+      </c>
+      <c r="I1110" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="J1110" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="K1110" s="22" t="s">
+        <v>7860</v>
+      </c>
+      <c r="L1110" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1110" t="s">
+        <v>256</v>
+      </c>
+      <c r="N1110" s="42" t="s">
+        <v>5788</v>
+      </c>
+      <c r="O1110" t="s">
+        <v>7861</v>
+      </c>
+      <c r="Q1110" s="48">
+        <v>45637.428865740738</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2024-12-19 @ 21:55 - v5.H.3.xlsb - 23 618 lignes - Compile OK
* Problème de casse
   - Goto ---> GoTo
   - .List ---> .list
   - Valeur ---> valeur
* modAppli_Utils.bas
   - Éliminer quelques déclarations de variables inutiles
   - Dans 'checkTEC' optimiser le traitement avec la mémoire et autres améliorations
* modFAC_Confirmation.bas
   - Mise au point du programme & tests
* wshFAC_Confirmation.doccls
   - Mise au point du programme & tests
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDCEE9D-9BA0-4017-BA23-34BAA7EAB45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34DDC8A-D4A3-4D9F-B010-C11D369E3460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Clients!$A$1:$P$1109</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Clients!$A$1:$P$1111</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Fournisseurs!$A$1:$K$20</definedName>
     <definedName name="dnrClients" localSheetId="0">OFFSET(Clients!#REF!,1,0,COUNTA(Clients!$A:$A)-1,2)</definedName>
     <definedName name="dnrClients" localSheetId="1">OFFSET(Fournisseurs!$A$1,1,0,COUNTA(Fournisseurs!$A:$A)-1,2)</definedName>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13186" uniqueCount="7863">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13200" uniqueCount="7870">
   <si>
     <t>Client_ID</t>
   </si>
@@ -23639,6 +23639,27 @@
   </si>
   <si>
     <t>Maude Saint-Pierre</t>
+  </si>
+  <si>
+    <t>Bois Franc Rive Sud Inc. [François Brodeur]</t>
+  </si>
+  <si>
+    <t>1815</t>
+  </si>
+  <si>
+    <t>Bois Franc Rive Sud Inc.</t>
+  </si>
+  <si>
+    <t>François Brodeur</t>
+  </si>
+  <si>
+    <t>fbrodeur@rive-sud.ca</t>
+  </si>
+  <si>
+    <t>SuiteA-4200 boul. Matte</t>
+  </si>
+  <si>
+    <t>J4Y 2Z2</t>
   </si>
 </sst>
 </file>
@@ -24704,12 +24725,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
   <sheetPr codeName="wshClients"/>
-  <dimension ref="A1:Q1110"/>
+  <dimension ref="A1:Q1111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A381" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A1077" activePane="bottomLeft"/>
+      <pane ySplit="615" topLeftCell="A1057" activePane="bottomLeft"/>
       <selection activeCell="Q1" sqref="Q1:Q1048576"/>
-      <selection pane="bottomLeft" activeCell="D1092" sqref="D1092"/>
+      <selection pane="bottomLeft" activeCell="A1074" sqref="A1074"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -69848,228 +69869,228 @@
     </row>
     <row r="1079" spans="1:17">
       <c r="A1079" s="3" t="s">
-        <v>7841</v>
+        <v>7855</v>
       </c>
       <c r="B1079" s="45" t="s">
-        <v>7842</v>
+        <v>7856</v>
       </c>
       <c r="C1079" s="45" t="s">
-        <v>7843</v>
+        <v>7857</v>
       </c>
       <c r="D1079" s="34" t="s">
-        <v>7844</v>
+        <v>7862</v>
       </c>
       <c r="E1079" s="23" t="s">
-        <v>7845</v>
+        <v>171</v>
       </c>
       <c r="F1079" s="34" t="s">
-        <v>2264</v>
+        <v>7858</v>
       </c>
       <c r="G1079" s="34" t="s">
-        <v>7846</v>
+        <v>7859</v>
       </c>
       <c r="I1079" s="34" t="s">
-        <v>2244</v>
+        <v>249</v>
       </c>
       <c r="J1079" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1079" s="34" t="s">
-        <v>2266</v>
+        <v>7860</v>
       </c>
       <c r="L1079" s="34" t="s">
         <v>156</v>
       </c>
       <c r="M1079" s="25" t="s">
-        <v>323</v>
+        <v>256</v>
       </c>
       <c r="N1079" s="24" t="s">
-        <v>5789</v>
+        <v>5788</v>
       </c>
       <c r="O1079" s="25" t="s">
-        <v>323</v>
-      </c>
-      <c r="P1079" s="25" t="s">
-        <v>5332</v>
-      </c>
+        <v>7861</v>
+      </c>
+      <c r="P1079" s="25"/>
       <c r="Q1079" s="48">
-        <v>45626.360127314816</v>
+        <v>45637.428865740738</v>
       </c>
     </row>
     <row r="1080" spans="1:17">
       <c r="A1080" s="3" t="s">
-        <v>7851</v>
+        <v>7841</v>
       </c>
       <c r="B1080" s="45" t="s">
-        <v>7847</v>
+        <v>7842</v>
       </c>
       <c r="C1080" s="45" t="s">
-        <v>7852</v>
+        <v>7843</v>
       </c>
       <c r="D1080" s="34" t="s">
-        <v>7848</v>
+        <v>7844</v>
       </c>
       <c r="E1080" s="23" t="s">
-        <v>172</v>
+        <v>7845</v>
       </c>
       <c r="F1080" s="34" t="s">
-        <v>7849</v>
+        <v>2264</v>
       </c>
       <c r="G1080" s="34" t="s">
-        <v>7853</v>
+        <v>7846</v>
       </c>
       <c r="I1080" s="34" t="s">
-        <v>305</v>
+        <v>2244</v>
       </c>
       <c r="J1080" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1080" s="34" t="s">
-        <v>1793</v>
+        <v>2266</v>
       </c>
       <c r="L1080" s="34" t="s">
         <v>156</v>
       </c>
       <c r="M1080" s="25" t="s">
-        <v>4174</v>
-      </c>
-      <c r="N1080" s="24"/>
+        <v>323</v>
+      </c>
+      <c r="N1080" s="24" t="s">
+        <v>5789</v>
+      </c>
       <c r="O1080" s="25" t="s">
-        <v>7850</v>
+        <v>323</v>
       </c>
       <c r="P1080" s="25" t="s">
-        <v>4174</v>
+        <v>5332</v>
       </c>
       <c r="Q1080" s="48">
-        <v>45630.409421296295</v>
+        <v>45626.360127314816</v>
       </c>
     </row>
     <row r="1081" spans="1:17">
       <c r="A1081" s="3" t="s">
-        <v>6551</v>
+        <v>7851</v>
       </c>
       <c r="B1081" s="45" t="s">
-        <v>46</v>
+        <v>7847</v>
       </c>
       <c r="C1081" s="45" t="s">
-        <v>7520</v>
+        <v>7852</v>
       </c>
       <c r="D1081" s="34" t="s">
-        <v>2263</v>
+        <v>7848</v>
       </c>
       <c r="E1081" s="23" t="s">
         <v>172</v>
       </c>
       <c r="F1081" s="34" t="s">
-        <v>2264</v>
+        <v>7849</v>
       </c>
       <c r="G1081" s="34" t="s">
-        <v>2265</v>
+        <v>7853</v>
       </c>
       <c r="I1081" s="34" t="s">
-        <v>2244</v>
+        <v>305</v>
       </c>
       <c r="J1081" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1081" s="34" t="s">
-        <v>2266</v>
+        <v>1793</v>
       </c>
       <c r="L1081" s="34" t="s">
         <v>156</v>
       </c>
       <c r="M1081" s="25" t="s">
-        <v>323</v>
-      </c>
-      <c r="N1081" s="24" t="s">
-        <v>5789</v>
-      </c>
+        <v>4174</v>
+      </c>
+      <c r="N1081" s="24"/>
       <c r="O1081" s="25" t="s">
-        <v>323</v>
+        <v>7850</v>
       </c>
       <c r="P1081" s="25" t="s">
-        <v>5332</v>
+        <v>4174</v>
       </c>
       <c r="Q1081" s="48">
-        <v>45591.506944444445</v>
+        <v>45630.409421296295</v>
       </c>
     </row>
     <row r="1082" spans="1:17">
       <c r="A1082" s="3" t="s">
-        <v>6968</v>
+        <v>7863</v>
       </c>
       <c r="B1082" s="45" t="s">
-        <v>5790</v>
+        <v>7864</v>
       </c>
       <c r="C1082" s="45" t="s">
-        <v>7510</v>
+        <v>7865</v>
       </c>
       <c r="D1082" s="34" t="s">
-        <v>6971</v>
+        <v>7866</v>
       </c>
       <c r="E1082" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="F1082" s="34"/>
+        <v>172</v>
+      </c>
+      <c r="F1082" s="34" t="s">
+        <v>7867</v>
+      </c>
       <c r="G1082" s="34" t="s">
-        <v>2267</v>
+        <v>7868</v>
       </c>
       <c r="I1082" s="34" t="s">
-        <v>2244</v>
+        <v>248</v>
       </c>
       <c r="J1082" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1082" s="34" t="s">
-        <v>2268</v>
+        <v>7869</v>
       </c>
       <c r="L1082" s="34" t="s">
         <v>156</v>
       </c>
       <c r="M1082" s="25" t="s">
-        <v>323</v>
+        <v>1475</v>
       </c>
       <c r="N1082" s="24" t="s">
         <v>2754</v>
       </c>
-      <c r="O1082" s="25" t="s">
-        <v>323</v>
-      </c>
-      <c r="P1082" s="25"/>
+      <c r="O1082" s="25"/>
+      <c r="P1082" s="25" t="s">
+        <v>1475</v>
+      </c>
       <c r="Q1082" s="48">
-        <v>45592.251759259256</v>
+        <v>45644.407916666663</v>
       </c>
     </row>
     <row r="1083" spans="1:17">
       <c r="A1083" s="3" t="s">
-        <v>6965</v>
+        <v>6551</v>
       </c>
       <c r="B1083" s="45" t="s">
-        <v>5791</v>
+        <v>46</v>
       </c>
       <c r="C1083" s="45" t="s">
-        <v>7486</v>
+        <v>7520</v>
       </c>
       <c r="D1083" s="34" t="s">
-        <v>6972</v>
+        <v>2263</v>
       </c>
       <c r="E1083" s="23" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F1083" s="34" t="s">
-        <v>2269</v>
+        <v>2264</v>
       </c>
       <c r="G1083" s="34" t="s">
-        <v>2270</v>
+        <v>2265</v>
       </c>
       <c r="I1083" s="34" t="s">
-        <v>254</v>
+        <v>2244</v>
       </c>
       <c r="J1083" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1083" s="34" t="s">
-        <v>2271</v>
+        <v>2266</v>
       </c>
       <c r="L1083" s="34" t="s">
         <v>156</v>
@@ -70078,46 +70099,46 @@
         <v>323</v>
       </c>
       <c r="N1083" s="24" t="s">
-        <v>5609</v>
+        <v>5789</v>
       </c>
       <c r="O1083" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="P1083" s="25"/>
+      <c r="P1083" s="25" t="s">
+        <v>5332</v>
+      </c>
       <c r="Q1083" s="48">
         <v>45591.506944444445</v>
       </c>
     </row>
     <row r="1084" spans="1:17">
       <c r="A1084" s="3" t="s">
-        <v>6969</v>
+        <v>6968</v>
       </c>
       <c r="B1084" s="45" t="s">
-        <v>5792</v>
+        <v>5790</v>
       </c>
       <c r="C1084" s="45" t="s">
-        <v>7518</v>
+        <v>7510</v>
       </c>
       <c r="D1084" s="34" t="s">
-        <v>6973</v>
+        <v>6971</v>
       </c>
       <c r="E1084" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="F1084" s="34" t="s">
-        <v>1581</v>
-      </c>
+      <c r="F1084" s="34"/>
       <c r="G1084" s="34" t="s">
-        <v>2272</v>
+        <v>2267</v>
       </c>
       <c r="I1084" s="34" t="s">
-        <v>157</v>
+        <v>2244</v>
       </c>
       <c r="J1084" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1084" s="34" t="s">
-        <v>1583</v>
+        <v>2268</v>
       </c>
       <c r="L1084" s="34" t="s">
         <v>156</v>
@@ -70131,43 +70152,41 @@
       <c r="O1084" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="P1084" s="25" t="s">
-        <v>5332</v>
-      </c>
+      <c r="P1084" s="25"/>
       <c r="Q1084" s="48">
-        <v>45591.506944444445</v>
+        <v>45592.251759259256</v>
       </c>
     </row>
     <row r="1085" spans="1:17">
       <c r="A1085" s="3" t="s">
-        <v>6552</v>
+        <v>6965</v>
       </c>
       <c r="B1085" s="45" t="s">
-        <v>5793</v>
+        <v>5791</v>
       </c>
       <c r="C1085" s="45" t="s">
-        <v>7501</v>
+        <v>7486</v>
       </c>
       <c r="D1085" s="34" t="s">
-        <v>2273</v>
+        <v>6972</v>
       </c>
       <c r="E1085" s="23" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="F1085" s="34" t="s">
-        <v>2274</v>
+        <v>2269</v>
       </c>
       <c r="G1085" s="34" t="s">
-        <v>2275</v>
+        <v>2270</v>
       </c>
       <c r="I1085" s="34" t="s">
-        <v>2276</v>
+        <v>254</v>
       </c>
       <c r="J1085" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1085" s="34" t="s">
-        <v>2277</v>
+        <v>2271</v>
       </c>
       <c r="L1085" s="34" t="s">
         <v>156</v>
@@ -70176,7 +70195,7 @@
         <v>323</v>
       </c>
       <c r="N1085" s="24" t="s">
-        <v>2754</v>
+        <v>5609</v>
       </c>
       <c r="O1085" s="25" t="s">
         <v>323</v>
@@ -70188,34 +70207,34 @@
     </row>
     <row r="1086" spans="1:17">
       <c r="A1086" s="3" t="s">
-        <v>6553</v>
+        <v>6969</v>
       </c>
       <c r="B1086" s="45" t="s">
-        <v>48</v>
+        <v>5792</v>
       </c>
       <c r="C1086" s="45" t="s">
-        <v>7281</v>
+        <v>7518</v>
       </c>
       <c r="D1086" s="34" t="s">
-        <v>2278</v>
+        <v>6973</v>
       </c>
       <c r="E1086" s="23" t="s">
-        <v>2279</v>
+        <v>171</v>
       </c>
       <c r="F1086" s="34" t="s">
-        <v>718</v>
+        <v>1581</v>
       </c>
       <c r="G1086" s="34" t="s">
-        <v>2280</v>
+        <v>2272</v>
       </c>
       <c r="I1086" s="34" t="s">
-        <v>1167</v>
+        <v>157</v>
       </c>
       <c r="J1086" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1086" s="34" t="s">
-        <v>721</v>
+        <v>1583</v>
       </c>
       <c r="L1086" s="34" t="s">
         <v>156</v>
@@ -70230,7 +70249,7 @@
         <v>323</v>
       </c>
       <c r="P1086" s="25" t="s">
-        <v>5802</v>
+        <v>5332</v>
       </c>
       <c r="Q1086" s="48">
         <v>45591.506944444445</v>
@@ -70238,34 +70257,34 @@
     </row>
     <row r="1087" spans="1:17">
       <c r="A1087" s="3" t="s">
-        <v>6554</v>
+        <v>6552</v>
       </c>
       <c r="B1087" s="45" t="s">
-        <v>5794</v>
+        <v>5793</v>
       </c>
       <c r="C1087" s="45" t="s">
-        <v>7566</v>
+        <v>7501</v>
       </c>
       <c r="D1087" s="34" t="s">
-        <v>2281</v>
+        <v>2273</v>
       </c>
       <c r="E1087" s="23" t="s">
-        <v>2279</v>
+        <v>172</v>
       </c>
       <c r="F1087" s="34" t="s">
-        <v>2282</v>
+        <v>2274</v>
       </c>
       <c r="G1087" s="34" t="s">
-        <v>2283</v>
+        <v>2275</v>
       </c>
       <c r="I1087" s="34" t="s">
-        <v>2284</v>
+        <v>2276</v>
       </c>
       <c r="J1087" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1087" s="34" t="s">
-        <v>2285</v>
+        <v>2277</v>
       </c>
       <c r="L1087" s="34" t="s">
         <v>156</v>
@@ -70286,34 +70305,34 @@
     </row>
     <row r="1088" spans="1:17">
       <c r="A1088" s="3" t="s">
-        <v>6970</v>
+        <v>6553</v>
       </c>
       <c r="B1088" s="45" t="s">
-        <v>5795</v>
+        <v>48</v>
       </c>
       <c r="C1088" s="45" t="s">
-        <v>7565</v>
+        <v>7281</v>
       </c>
       <c r="D1088" s="34" t="s">
-        <v>6974</v>
+        <v>2278</v>
       </c>
       <c r="E1088" s="23" t="s">
         <v>2279</v>
       </c>
       <c r="F1088" s="34" t="s">
-        <v>2287</v>
+        <v>718</v>
       </c>
       <c r="G1088" s="34" t="s">
-        <v>2288</v>
+        <v>2280</v>
       </c>
       <c r="I1088" s="34" t="s">
-        <v>423</v>
+        <v>1167</v>
       </c>
       <c r="J1088" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1088" s="34" t="s">
-        <v>2289</v>
+        <v>721</v>
       </c>
       <c r="L1088" s="34" t="s">
         <v>156</v>
@@ -70328,7 +70347,7 @@
         <v>323</v>
       </c>
       <c r="P1088" s="25" t="s">
-        <v>5332</v>
+        <v>5802</v>
       </c>
       <c r="Q1088" s="48">
         <v>45591.506944444445</v>
@@ -70336,34 +70355,34 @@
     </row>
     <row r="1089" spans="1:17">
       <c r="A1089" s="3" t="s">
-        <v>6555</v>
+        <v>6554</v>
       </c>
       <c r="B1089" s="45" t="s">
-        <v>5796</v>
+        <v>5794</v>
       </c>
       <c r="C1089" s="45" t="s">
-        <v>7602</v>
+        <v>7566</v>
       </c>
       <c r="D1089" s="34" t="s">
-        <v>2290</v>
+        <v>2281</v>
       </c>
       <c r="E1089" s="23" t="s">
-        <v>172</v>
+        <v>2279</v>
       </c>
       <c r="F1089" s="34" t="s">
-        <v>2291</v>
+        <v>2282</v>
       </c>
       <c r="G1089" s="34" t="s">
-        <v>2292</v>
+        <v>2283</v>
       </c>
       <c r="I1089" s="34" t="s">
-        <v>248</v>
+        <v>2284</v>
       </c>
       <c r="J1089" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1089" s="34" t="s">
-        <v>2293</v>
+        <v>2285</v>
       </c>
       <c r="L1089" s="34" t="s">
         <v>156</v>
@@ -70377,43 +70396,41 @@
       <c r="O1089" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="P1089" s="25" t="s">
-        <v>5332</v>
-      </c>
+      <c r="P1089" s="25"/>
       <c r="Q1089" s="48">
         <v>45591.506944444445</v>
       </c>
     </row>
     <row r="1090" spans="1:17">
       <c r="A1090" s="3" t="s">
-        <v>7840</v>
+        <v>6970</v>
       </c>
       <c r="B1090" s="45" t="s">
-        <v>5797</v>
+        <v>5795</v>
       </c>
       <c r="C1090" s="45" t="s">
-        <v>7499</v>
+        <v>7565</v>
       </c>
       <c r="D1090" s="34" t="s">
-        <v>2294</v>
+        <v>6974</v>
       </c>
       <c r="E1090" s="23" t="s">
-        <v>172</v>
+        <v>2279</v>
       </c>
       <c r="F1090" s="34" t="s">
-        <v>2295</v>
+        <v>2287</v>
       </c>
       <c r="G1090" s="34" t="s">
-        <v>2296</v>
+        <v>2288</v>
       </c>
       <c r="I1090" s="34" t="s">
-        <v>2297</v>
+        <v>423</v>
       </c>
       <c r="J1090" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1090" s="34" t="s">
-        <v>2298</v>
+        <v>2289</v>
       </c>
       <c r="L1090" s="34" t="s">
         <v>156</v>
@@ -70422,46 +70439,48 @@
         <v>323</v>
       </c>
       <c r="N1090" s="24" t="s">
-        <v>5798</v>
+        <v>2754</v>
       </c>
       <c r="O1090" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="P1090" s="25"/>
+      <c r="P1090" s="25" t="s">
+        <v>5332</v>
+      </c>
       <c r="Q1090" s="48">
-        <v>45626.355034722219</v>
+        <v>45591.506944444445</v>
       </c>
     </row>
     <row r="1091" spans="1:17">
       <c r="A1091" s="3" t="s">
-        <v>6556</v>
+        <v>6555</v>
       </c>
       <c r="B1091" s="45" t="s">
-        <v>5799</v>
+        <v>5796</v>
       </c>
       <c r="C1091" s="45" t="s">
-        <v>7505</v>
+        <v>7602</v>
       </c>
       <c r="D1091" s="34" t="s">
-        <v>2299</v>
+        <v>2290</v>
       </c>
       <c r="E1091" s="23" t="s">
-        <v>2300</v>
+        <v>172</v>
       </c>
       <c r="F1091" s="34" t="s">
-        <v>2301</v>
+        <v>2291</v>
       </c>
       <c r="G1091" s="34" t="s">
-        <v>2302</v>
+        <v>2292</v>
       </c>
       <c r="I1091" s="34" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="J1091" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1091" s="34" t="s">
-        <v>2303</v>
+        <v>2293</v>
       </c>
       <c r="L1091" s="34" t="s">
         <v>156</v>
@@ -70475,41 +70494,43 @@
       <c r="O1091" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="P1091" s="25"/>
+      <c r="P1091" s="25" t="s">
+        <v>5332</v>
+      </c>
       <c r="Q1091" s="48">
         <v>45591.506944444445</v>
       </c>
     </row>
     <row r="1092" spans="1:17">
       <c r="A1092" s="3" t="s">
-        <v>6557</v>
+        <v>7840</v>
       </c>
       <c r="B1092" s="45" t="s">
-        <v>5800</v>
+        <v>5797</v>
       </c>
       <c r="C1092" s="45" t="s">
-        <v>7313</v>
+        <v>7499</v>
       </c>
       <c r="D1092" s="34" t="s">
-        <v>2304</v>
+        <v>2294</v>
       </c>
       <c r="E1092" s="23" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F1092" s="34" t="s">
-        <v>2305</v>
+        <v>2295</v>
       </c>
       <c r="G1092" s="34" t="s">
-        <v>2306</v>
+        <v>2296</v>
       </c>
       <c r="I1092" s="34" t="s">
-        <v>1533</v>
+        <v>2297</v>
       </c>
       <c r="J1092" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1092" s="34" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
       <c r="L1092" s="34" t="s">
         <v>156</v>
@@ -70518,46 +70539,46 @@
         <v>323</v>
       </c>
       <c r="N1092" s="24" t="s">
-        <v>5360</v>
+        <v>5798</v>
       </c>
       <c r="O1092" s="25" t="s">
         <v>323</v>
       </c>
       <c r="P1092" s="25"/>
       <c r="Q1092" s="48">
-        <v>45591.506944444445</v>
+        <v>45626.355034722219</v>
       </c>
     </row>
     <row r="1093" spans="1:17">
       <c r="A1093" s="3" t="s">
-        <v>6558</v>
+        <v>6556</v>
       </c>
       <c r="B1093" s="45" t="s">
-        <v>5801</v>
+        <v>5799</v>
       </c>
       <c r="C1093" s="45" t="s">
-        <v>7503</v>
+        <v>7505</v>
       </c>
       <c r="D1093" s="34" t="s">
-        <v>2304</v>
+        <v>2299</v>
       </c>
       <c r="E1093" s="23" t="s">
-        <v>171</v>
+        <v>2300</v>
       </c>
       <c r="F1093" s="34" t="s">
-        <v>2305</v>
+        <v>2301</v>
       </c>
       <c r="G1093" s="34" t="s">
-        <v>2306</v>
+        <v>2302</v>
       </c>
       <c r="I1093" s="34" t="s">
-        <v>1533</v>
+        <v>254</v>
       </c>
       <c r="J1093" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1093" s="34" t="s">
-        <v>2307</v>
+        <v>2303</v>
       </c>
       <c r="L1093" s="34" t="s">
         <v>156</v>
@@ -70566,7 +70587,7 @@
         <v>323</v>
       </c>
       <c r="N1093" s="24" t="s">
-        <v>5360</v>
+        <v>2754</v>
       </c>
       <c r="O1093" s="25" t="s">
         <v>323</v>
@@ -70578,31 +70599,34 @@
     </row>
     <row r="1094" spans="1:17">
       <c r="A1094" s="3" t="s">
-        <v>5867</v>
+        <v>6557</v>
       </c>
       <c r="B1094" s="45" t="s">
-        <v>5331</v>
+        <v>5800</v>
+      </c>
+      <c r="C1094" s="45" t="s">
+        <v>7313</v>
       </c>
       <c r="D1094" s="34" t="s">
-        <v>2278</v>
+        <v>2304</v>
       </c>
       <c r="E1094" s="23" t="s">
-        <v>835</v>
+        <v>171</v>
       </c>
       <c r="F1094" s="34" t="s">
-        <v>718</v>
+        <v>2305</v>
       </c>
       <c r="G1094" s="34" t="s">
-        <v>2280</v>
+        <v>2306</v>
       </c>
       <c r="I1094" s="34" t="s">
-        <v>1167</v>
+        <v>1533</v>
       </c>
       <c r="J1094" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1094" s="34" t="s">
-        <v>721</v>
+        <v>2307</v>
       </c>
       <c r="L1094" s="34" t="s">
         <v>156</v>
@@ -70611,48 +70635,46 @@
         <v>323</v>
       </c>
       <c r="N1094" s="24" t="s">
-        <v>5798</v>
+        <v>5360</v>
       </c>
       <c r="O1094" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="P1094" s="25" t="s">
-        <v>5332</v>
-      </c>
+      <c r="P1094" s="25"/>
       <c r="Q1094" s="48">
         <v>45591.506944444445</v>
       </c>
     </row>
     <row r="1095" spans="1:17">
       <c r="A1095" s="3" t="s">
-        <v>6559</v>
+        <v>6558</v>
       </c>
       <c r="B1095" s="45" t="s">
-        <v>5803</v>
+        <v>5801</v>
       </c>
       <c r="C1095" s="45" t="s">
-        <v>7512</v>
+        <v>7503</v>
       </c>
       <c r="D1095" s="34" t="s">
-        <v>2286</v>
+        <v>2304</v>
       </c>
       <c r="E1095" s="23" t="s">
-        <v>858</v>
+        <v>171</v>
       </c>
       <c r="F1095" s="34" t="s">
-        <v>2287</v>
+        <v>2305</v>
       </c>
       <c r="G1095" s="34" t="s">
-        <v>2288</v>
+        <v>2306</v>
       </c>
       <c r="I1095" s="34" t="s">
-        <v>423</v>
+        <v>1533</v>
       </c>
       <c r="J1095" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1095" s="34" t="s">
-        <v>2289</v>
+        <v>2307</v>
       </c>
       <c r="L1095" s="34" t="s">
         <v>156</v>
@@ -70661,48 +70683,43 @@
         <v>323</v>
       </c>
       <c r="N1095" s="24" t="s">
-        <v>5804</v>
+        <v>5360</v>
       </c>
       <c r="O1095" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="P1095" s="25" t="s">
-        <v>5332</v>
-      </c>
+      <c r="P1095" s="25"/>
       <c r="Q1095" s="48">
         <v>45591.506944444445</v>
       </c>
     </row>
     <row r="1096" spans="1:17">
       <c r="A1096" s="3" t="s">
-        <v>6560</v>
+        <v>5867</v>
       </c>
       <c r="B1096" s="45" t="s">
-        <v>5805</v>
-      </c>
-      <c r="C1096" s="45" t="s">
-        <v>7546</v>
+        <v>5331</v>
       </c>
       <c r="D1096" s="34" t="s">
-        <v>2286</v>
+        <v>2278</v>
       </c>
       <c r="E1096" s="23" t="s">
-        <v>858</v>
+        <v>835</v>
       </c>
       <c r="F1096" s="34" t="s">
-        <v>2287</v>
+        <v>718</v>
       </c>
       <c r="G1096" s="34" t="s">
-        <v>2288</v>
+        <v>2280</v>
       </c>
       <c r="I1096" s="34" t="s">
-        <v>423</v>
+        <v>1167</v>
       </c>
       <c r="J1096" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1096" s="34" t="s">
-        <v>2289</v>
+        <v>721</v>
       </c>
       <c r="L1096" s="34" t="s">
         <v>156</v>
@@ -70711,7 +70728,7 @@
         <v>323</v>
       </c>
       <c r="N1096" s="24" t="s">
-        <v>5804</v>
+        <v>5798</v>
       </c>
       <c r="O1096" s="25" t="s">
         <v>323</v>
@@ -70725,34 +70742,34 @@
     </row>
     <row r="1097" spans="1:17">
       <c r="A1097" s="3" t="s">
-        <v>6966</v>
+        <v>6559</v>
       </c>
       <c r="B1097" s="45" t="s">
-        <v>5806</v>
+        <v>5803</v>
       </c>
       <c r="C1097" s="45" t="s">
-        <v>7442</v>
+        <v>7512</v>
       </c>
       <c r="D1097" s="34" t="s">
-        <v>6975</v>
+        <v>2286</v>
       </c>
       <c r="E1097" s="23" t="s">
         <v>858</v>
       </c>
       <c r="F1097" s="34" t="s">
-        <v>2308</v>
+        <v>2287</v>
       </c>
       <c r="G1097" s="34" t="s">
-        <v>2309</v>
+        <v>2288</v>
       </c>
       <c r="I1097" s="34" t="s">
-        <v>2310</v>
+        <v>423</v>
       </c>
       <c r="J1097" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1097" s="34" t="s">
-        <v>2311</v>
+        <v>2289</v>
       </c>
       <c r="L1097" s="34" t="s">
         <v>156</v>
@@ -70761,46 +70778,48 @@
         <v>323</v>
       </c>
       <c r="N1097" s="24" t="s">
-        <v>2754</v>
+        <v>5804</v>
       </c>
       <c r="O1097" s="25" t="s">
-        <v>2312</v>
-      </c>
-      <c r="P1097" s="25"/>
+        <v>323</v>
+      </c>
+      <c r="P1097" s="25" t="s">
+        <v>5332</v>
+      </c>
       <c r="Q1097" s="48">
         <v>45591.506944444445</v>
       </c>
     </row>
     <row r="1098" spans="1:17">
       <c r="A1098" s="3" t="s">
-        <v>6561</v>
+        <v>6560</v>
       </c>
       <c r="B1098" s="45" t="s">
-        <v>5807</v>
+        <v>5805</v>
       </c>
       <c r="C1098" s="45" t="s">
-        <v>7606</v>
+        <v>7546</v>
       </c>
       <c r="D1098" s="34" t="s">
-        <v>2313</v>
+        <v>2286</v>
       </c>
       <c r="E1098" s="23" t="s">
-        <v>172</v>
+        <v>858</v>
       </c>
       <c r="F1098" s="34" t="s">
-        <v>2314</v>
+        <v>2287</v>
       </c>
       <c r="G1098" s="34" t="s">
-        <v>2315</v>
+        <v>2288</v>
       </c>
       <c r="I1098" s="34" t="s">
-        <v>168</v>
+        <v>423</v>
       </c>
       <c r="J1098" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1098" s="34" t="s">
-        <v>2160</v>
+        <v>2289</v>
       </c>
       <c r="L1098" s="34" t="s">
         <v>156</v>
@@ -70809,49 +70828,48 @@
         <v>323</v>
       </c>
       <c r="N1098" s="24" t="s">
-        <v>5771</v>
+        <v>5804</v>
       </c>
       <c r="O1098" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="P1098" s="25"/>
+      <c r="P1098" s="25" t="s">
+        <v>5332</v>
+      </c>
       <c r="Q1098" s="48">
         <v>45591.506944444445</v>
       </c>
     </row>
     <row r="1099" spans="1:17">
       <c r="A1099" s="3" t="s">
-        <v>6562</v>
+        <v>6966</v>
       </c>
       <c r="B1099" s="45" t="s">
-        <v>5808</v>
+        <v>5806</v>
       </c>
       <c r="C1099" s="45" t="s">
-        <v>7489</v>
+        <v>7442</v>
       </c>
       <c r="D1099" s="34" t="s">
-        <v>2313</v>
+        <v>6975</v>
       </c>
       <c r="E1099" s="23" t="s">
-        <v>172</v>
+        <v>858</v>
       </c>
       <c r="F1099" s="34" t="s">
-        <v>2316</v>
+        <v>2308</v>
       </c>
       <c r="G1099" s="34" t="s">
-        <v>253</v>
-      </c>
-      <c r="H1099" s="3" t="s">
-        <v>2317</v>
+        <v>2309</v>
       </c>
       <c r="I1099" s="34" t="s">
-        <v>254</v>
+        <v>2310</v>
       </c>
       <c r="J1099" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1099" s="34" t="s">
-        <v>255</v>
+        <v>2311</v>
       </c>
       <c r="L1099" s="34" t="s">
         <v>156</v>
@@ -70863,45 +70881,43 @@
         <v>2754</v>
       </c>
       <c r="O1099" s="25" t="s">
-        <v>323</v>
-      </c>
-      <c r="P1099" s="25" t="s">
-        <v>2318</v>
-      </c>
+        <v>2312</v>
+      </c>
+      <c r="P1099" s="25"/>
       <c r="Q1099" s="48">
         <v>45591.506944444445</v>
       </c>
     </row>
     <row r="1100" spans="1:17">
       <c r="A1100" s="3" t="s">
-        <v>6563</v>
+        <v>6561</v>
       </c>
       <c r="B1100" s="45" t="s">
-        <v>5809</v>
+        <v>5807</v>
       </c>
       <c r="C1100" s="45" t="s">
-        <v>7420</v>
+        <v>7606</v>
       </c>
       <c r="D1100" s="34" t="s">
-        <v>2319</v>
+        <v>2313</v>
       </c>
       <c r="E1100" s="23" t="s">
         <v>172</v>
       </c>
       <c r="F1100" s="34" t="s">
-        <v>2320</v>
+        <v>2314</v>
       </c>
       <c r="G1100" s="34" t="s">
-        <v>2321</v>
+        <v>2315</v>
       </c>
       <c r="I1100" s="34" t="s">
-        <v>1648</v>
+        <v>168</v>
       </c>
       <c r="J1100" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1100" s="34" t="s">
-        <v>2322</v>
+        <v>2160</v>
       </c>
       <c r="L1100" s="34" t="s">
         <v>156</v>
@@ -70910,7 +70926,7 @@
         <v>323</v>
       </c>
       <c r="N1100" s="24" t="s">
-        <v>5789</v>
+        <v>5771</v>
       </c>
       <c r="O1100" s="25" t="s">
         <v>323</v>
@@ -70922,34 +70938,37 @@
     </row>
     <row r="1101" spans="1:17">
       <c r="A1101" s="3" t="s">
-        <v>6564</v>
+        <v>6562</v>
       </c>
       <c r="B1101" s="45" t="s">
-        <v>5333</v>
+        <v>5808</v>
       </c>
       <c r="C1101" s="45" t="s">
-        <v>7557</v>
+        <v>7489</v>
       </c>
       <c r="D1101" s="34" t="s">
-        <v>7700</v>
+        <v>2313</v>
       </c>
       <c r="E1101" s="23" t="s">
         <v>172</v>
       </c>
       <c r="F1101" s="34" t="s">
-        <v>2323</v>
+        <v>2316</v>
       </c>
       <c r="G1101" s="34" t="s">
-        <v>2324</v>
+        <v>253</v>
+      </c>
+      <c r="H1101" s="3" t="s">
+        <v>2317</v>
       </c>
       <c r="I1101" s="34" t="s">
-        <v>2325</v>
+        <v>254</v>
       </c>
       <c r="J1101" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1101" s="34" t="s">
-        <v>2326</v>
+        <v>255</v>
       </c>
       <c r="L1101" s="34" t="s">
         <v>156</v>
@@ -70963,41 +70982,43 @@
       <c r="O1101" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="P1101" s="25"/>
+      <c r="P1101" s="25" t="s">
+        <v>2318</v>
+      </c>
       <c r="Q1101" s="48">
-        <v>45599.491631944446</v>
+        <v>45591.506944444445</v>
       </c>
     </row>
     <row r="1102" spans="1:17">
       <c r="A1102" s="3" t="s">
-        <v>6565</v>
+        <v>6563</v>
       </c>
       <c r="B1102" s="45" t="s">
-        <v>5810</v>
+        <v>5809</v>
       </c>
       <c r="C1102" s="45" t="s">
-        <v>7504</v>
+        <v>7420</v>
       </c>
       <c r="D1102" s="34" t="s">
-        <v>2327</v>
+        <v>2319</v>
       </c>
       <c r="E1102" s="23" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F1102" s="34" t="s">
-        <v>2328</v>
+        <v>2320</v>
       </c>
       <c r="G1102" s="34" t="s">
-        <v>2306</v>
+        <v>2321</v>
       </c>
       <c r="I1102" s="34" t="s">
-        <v>1533</v>
+        <v>1648</v>
       </c>
       <c r="J1102" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1102" s="34" t="s">
-        <v>2307</v>
+        <v>2322</v>
       </c>
       <c r="L1102" s="34" t="s">
         <v>156</v>
@@ -71006,7 +71027,7 @@
         <v>323</v>
       </c>
       <c r="N1102" s="24" t="s">
-        <v>5360</v>
+        <v>5789</v>
       </c>
       <c r="O1102" s="25" t="s">
         <v>323</v>
@@ -71018,34 +71039,34 @@
     </row>
     <row r="1103" spans="1:17">
       <c r="A1103" s="3" t="s">
-        <v>7718</v>
+        <v>6564</v>
       </c>
       <c r="B1103" s="45" t="s">
-        <v>5811</v>
+        <v>5333</v>
       </c>
       <c r="C1103" s="45" t="s">
-        <v>7245</v>
+        <v>7557</v>
       </c>
       <c r="D1103" s="34" t="s">
-        <v>2299</v>
+        <v>7700</v>
       </c>
       <c r="E1103" s="23" t="s">
         <v>172</v>
       </c>
       <c r="F1103" s="34" t="s">
-        <v>2301</v>
+        <v>2323</v>
       </c>
       <c r="G1103" s="34" t="s">
-        <v>2329</v>
+        <v>2324</v>
       </c>
       <c r="I1103" s="34" t="s">
-        <v>249</v>
+        <v>2325</v>
       </c>
       <c r="J1103" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1103" s="34" t="s">
-        <v>2330</v>
+        <v>2326</v>
       </c>
       <c r="L1103" s="34" t="s">
         <v>156</v>
@@ -71054,49 +71075,46 @@
         <v>323</v>
       </c>
       <c r="N1103" s="24" t="s">
-        <v>5789</v>
+        <v>2754</v>
       </c>
       <c r="O1103" s="25" t="s">
         <v>323</v>
       </c>
       <c r="P1103" s="25"/>
       <c r="Q1103" s="48">
-        <v>45602.572002314817</v>
+        <v>45599.491631944446</v>
       </c>
     </row>
     <row r="1104" spans="1:17">
       <c r="A1104" s="3" t="s">
-        <v>6566</v>
+        <v>6565</v>
       </c>
       <c r="B1104" s="45" t="s">
-        <v>5812</v>
+        <v>5810</v>
       </c>
       <c r="C1104" s="45" t="s">
-        <v>7500</v>
+        <v>7504</v>
       </c>
       <c r="D1104" s="34" t="s">
-        <v>2331</v>
+        <v>2327</v>
       </c>
       <c r="E1104" s="23" t="s">
         <v>171</v>
       </c>
       <c r="F1104" s="34" t="s">
-        <v>2332</v>
+        <v>2328</v>
       </c>
       <c r="G1104" s="34" t="s">
-        <v>2333</v>
-      </c>
-      <c r="H1104" s="3" t="s">
-        <v>2334</v>
+        <v>2306</v>
       </c>
       <c r="I1104" s="34" t="s">
-        <v>254</v>
+        <v>1533</v>
       </c>
       <c r="J1104" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1104" s="34" t="s">
-        <v>2335</v>
+        <v>2307</v>
       </c>
       <c r="L1104" s="34" t="s">
         <v>156</v>
@@ -71105,7 +71123,7 @@
         <v>323</v>
       </c>
       <c r="N1104" s="24" t="s">
-        <v>5780</v>
+        <v>5360</v>
       </c>
       <c r="O1104" s="25" t="s">
         <v>323</v>
@@ -71117,34 +71135,34 @@
     </row>
     <row r="1105" spans="1:17">
       <c r="A1105" s="3" t="s">
-        <v>6567</v>
+        <v>7718</v>
       </c>
       <c r="B1105" s="45" t="s">
-        <v>5813</v>
+        <v>5811</v>
       </c>
       <c r="C1105" s="45" t="s">
-        <v>7612</v>
+        <v>7245</v>
       </c>
       <c r="D1105" s="34" t="s">
-        <v>2336</v>
+        <v>2299</v>
       </c>
       <c r="E1105" s="23" t="s">
         <v>172</v>
       </c>
       <c r="F1105" s="34" t="s">
-        <v>2337</v>
+        <v>2301</v>
       </c>
       <c r="G1105" s="34" t="s">
-        <v>2338</v>
+        <v>2329</v>
       </c>
       <c r="I1105" s="34" t="s">
-        <v>2339</v>
+        <v>249</v>
       </c>
       <c r="J1105" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1105" s="34" t="s">
-        <v>2340</v>
+        <v>2330</v>
       </c>
       <c r="L1105" s="34" t="s">
         <v>156</v>
@@ -71153,46 +71171,49 @@
         <v>323</v>
       </c>
       <c r="N1105" s="24" t="s">
-        <v>5780</v>
+        <v>5789</v>
       </c>
       <c r="O1105" s="25" t="s">
         <v>323</v>
       </c>
       <c r="P1105" s="25"/>
       <c r="Q1105" s="48">
-        <v>45591.506944444445</v>
+        <v>45602.572002314817</v>
       </c>
     </row>
     <row r="1106" spans="1:17">
       <c r="A1106" s="3" t="s">
-        <v>6568</v>
+        <v>6566</v>
       </c>
       <c r="B1106" s="45" t="s">
-        <v>5814</v>
+        <v>5812</v>
       </c>
       <c r="C1106" s="45" t="s">
-        <v>7507</v>
+        <v>7500</v>
       </c>
       <c r="D1106" s="34" t="s">
-        <v>2281</v>
+        <v>2331</v>
       </c>
       <c r="E1106" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F1106" s="34" t="s">
-        <v>2282</v>
+        <v>2332</v>
       </c>
       <c r="G1106" s="34" t="s">
-        <v>2283</v>
+        <v>2333</v>
+      </c>
+      <c r="H1106" s="3" t="s">
+        <v>2334</v>
       </c>
       <c r="I1106" s="34" t="s">
-        <v>2284</v>
+        <v>254</v>
       </c>
       <c r="J1106" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1106" s="34" t="s">
-        <v>2285</v>
+        <v>2335</v>
       </c>
       <c r="L1106" s="34" t="s">
         <v>156</v>
@@ -71201,7 +71222,7 @@
         <v>323</v>
       </c>
       <c r="N1106" s="24" t="s">
-        <v>2754</v>
+        <v>5780</v>
       </c>
       <c r="O1106" s="25" t="s">
         <v>323</v>
@@ -71213,34 +71234,34 @@
     </row>
     <row r="1107" spans="1:17">
       <c r="A1107" s="3" t="s">
-        <v>7717</v>
+        <v>6567</v>
       </c>
       <c r="B1107" s="45" t="s">
-        <v>6985</v>
+        <v>5813</v>
       </c>
       <c r="C1107" s="45" t="s">
-        <v>7234</v>
+        <v>7612</v>
       </c>
       <c r="D1107" s="34" t="s">
-        <v>2876</v>
+        <v>2336</v>
       </c>
       <c r="E1107" s="23" t="s">
         <v>172</v>
       </c>
       <c r="F1107" s="34" t="s">
-        <v>7854</v>
+        <v>2337</v>
       </c>
       <c r="G1107" s="34" t="s">
-        <v>2877</v>
+        <v>2338</v>
       </c>
       <c r="I1107" s="34" t="s">
-        <v>6986</v>
+        <v>2339</v>
       </c>
       <c r="J1107" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1107" s="34" t="s">
-        <v>2878</v>
+        <v>2340</v>
       </c>
       <c r="L1107" s="34" t="s">
         <v>156</v>
@@ -71249,191 +71270,240 @@
         <v>323</v>
       </c>
       <c r="N1107" s="24" t="s">
-        <v>5609</v>
+        <v>5780</v>
       </c>
       <c r="O1107" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="P1107" s="25" t="s">
-        <v>5332</v>
-      </c>
+      <c r="P1107" s="25"/>
       <c r="Q1107" s="48">
-        <v>45634.650567129633</v>
+        <v>45591.506944444445</v>
       </c>
     </row>
     <row r="1108" spans="1:17">
       <c r="A1108" s="3" t="s">
-        <v>7706</v>
+        <v>6568</v>
       </c>
       <c r="B1108" s="45" t="s">
-        <v>7707</v>
+        <v>5814</v>
       </c>
       <c r="C1108" s="45" t="s">
-        <v>7708</v>
+        <v>7507</v>
       </c>
       <c r="D1108" s="34" t="s">
-        <v>7709</v>
+        <v>2281</v>
       </c>
       <c r="E1108" s="23" t="s">
         <v>172</v>
       </c>
       <c r="F1108" s="34" t="s">
-        <v>7710</v>
+        <v>2282</v>
       </c>
       <c r="G1108" s="34" t="s">
-        <v>7711</v>
+        <v>2283</v>
       </c>
       <c r="I1108" s="34" t="s">
-        <v>7712</v>
+        <v>2284</v>
       </c>
       <c r="J1108" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1108" s="34" t="s">
-        <v>7713</v>
+        <v>2285</v>
       </c>
       <c r="L1108" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="M1108" s="25"/>
+      <c r="M1108" s="25" t="s">
+        <v>323</v>
+      </c>
       <c r="N1108" s="24" t="s">
         <v>2754</v>
       </c>
-      <c r="O1108" s="25"/>
+      <c r="O1108" s="25" t="s">
+        <v>323</v>
+      </c>
       <c r="P1108" s="25"/>
       <c r="Q1108" s="48">
-        <v>45602.420393518521</v>
+        <v>45591.506944444445</v>
       </c>
     </row>
     <row r="1109" spans="1:17">
       <c r="A1109" s="3" t="s">
-        <v>7714</v>
+        <v>7717</v>
       </c>
       <c r="B1109" s="45" t="s">
-        <v>7715</v>
+        <v>6985</v>
       </c>
       <c r="C1109" s="45" t="s">
-        <v>7716</v>
+        <v>7234</v>
       </c>
       <c r="D1109" s="34" t="s">
-        <v>7709</v>
+        <v>2876</v>
       </c>
       <c r="E1109" s="23" t="s">
         <v>172</v>
       </c>
       <c r="F1109" s="34" t="s">
-        <v>7710</v>
+        <v>7854</v>
       </c>
       <c r="G1109" s="34" t="s">
-        <v>7711</v>
+        <v>2877</v>
       </c>
       <c r="I1109" s="34" t="s">
-        <v>7712</v>
+        <v>6986</v>
       </c>
       <c r="J1109" s="34" t="s">
         <v>575</v>
       </c>
       <c r="K1109" s="34" t="s">
-        <v>7713</v>
+        <v>2878</v>
       </c>
       <c r="L1109" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="M1109" s="25"/>
+      <c r="M1109" s="25" t="s">
+        <v>323</v>
+      </c>
       <c r="N1109" s="24" t="s">
-        <v>2754</v>
-      </c>
-      <c r="O1109" s="25"/>
-      <c r="P1109" s="25"/>
+        <v>5609</v>
+      </c>
+      <c r="O1109" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="P1109" s="25" t="s">
+        <v>5332</v>
+      </c>
       <c r="Q1109" s="48">
-        <v>45602.422002314815</v>
+        <v>45634.650567129633</v>
       </c>
     </row>
     <row r="1110" spans="1:17">
       <c r="A1110" s="3" t="s">
-        <v>7855</v>
+        <v>7706</v>
       </c>
       <c r="B1110" s="45" t="s">
-        <v>7856</v>
+        <v>7707</v>
       </c>
       <c r="C1110" s="45" t="s">
-        <v>7857</v>
-      </c>
-      <c r="D1110" s="21" t="s">
-        <v>7862</v>
+        <v>7708</v>
+      </c>
+      <c r="D1110" s="34" t="s">
+        <v>7709</v>
       </c>
       <c r="E1110" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="F1110" s="21" t="s">
-        <v>7858</v>
-      </c>
-      <c r="G1110" s="3" t="s">
-        <v>7859</v>
-      </c>
-      <c r="I1110" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="J1110" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="K1110" s="22" t="s">
-        <v>7860</v>
-      </c>
-      <c r="L1110" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="M1110" t="s">
-        <v>256</v>
-      </c>
-      <c r="N1110" s="42" t="s">
-        <v>5788</v>
-      </c>
-      <c r="O1110" t="s">
-        <v>7861</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="F1110" s="34" t="s">
+        <v>7710</v>
+      </c>
+      <c r="G1110" s="34" t="s">
+        <v>7711</v>
+      </c>
+      <c r="I1110" s="34" t="s">
+        <v>7712</v>
+      </c>
+      <c r="J1110" s="34" t="s">
+        <v>575</v>
+      </c>
+      <c r="K1110" s="34" t="s">
+        <v>7713</v>
+      </c>
+      <c r="L1110" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1110" s="25"/>
+      <c r="N1110" s="24" t="s">
+        <v>2754</v>
+      </c>
+      <c r="O1110" s="25"/>
+      <c r="P1110" s="25"/>
       <c r="Q1110" s="48">
-        <v>45637.428865740738</v>
+        <v>45602.420393518521</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:17">
+      <c r="A1111" s="3" t="s">
+        <v>7714</v>
+      </c>
+      <c r="B1111" s="45" t="s">
+        <v>7715</v>
+      </c>
+      <c r="C1111" s="45" t="s">
+        <v>7716</v>
+      </c>
+      <c r="D1111" s="34" t="s">
+        <v>7709</v>
+      </c>
+      <c r="E1111" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1111" s="34" t="s">
+        <v>7710</v>
+      </c>
+      <c r="G1111" s="34" t="s">
+        <v>7711</v>
+      </c>
+      <c r="I1111" s="34" t="s">
+        <v>7712</v>
+      </c>
+      <c r="J1111" s="34" t="s">
+        <v>575</v>
+      </c>
+      <c r="K1111" s="34" t="s">
+        <v>7713</v>
+      </c>
+      <c r="L1111" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1111" s="25"/>
+      <c r="N1111" s="24" t="s">
+        <v>2754</v>
+      </c>
+      <c r="O1111" s="25"/>
+      <c r="P1111" s="25"/>
+      <c r="Q1111" s="48">
+        <v>45602.422002314815</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P1109" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P1106">
-      <sortCondition ref="B2:B1106"/>
-      <sortCondition ref="A2:A1106"/>
+  <autoFilter ref="A1:P1111" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P1108">
+      <sortCondition ref="B2:B1108"/>
+      <sortCondition ref="A2:A1108"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A2:Q1109">
+  <conditionalFormatting sqref="A2:Q1111">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND($A2&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F1106" r:id="rId1" xr:uid="{F456DE86-0DC4-459B-8786-AEB12C0F36B0}"/>
-    <hyperlink ref="F1105" r:id="rId2" xr:uid="{A987B60B-629E-450A-AFE5-A7284329CD96}"/>
-    <hyperlink ref="F1104" r:id="rId3" xr:uid="{BDA96C0A-370D-46F7-82B7-86D5AE155E9F}"/>
-    <hyperlink ref="F1103" r:id="rId4" xr:uid="{E0EF30A2-FEE8-48F7-905E-3DCEE9D90336}"/>
-    <hyperlink ref="F1102" r:id="rId5" xr:uid="{F5EE9F94-288C-4D35-98F2-B7DF314331DE}"/>
-    <hyperlink ref="F1101" r:id="rId6" xr:uid="{A71B48CB-C499-456A-8FFD-47EFE60A828E}"/>
-    <hyperlink ref="F1100" r:id="rId7" xr:uid="{AF04FF5C-ADCA-44DC-B3B2-A425FC0DCFD9}"/>
-    <hyperlink ref="F1099" r:id="rId8" xr:uid="{F55EAFC5-5519-4A1F-80D4-95B4D202FE38}"/>
-    <hyperlink ref="F1098" r:id="rId9" xr:uid="{5FE20200-FB86-452E-8BE1-863A3C65BD07}"/>
-    <hyperlink ref="F1097" r:id="rId10" xr:uid="{8F88B4B6-197E-4940-B572-1769D2C402A3}"/>
-    <hyperlink ref="F1096" r:id="rId11" xr:uid="{DACEA89F-4573-408A-AA3D-AAFC4DF8DB2E}"/>
-    <hyperlink ref="F1095" r:id="rId12" xr:uid="{BF25E2D2-8541-4371-99B7-17A8B86CC8F6}"/>
-    <hyperlink ref="F1094" r:id="rId13" xr:uid="{57CD897B-E530-431D-A4B5-59D9C0F63217}"/>
-    <hyperlink ref="F1093" r:id="rId14" xr:uid="{CEEE77DB-0464-4890-9DA6-629F365AAC93}"/>
-    <hyperlink ref="F1092" r:id="rId15" xr:uid="{D183A8CF-2618-4DDD-8523-A347B0789735}"/>
-    <hyperlink ref="F1091" r:id="rId16" xr:uid="{B44DC245-3939-4FC4-B86F-7F55F80E20F1}"/>
-    <hyperlink ref="F1090" r:id="rId17" xr:uid="{77BEB31C-67F9-4892-974A-C42D173ACEC7}"/>
-    <hyperlink ref="F1089" r:id="rId18" xr:uid="{802015E0-18C1-4D8F-BD48-60606EF00558}"/>
-    <hyperlink ref="F1088" r:id="rId19" xr:uid="{185AA3D8-0081-42DB-B36C-3B1B4DF6AE78}"/>
-    <hyperlink ref="F1087" r:id="rId20" xr:uid="{C92F0FF0-F014-47C6-8A1D-37500F8CB37C}"/>
-    <hyperlink ref="F1086" r:id="rId21" xr:uid="{A79E531F-E421-48DC-B313-0C433AA33C66}"/>
-    <hyperlink ref="F1085" r:id="rId22" xr:uid="{CF6C1299-30F9-427A-9C11-CDEF3096DB13}"/>
-    <hyperlink ref="F1084" r:id="rId23" xr:uid="{B0ED86D2-3643-405A-B6A7-581D3F444E88}"/>
-    <hyperlink ref="F1083" r:id="rId24" xr:uid="{3643C6A3-6F1E-403F-B5BD-A7251D505F5B}"/>
-    <hyperlink ref="F1081" r:id="rId25" xr:uid="{0E92FFCB-F966-4697-91BE-A3130C1CAE25}"/>
+    <hyperlink ref="F1108" r:id="rId1" xr:uid="{F456DE86-0DC4-459B-8786-AEB12C0F36B0}"/>
+    <hyperlink ref="F1107" r:id="rId2" xr:uid="{A987B60B-629E-450A-AFE5-A7284329CD96}"/>
+    <hyperlink ref="F1106" r:id="rId3" xr:uid="{BDA96C0A-370D-46F7-82B7-86D5AE155E9F}"/>
+    <hyperlink ref="F1105" r:id="rId4" xr:uid="{E0EF30A2-FEE8-48F7-905E-3DCEE9D90336}"/>
+    <hyperlink ref="F1104" r:id="rId5" xr:uid="{F5EE9F94-288C-4D35-98F2-B7DF314331DE}"/>
+    <hyperlink ref="F1103" r:id="rId6" xr:uid="{A71B48CB-C499-456A-8FFD-47EFE60A828E}"/>
+    <hyperlink ref="F1102" r:id="rId7" xr:uid="{AF04FF5C-ADCA-44DC-B3B2-A425FC0DCFD9}"/>
+    <hyperlink ref="F1101" r:id="rId8" xr:uid="{F55EAFC5-5519-4A1F-80D4-95B4D202FE38}"/>
+    <hyperlink ref="F1100" r:id="rId9" xr:uid="{5FE20200-FB86-452E-8BE1-863A3C65BD07}"/>
+    <hyperlink ref="F1099" r:id="rId10" xr:uid="{8F88B4B6-197E-4940-B572-1769D2C402A3}"/>
+    <hyperlink ref="F1098" r:id="rId11" xr:uid="{DACEA89F-4573-408A-AA3D-AAFC4DF8DB2E}"/>
+    <hyperlink ref="F1097" r:id="rId12" xr:uid="{BF25E2D2-8541-4371-99B7-17A8B86CC8F6}"/>
+    <hyperlink ref="F1096" r:id="rId13" xr:uid="{57CD897B-E530-431D-A4B5-59D9C0F63217}"/>
+    <hyperlink ref="F1095" r:id="rId14" xr:uid="{CEEE77DB-0464-4890-9DA6-629F365AAC93}"/>
+    <hyperlink ref="F1094" r:id="rId15" xr:uid="{D183A8CF-2618-4DDD-8523-A347B0789735}"/>
+    <hyperlink ref="F1093" r:id="rId16" xr:uid="{B44DC245-3939-4FC4-B86F-7F55F80E20F1}"/>
+    <hyperlink ref="F1092" r:id="rId17" xr:uid="{77BEB31C-67F9-4892-974A-C42D173ACEC7}"/>
+    <hyperlink ref="F1091" r:id="rId18" xr:uid="{802015E0-18C1-4D8F-BD48-60606EF00558}"/>
+    <hyperlink ref="F1090" r:id="rId19" xr:uid="{185AA3D8-0081-42DB-B36C-3B1B4DF6AE78}"/>
+    <hyperlink ref="F1089" r:id="rId20" xr:uid="{C92F0FF0-F014-47C6-8A1D-37500F8CB37C}"/>
+    <hyperlink ref="F1088" r:id="rId21" xr:uid="{A79E531F-E421-48DC-B313-0C433AA33C66}"/>
+    <hyperlink ref="F1087" r:id="rId22" xr:uid="{CF6C1299-30F9-427A-9C11-CDEF3096DB13}"/>
+    <hyperlink ref="F1086" r:id="rId23" xr:uid="{B0ED86D2-3643-405A-B6A7-581D3F444E88}"/>
+    <hyperlink ref="F1085" r:id="rId24" xr:uid="{3643C6A3-6F1E-403F-B5BD-A7251D505F5B}"/>
+    <hyperlink ref="F1083" r:id="rId25" xr:uid="{0E92FFCB-F966-4697-91BE-A3130C1CAE25}"/>
     <hyperlink ref="F373" r:id="rId26" xr:uid="{B4AE46D0-0113-43B5-920F-41BAD7FB12F3}"/>
     <hyperlink ref="F360" r:id="rId27" xr:uid="{6A53CFF1-B4AE-4894-AF74-B4B080E1676D}"/>
     <hyperlink ref="F357" r:id="rId28" xr:uid="{FC91B321-7F3C-4B7C-978D-FF322BE215D6}"/>

</xml_diff>

<commit_message>
2024-12-21 @ 10:41 - v5.H.4.xlsb - 23 760 lignes - Compile OK
* modAppli_Utils.bas
   - Amélioration de la procédure 'CreateOrReplaceWorksheet'
   - Amélioration (performance) de la procédure 'Get_Deplacements_From_TEC'
* modFAC_Finale.bas
   - Changer l'appel à 'NomFeuilleExiste'
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34DDC8A-D4A3-4D9F-B010-C11D369E3460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE74073-7AE1-4E90-B57D-86C1FB95A656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13200" uniqueCount="7870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13212" uniqueCount="7877">
   <si>
     <t>Client_ID</t>
   </si>
@@ -23660,6 +23660,27 @@
   </si>
   <si>
     <t>J4Y 2Z2</t>
+  </si>
+  <si>
+    <t>9331-3104 Québec Inc (Isolation LG4) [Carole Charbonneau]</t>
+  </si>
+  <si>
+    <t>1816</t>
+  </si>
+  <si>
+    <t>Isolation LG4</t>
+  </si>
+  <si>
+    <t>Carole Charbonneau</t>
+  </si>
+  <si>
+    <t>carole@lg4isolation.ca</t>
+  </si>
+  <si>
+    <t>103-1105 rue Armand-Bombardier</t>
+  </si>
+  <si>
+    <t>J6Y 1S9</t>
   </si>
 </sst>
 </file>
@@ -24725,7 +24746,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
   <sheetPr codeName="wshClients"/>
-  <dimension ref="A1:Q1111"/>
+  <dimension ref="A1:Q1112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A381" workbookViewId="0">
       <pane ySplit="615" topLeftCell="A1057" activePane="bottomLeft"/>
@@ -71464,6 +71485,47 @@
       <c r="P1111" s="25"/>
       <c r="Q1111" s="48">
         <v>45602.422002314815</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:17">
+      <c r="A1112" s="3" t="s">
+        <v>7870</v>
+      </c>
+      <c r="B1112" s="45" t="s">
+        <v>7871</v>
+      </c>
+      <c r="C1112" s="45" t="s">
+        <v>7872</v>
+      </c>
+      <c r="D1112" s="21" t="s">
+        <v>7873</v>
+      </c>
+      <c r="F1112" s="21" t="s">
+        <v>7874</v>
+      </c>
+      <c r="G1112" s="3" t="s">
+        <v>7875</v>
+      </c>
+      <c r="I1112" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="J1112" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="K1112" s="22" t="s">
+        <v>7876</v>
+      </c>
+      <c r="L1112" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1112" t="s">
+        <v>3714</v>
+      </c>
+      <c r="O1112" t="s">
+        <v>3714</v>
+      </c>
+      <c r="Q1112" s="48">
+        <v>45646.505231481482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2025-01-09 @ 16:24 - v5.M.xlsb - 24 210 lignes - Compile OK
* Globaux
   - Éliminer les '_' dans les variables (ex: Client_ID ---> CLientID, etc.)
* Problème de casse
   - .listBox ---> .ListBox
* modzDataConversion.bas
   - Au passage, changer la référence aux colonnes en utilisant les énumérations
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC77E07-3B54-4602-B0DC-60A7D51B0FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1284E2-5536-4D44-A95D-E9DB28A19055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="30960" windowHeight="12204" activeTab="1" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13212" uniqueCount="7876">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13214" uniqueCount="7878">
   <si>
     <t>GL_ID</t>
   </si>
@@ -23678,6 +23678,12 @@
   </si>
   <si>
     <t>atheriault@wt.ca</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>1817</t>
   </si>
 </sst>
 </file>
@@ -24743,33 +24749,33 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
   <sheetPr codeName="wshClients"/>
-  <dimension ref="A1:Q1112"/>
+  <dimension ref="A1:Q1113"/>
   <sheetViews>
     <sheetView topLeftCell="I381" workbookViewId="0">
-      <pane ySplit="612" activePane="bottomLeft"/>
+      <pane ySplit="615" activePane="bottomLeft"/>
       <selection activeCell="Q1" sqref="Q1:Q1048576"/>
       <selection pane="bottomLeft" activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" style="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.5546875" style="45" customWidth="1"/>
-    <col min="4" max="4" width="33.109375" style="21" customWidth="1"/>
-    <col min="5" max="5" width="33.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.88671875" style="21" customWidth="1"/>
+    <col min="1" max="1" width="55.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" style="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" style="45" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.85546875" style="21" customWidth="1"/>
     <col min="7" max="7" width="32" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" style="22" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="42.44140625" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" style="42" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="35.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.6640625" style="48" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" style="48" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -71520,6 +71526,17 @@
       </c>
       <c r="Q1112" s="48">
         <v>45646.505231481482</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:17">
+      <c r="A1113" s="3" t="s">
+        <v>7876</v>
+      </c>
+      <c r="B1113" s="45" t="s">
+        <v>7877</v>
+      </c>
+      <c r="Q1113" s="48">
+        <v>45666.669074074074</v>
       </c>
     </row>
   </sheetData>
@@ -71821,26 +71838,26 @@
   <dimension ref="A1:O63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="612" activePane="bottomLeft"/>
+      <pane ySplit="615" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1048576"/>
       <selection pane="bottomLeft" activeCell="K1" sqref="K1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.44140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="11.5546875" style="1"/>
+    <col min="11" max="11" width="17.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -73712,18 +73729,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.6640625" style="2" customWidth="1"/>
-    <col min="10" max="13" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="33.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" style="2" customWidth="1"/>
+    <col min="10" max="13" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -74659,7 +74676,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" thickBot="1">
+    <row r="67" spans="1:4" ht="15.75" thickBot="1">
       <c r="A67" s="12" t="s">
         <v>127</v>
       </c>

</xml_diff>

<commit_message>
2025-01-10 @ 20:45 - v5.M.1.xlsb - 24 279 lignes - Compile OK
* Problème de casse
   - .GoTO ---> .Goto
   - LastRow ---> lastRow
   - .ListBox ---> .listBox
   - .update ---> .Update
   - Sheetname ---> sheetname
* modAppli_Utils.bas
   - Enlever les formules pour la colonne Balance dans FAC_Comptes_Clients
* modCC_Régularisation.bas
   - Mise au point du programme de Régularisations
   - Gros (long) problème avec la requête SQL qui refuse de mettre à jour un champ qui contient une formule
* modDev_Utils.bas
   - Transfert des log dans un fichier cumulatif de log pour fins d'analyse
* modENC_Saisie.bas
   - Ajouter les régularisations plutôt que de les soustraire...
* modFunctions.bas
   - Nouvelle fonction pour extraire les secondes des entrées du log
* modLog_Analysis.bas
   - Mise au point du programme pour importer les entrées du log
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1284E2-5536-4D44-A95D-E9DB28A19055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347EA8B1-2DC5-48D0-B0FC-7BE6915723AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="38280" yWindow="-105" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13214" uniqueCount="7878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13230" uniqueCount="7888">
   <si>
     <t>GL_ID</t>
   </si>
@@ -23680,10 +23680,40 @@
     <t>atheriault@wt.ca</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>Zaraté + Lavigne Architectes Inc. [Maxime Brosseau]</t>
   </si>
   <si>
     <t>1817</t>
+  </si>
+  <si>
+    <t>Zaraté Lavigne</t>
+  </si>
+  <si>
+    <t>Maxime Brosseau</t>
+  </si>
+  <si>
+    <t>m.brosseau@zaratelavigne.com</t>
+  </si>
+  <si>
+    <t>370 rue Sauvé O</t>
+  </si>
+  <si>
+    <t>H3L 1Z8</t>
+  </si>
+  <si>
+    <t>Sacha Matteau</t>
+  </si>
+  <si>
+    <t>Services Juridiques, François-Pierre Laforest Inc.</t>
+  </si>
+  <si>
+    <t>6728 rue Fabre</t>
+  </si>
+  <si>
+    <t>H2G 2Z6</t>
+  </si>
+  <si>
+    <t>Juriglobal Inc.</t>
   </si>
 </sst>
 </file>
@@ -69770,7 +69800,7 @@
     </row>
     <row r="1076" spans="1:17">
       <c r="A1076" s="3" t="s">
-        <v>7012</v>
+        <v>7884</v>
       </c>
       <c r="B1076" s="45" t="s">
         <v>7013</v>
@@ -69787,11 +69817,21 @@
       <c r="F1076" s="34" t="s">
         <v>7014</v>
       </c>
-      <c r="G1076" s="34"/>
-      <c r="I1076" s="34"/>
-      <c r="J1076" s="34"/>
-      <c r="K1076" s="34"/>
-      <c r="L1076" s="34"/>
+      <c r="G1076" s="34" t="s">
+        <v>7885</v>
+      </c>
+      <c r="I1076" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="J1076" s="34" t="s">
+        <v>566</v>
+      </c>
+      <c r="K1076" s="34" t="s">
+        <v>7886</v>
+      </c>
+      <c r="L1076" s="34" t="s">
+        <v>153</v>
+      </c>
       <c r="M1076" s="25" t="s">
         <v>3658</v>
       </c>
@@ -69799,9 +69839,11 @@
         <v>2741</v>
       </c>
       <c r="O1076" s="25"/>
-      <c r="P1076" s="25"/>
+      <c r="P1076" s="25" t="s">
+        <v>7887</v>
+      </c>
       <c r="Q1076" s="48">
-        <v>45591.506944444445</v>
+        <v>45667.442488425928</v>
       </c>
     </row>
     <row r="1077" spans="1:17">
@@ -71535,8 +71577,38 @@
       <c r="B1113" s="45" t="s">
         <v>7877</v>
       </c>
+      <c r="C1113" s="45" t="s">
+        <v>7878</v>
+      </c>
+      <c r="D1113" s="21" t="s">
+        <v>7879</v>
+      </c>
+      <c r="E1113" s="23" t="s">
+        <v>2776</v>
+      </c>
+      <c r="F1113" s="21" t="s">
+        <v>7880</v>
+      </c>
+      <c r="G1113" s="3" t="s">
+        <v>7881</v>
+      </c>
+      <c r="I1113" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="J1113" s="22" t="s">
+        <v>566</v>
+      </c>
+      <c r="K1113" s="22" t="s">
+        <v>7882</v>
+      </c>
+      <c r="L1113" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1113" t="s">
+        <v>7883</v>
+      </c>
       <c r="Q1113" s="48">
-        <v>45666.669074074074</v>
+        <v>45666.704988425925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2025-02-13 @ 11:06 - v5.P.4.xlsb - 28 094 lignes - Compile OK
* modAppli_Utils.bas
- Dans Vérification d'intégrité - Forcer le format yyyy-mm-dd hh:mm:ss sur l'affichage des tables
- Ajouter une validation additionnelle pour éviter que la date ne soit supérieure à la date du jour (problème inversement jour & mois)
- Éliminer du code mort (Get_Deplacements_From_TEC_OK)
- Corriger un bug avec le calcul de la durée depuis la date dernière modification du fichier GCF_MASTER.xlsx
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18412ED4-6B70-4976-A43A-62314556A9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A5DFE4-45D7-4652-8FF0-06F49C73B77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="38280" yWindow="-16305" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14435" uniqueCount="8254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14462" uniqueCount="8265">
   <si>
     <t>GL_ID</t>
   </si>
@@ -24812,6 +24812,39 @@
   </si>
   <si>
     <t>9245-7589 Québec Inc. [Dominique Laurin] Resto Spag</t>
+  </si>
+  <si>
+    <t>Les entreprises électriques Michel Guertin Inc. [Nathalie Audet]</t>
+  </si>
+  <si>
+    <t>1820</t>
+  </si>
+  <si>
+    <t>Les entreprises électriques Michel Guertin Inc.</t>
+  </si>
+  <si>
+    <t>Nathalie Audet</t>
+  </si>
+  <si>
+    <t>5812 rue Hadley</t>
+  </si>
+  <si>
+    <t>H4E 3N6</t>
+  </si>
+  <si>
+    <t>Gestion Immobilière Vincla Inc. [Patrick Forget]</t>
+  </si>
+  <si>
+    <t>1821</t>
+  </si>
+  <si>
+    <t>Patrick Forget</t>
+  </si>
+  <si>
+    <t>patforget@live.ca</t>
+  </si>
+  <si>
+    <t>163 rue Louis-Cyr</t>
   </si>
 </sst>
 </file>
@@ -25889,7 +25922,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
   <sheetPr codeName="wshClients"/>
-  <dimension ref="A1:R1120"/>
+  <dimension ref="A1:R1122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A1074" activePane="bottomLeft" state="frozen"/>
@@ -76378,6 +76411,97 @@
       </c>
       <c r="R1120" s="48">
         <v>45686.720590277779</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:18">
+      <c r="A1121" s="3" t="s">
+        <v>8254</v>
+      </c>
+      <c r="B1121" s="52" t="s">
+        <v>8255</v>
+      </c>
+      <c r="C1121" s="45" t="s">
+        <v>8256</v>
+      </c>
+      <c r="D1121" s="21" t="s">
+        <v>8257</v>
+      </c>
+      <c r="G1121" s="3" t="s">
+        <v>8258</v>
+      </c>
+      <c r="I1121" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="J1121" s="22" t="s">
+        <v>566</v>
+      </c>
+      <c r="K1121" s="22" t="s">
+        <v>8259</v>
+      </c>
+      <c r="L1121" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1121" t="s">
+        <v>704</v>
+      </c>
+      <c r="P1121" t="s">
+        <v>704</v>
+      </c>
+      <c r="Q1121" t="s">
+        <v>8254</v>
+      </c>
+      <c r="R1121" s="48">
+        <v>45700.382939814815</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:18">
+      <c r="A1122" s="3" t="s">
+        <v>8260</v>
+      </c>
+      <c r="B1122" s="52" t="s">
+        <v>8261</v>
+      </c>
+      <c r="C1122" s="45" t="s">
+        <v>8262</v>
+      </c>
+      <c r="D1122" s="21" t="s">
+        <v>8262</v>
+      </c>
+      <c r="E1122" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1122" s="21" t="s">
+        <v>8263</v>
+      </c>
+      <c r="G1122" s="3" t="s">
+        <v>8264</v>
+      </c>
+      <c r="I1122" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J1122" s="22" t="s">
+        <v>566</v>
+      </c>
+      <c r="K1122" s="22" t="s">
+        <v>3424</v>
+      </c>
+      <c r="L1122" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1122" t="s">
+        <v>620</v>
+      </c>
+      <c r="N1122" s="42" t="s">
+        <v>5752</v>
+      </c>
+      <c r="O1122" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q1122" t="s">
+        <v>8260</v>
+      </c>
+      <c r="R1122" s="48">
+        <v>45700.485648148147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2025-02-19 @ 12:20 - v6.A.1.xlsb - 28 221 lignes - Compile OK
* modAppli.bas
- Ajouter la version de l'application dans le fichier d'activité par utilisateur
- Ajouter l'utilisateur 'gchar' à la liste des utilisateurs
* modMenu.bas
- Ajouter l'utilisateur 'gchar' à la liste des utilisateurs
* ufSaisieHeures.frm
- Ajouter l'utilisateur 'gchar' à la liste des utilisateurs
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A5DFE4-45D7-4652-8FF0-06F49C73B77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7672A9F2-A57E-4BFD-AF78-489ECC1872CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-16305" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="11385" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14462" uniqueCount="8265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14469" uniqueCount="8271">
   <si>
     <t>GL_ID</t>
   </si>
@@ -24845,6 +24845,24 @@
   </si>
   <si>
     <t>163 rue Louis-Cyr</t>
+  </si>
+  <si>
+    <t>Kin Foundry Team [Shanice]</t>
+  </si>
+  <si>
+    <t>2059</t>
+  </si>
+  <si>
+    <t>Shanice</t>
+  </si>
+  <si>
+    <t>comptable</t>
+  </si>
+  <si>
+    <t>hello@kinfoundry.ca</t>
+  </si>
+  <si>
+    <t>Vladimir Gervaus</t>
   </si>
 </sst>
 </file>
@@ -25922,7 +25940,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
   <sheetPr codeName="wshClients"/>
-  <dimension ref="A1:R1122"/>
+  <dimension ref="A1:R1123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A1074" activePane="bottomLeft" state="frozen"/>
@@ -76502,6 +76520,32 @@
       </c>
       <c r="R1122" s="48">
         <v>45700.485648148147</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:18">
+      <c r="A1123" s="3" t="s">
+        <v>8265</v>
+      </c>
+      <c r="B1123" s="52" t="s">
+        <v>8266</v>
+      </c>
+      <c r="D1123" s="21" t="s">
+        <v>8267</v>
+      </c>
+      <c r="E1123" s="23" t="s">
+        <v>8268</v>
+      </c>
+      <c r="F1123" s="21" t="s">
+        <v>8269</v>
+      </c>
+      <c r="M1123" t="s">
+        <v>8270</v>
+      </c>
+      <c r="Q1123" t="s">
+        <v>8265</v>
+      </c>
+      <c r="R1123" s="48">
+        <v>45704.650717592594</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2025-05-02 @ 14:22 - v6.C.4.xlsb - 29 524 lignes - Compile OK
* modFAC_Brouillon.bas
- .listBox ---> .ListBox
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FF2FB5-FB07-4D04-9212-4E3B4D307A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F65896-EE64-49C5-BA1E-FC86F30503A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14590" uniqueCount="8334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14593" uniqueCount="8336">
   <si>
     <t>GL_ID</t>
   </si>
@@ -25044,6 +25044,12 @@
   </si>
   <si>
     <t>547</t>
+  </si>
+  <si>
+    <t>TEST 2</t>
+  </si>
+  <si>
+    <t>549</t>
   </si>
 </sst>
 </file>
@@ -25765,7 +25771,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
   <sheetPr codeName="wshClients"/>
-  <dimension ref="A1:R1135"/>
+  <dimension ref="A1:R1136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A369" activePane="bottomLeft" state="frozen"/>
@@ -76856,6 +76862,20 @@
       </c>
       <c r="R1135" s="52">
         <v>45779.588923611103</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:18">
+      <c r="A1136" s="34" t="s">
+        <v>8334</v>
+      </c>
+      <c r="B1136" s="34" t="s">
+        <v>8335</v>
+      </c>
+      <c r="Q1136" s="34" t="s">
+        <v>8334</v>
+      </c>
+      <c r="R1136" s="52">
+        <v>45779.595486111102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2025-05-09 @ 22:55 - v6.C.6.xlsb
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5287F1B4-1154-4057-9E6F-6C018F43F995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC4C920-4515-496F-BD67-983AE0DA90C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14716" uniqueCount="8395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14770" uniqueCount="8426">
   <si>
     <t>GL_ID</t>
   </si>
@@ -25227,6 +25227,99 @@
   </si>
   <si>
     <t>K1M 1X6</t>
+  </si>
+  <si>
+    <t>Evan Trickey [Véronique Poulin]</t>
+  </si>
+  <si>
+    <t>553</t>
+  </si>
+  <si>
+    <t>Les Fondations Jono Inc.</t>
+  </si>
+  <si>
+    <t>Véronique Poulin</t>
+  </si>
+  <si>
+    <t>veronique.poulin.1@hotmail.com</t>
+  </si>
+  <si>
+    <t>846 rue Marc-Aurèle Fortin</t>
+  </si>
+  <si>
+    <t>Saint-Lin-Leurentides</t>
+  </si>
+  <si>
+    <t>J5M 2S7</t>
+  </si>
+  <si>
+    <t>Evan Trickey [Véronique Poulin] Les Fondations Jono Inc.</t>
+  </si>
+  <si>
+    <t>Solution Maxpark Inc. [Gary Bastien]</t>
+  </si>
+  <si>
+    <t>Solution Maxpark Inc.</t>
+  </si>
+  <si>
+    <t>Gary Bastien</t>
+  </si>
+  <si>
+    <t>fourparkinc@gmail.com</t>
+  </si>
+  <si>
+    <t>306-1555 boul de l'Avenir</t>
+  </si>
+  <si>
+    <t>Succession François Ricard [marcelle.cossette-ricard@umontreal.ca]</t>
+  </si>
+  <si>
+    <t>Succession François Ricard</t>
+  </si>
+  <si>
+    <t>marcelle.cossette-ricard@umontreal.ca</t>
+  </si>
+  <si>
+    <t>451 Avenue Stuart</t>
+  </si>
+  <si>
+    <t>H2V 3N1</t>
+  </si>
+  <si>
+    <t>Linda Morrissette</t>
+  </si>
+  <si>
+    <t>554</t>
+  </si>
+  <si>
+    <t>lindamorisset@videotron.ca</t>
+  </si>
+  <si>
+    <t>3492 Boul Lévesque Est</t>
+  </si>
+  <si>
+    <t>H7E 2P8</t>
+  </si>
+  <si>
+    <t>9429-0756 Québec Inc. [Émerson Lopez]</t>
+  </si>
+  <si>
+    <t>9429-0756 Québec Inc.</t>
+  </si>
+  <si>
+    <t>Émerson Lopez</t>
+  </si>
+  <si>
+    <t>emersonlopezc@gmail.com</t>
+  </si>
+  <si>
+    <t>Sylin Paul, CPA</t>
+  </si>
+  <si>
+    <t>703-10550 Place de l'Acadie</t>
+  </si>
+  <si>
+    <t>H4N 0B3</t>
   </si>
 </sst>
 </file>
@@ -25462,7 +25555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -25588,19 +25681,15 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -25935,12 +26024,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
   <sheetPr codeName="wshClients"/>
-  <dimension ref="A1:R1144"/>
+  <dimension ref="A1:R1149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A1120" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A1110" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="C1134" sqref="C1134"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD1142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -77232,98 +77321,281 @@
       </c>
     </row>
     <row r="1143" spans="1:18">
-      <c r="A1143" s="3" t="s">
+      <c r="A1143" s="31" t="s">
         <v>8383</v>
       </c>
-      <c r="B1143" s="46" t="s">
+      <c r="B1143" s="31" t="s">
         <v>8384</v>
       </c>
-      <c r="C1143" s="41" t="s">
+      <c r="C1143" s="31" t="s">
         <v>8385</v>
       </c>
-      <c r="D1143" s="21" t="s">
+      <c r="D1143" s="31" t="s">
         <v>8386</v>
       </c>
-      <c r="E1143" s="23" t="s">
+      <c r="E1143" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="F1143" s="21" t="s">
+      <c r="F1143" s="31" t="s">
         <v>8387</v>
       </c>
-      <c r="G1143" s="3" t="s">
+      <c r="G1143" s="31" t="s">
         <v>8388</v>
       </c>
-      <c r="I1143" s="3" t="s">
+      <c r="I1143" s="31" t="s">
         <v>272</v>
       </c>
-      <c r="J1143" s="22" t="s">
-        <v>563</v>
-      </c>
-      <c r="K1143" s="22" t="s">
+      <c r="J1143" s="31" t="s">
+        <v>563</v>
+      </c>
+      <c r="K1143" s="31" t="s">
         <v>8389</v>
       </c>
-      <c r="L1143" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="M1143" s="25" t="s">
+      <c r="L1143" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1143" s="31" t="s">
         <v>270</v>
       </c>
-      <c r="N1143" s="24" t="s">
+      <c r="N1143" s="31" t="s">
         <v>5737</v>
       </c>
-      <c r="O1143" s="25" t="s">
+      <c r="O1143" s="31" t="s">
         <v>270</v>
       </c>
-      <c r="P1143" s="25"/>
-      <c r="Q1143" s="25" t="s">
+      <c r="Q1143" s="31" t="s">
         <v>8383</v>
       </c>
-      <c r="R1143" s="43">
+      <c r="R1143" s="47">
         <v>45782.397962962998</v>
       </c>
     </row>
     <row r="1144" spans="1:18">
-      <c r="A1144" s="3" t="s">
+      <c r="A1144" s="31" t="s">
         <v>8390</v>
       </c>
-      <c r="B1144" s="46" t="s">
+      <c r="B1144" s="31" t="s">
         <v>8391</v>
       </c>
-      <c r="C1144" s="41" t="s">
+      <c r="C1144" s="31" t="s">
         <v>8390</v>
       </c>
-      <c r="D1144" s="21" t="s">
+      <c r="D1144" s="31" t="s">
         <v>8390</v>
       </c>
-      <c r="F1144" s="21" t="s">
+      <c r="F1144" s="31" t="s">
         <v>8392</v>
       </c>
-      <c r="G1144" s="3" t="s">
+      <c r="G1144" s="31" t="s">
         <v>8393</v>
       </c>
-      <c r="I1144" s="3" t="s">
+      <c r="I1144" s="31" t="s">
         <v>1690</v>
       </c>
-      <c r="J1144" s="22" t="s">
-        <v>563</v>
-      </c>
-      <c r="K1144" s="22" t="s">
+      <c r="J1144" s="31" t="s">
+        <v>563</v>
+      </c>
+      <c r="K1144" s="31" t="s">
         <v>8394</v>
       </c>
-      <c r="L1144" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="M1144" s="25"/>
-      <c r="N1144" s="24" t="s">
+      <c r="L1144" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="N1144" s="31" t="s">
         <v>2734</v>
       </c>
-      <c r="O1144" s="25"/>
-      <c r="P1144" s="25"/>
-      <c r="Q1144" s="25" t="s">
+      <c r="Q1144" s="31" t="s">
         <v>8390</v>
       </c>
-      <c r="R1144" s="43">
+      <c r="R1144" s="47">
         <v>45784.2397569444</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:18">
+      <c r="A1145" s="31" t="s">
+        <v>8395</v>
+      </c>
+      <c r="B1145" s="31" t="s">
+        <v>8396</v>
+      </c>
+      <c r="C1145" s="31" t="s">
+        <v>8397</v>
+      </c>
+      <c r="D1145" s="31" t="s">
+        <v>8398</v>
+      </c>
+      <c r="F1145" s="31" t="s">
+        <v>8399</v>
+      </c>
+      <c r="G1145" s="31" t="s">
+        <v>8400</v>
+      </c>
+      <c r="I1145" s="31" t="s">
+        <v>8401</v>
+      </c>
+      <c r="J1145" s="31" t="s">
+        <v>2354</v>
+      </c>
+      <c r="K1145" s="31" t="s">
+        <v>8402</v>
+      </c>
+      <c r="L1145" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="O1145" s="31" t="s">
+        <v>802</v>
+      </c>
+      <c r="Q1145" s="31" t="s">
+        <v>8403</v>
+      </c>
+      <c r="R1145" s="47">
+        <v>45784.685474537</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:18">
+      <c r="A1146" s="31" t="s">
+        <v>8404</v>
+      </c>
+      <c r="B1146" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1146" s="31" t="s">
+        <v>8405</v>
+      </c>
+      <c r="D1146" s="31" t="s">
+        <v>8406</v>
+      </c>
+      <c r="F1146" s="31" t="s">
+        <v>8407</v>
+      </c>
+      <c r="G1146" s="31" t="s">
+        <v>8408</v>
+      </c>
+      <c r="I1146" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="J1146" s="31" t="s">
+        <v>563</v>
+      </c>
+      <c r="K1146" s="31" t="s">
+        <v>4017</v>
+      </c>
+      <c r="Q1146" s="31" t="s">
+        <v>8404</v>
+      </c>
+      <c r="R1146" s="47">
+        <v>45784.950891203698</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:18">
+      <c r="A1147" s="31" t="s">
+        <v>8409</v>
+      </c>
+      <c r="B1147" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1147" s="31" t="s">
+        <v>8410</v>
+      </c>
+      <c r="D1147" s="31" t="s">
+        <v>8411</v>
+      </c>
+      <c r="F1147" s="31" t="s">
+        <v>8411</v>
+      </c>
+      <c r="G1147" s="31" t="s">
+        <v>8412</v>
+      </c>
+      <c r="I1147" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="J1147" s="31" t="s">
+        <v>563</v>
+      </c>
+      <c r="K1147" s="31" t="s">
+        <v>8413</v>
+      </c>
+      <c r="Q1147" s="31" t="s">
+        <v>8409</v>
+      </c>
+      <c r="R1147" s="47">
+        <v>45784.950520833299</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:18">
+      <c r="A1148" s="31" t="s">
+        <v>8414</v>
+      </c>
+      <c r="B1148" s="31" t="s">
+        <v>8415</v>
+      </c>
+      <c r="C1148" s="31" t="s">
+        <v>8414</v>
+      </c>
+      <c r="D1148" s="31" t="s">
+        <v>8414</v>
+      </c>
+      <c r="F1148" s="31" t="s">
+        <v>8416</v>
+      </c>
+      <c r="G1148" s="31" t="s">
+        <v>8417</v>
+      </c>
+      <c r="I1148" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="J1148" s="31" t="s">
+        <v>563</v>
+      </c>
+      <c r="K1148" s="31" t="s">
+        <v>8418</v>
+      </c>
+      <c r="L1148" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q1148" s="31" t="s">
+        <v>8414</v>
+      </c>
+      <c r="R1148" s="47">
+        <v>45785.484560185199</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:18">
+      <c r="A1149" s="31" t="s">
+        <v>8419</v>
+      </c>
+      <c r="B1149" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1149" s="31" t="s">
+        <v>8420</v>
+      </c>
+      <c r="D1149" s="31" t="s">
+        <v>8421</v>
+      </c>
+      <c r="F1149" s="31" t="s">
+        <v>8422</v>
+      </c>
+      <c r="G1149" s="31" t="s">
+        <v>8424</v>
+      </c>
+      <c r="I1149" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="J1149" s="31" t="s">
+        <v>563</v>
+      </c>
+      <c r="K1149" s="31" t="s">
+        <v>8425</v>
+      </c>
+      <c r="M1149" s="31" t="s">
+        <v>8423</v>
+      </c>
+      <c r="Q1149" s="31" t="s">
+        <v>8419</v>
+      </c>
+      <c r="R1149" s="47">
+        <v>45785.929756944402</v>
       </c>
     </row>
   </sheetData>
@@ -77332,13 +77604,8 @@
     <sortCondition ref="B1136"/>
   </sortState>
   <conditionalFormatting sqref="A2:R1142">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>AND($A2&lt;&gt;"",MOD(ROW(),2)=0)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1143:R1144">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND($A1143&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -79478,7 +79745,7 @@
     <sortCondition ref="A1:A20"/>
   </sortState>
   <conditionalFormatting sqref="A2:L9999">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>AND($A2&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -86350,7 +86617,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:D67">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
2025-05-28 @ 17:48 - Without code
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26180405-93BA-4924-9F6A-C9593C0826F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FEE0F3-A4FC-4650-AA21-7223D3610712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -25630,7 +25630,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -25756,15 +25756,19 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -26104,7 +26108,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A1121" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD1151"/>
+      <selection pane="bottomLeft" activeCell="A1153" sqref="A1153:XFD1153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -74378,37 +74382,41 @@
       </c>
     </row>
     <row r="1153" spans="1:18">
-      <c r="A1153" s="31" t="s">
+      <c r="A1153" s="3" t="s">
         <v>8446</v>
       </c>
-      <c r="B1153" s="31" t="s">
+      <c r="B1153" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="C1153" s="31" t="s">
+      <c r="C1153" s="41" t="s">
         <v>8447</v>
       </c>
-      <c r="E1153" s="31" t="s">
+      <c r="E1153" s="23" t="s">
         <v>6080</v>
       </c>
-      <c r="F1153" s="31" t="s">
+      <c r="F1153" s="21" t="s">
         <v>8448</v>
       </c>
-      <c r="G1153" s="31" t="s">
+      <c r="G1153" s="3" t="s">
         <v>8449</v>
       </c>
-      <c r="I1153" s="31" t="s">
+      <c r="I1153" s="3" t="s">
         <v>8266</v>
       </c>
-      <c r="J1153" s="31" t="s">
+      <c r="J1153" s="22" t="s">
         <v>8267</v>
       </c>
-      <c r="K1153" s="31" t="s">
+      <c r="K1153" s="22" t="s">
         <v>8450</v>
       </c>
-      <c r="Q1153" s="31" t="s">
+      <c r="M1153" s="25"/>
+      <c r="N1153" s="24"/>
+      <c r="O1153" s="25"/>
+      <c r="P1153" s="25"/>
+      <c r="Q1153" s="25" t="s">
         <v>8446</v>
       </c>
-      <c r="R1153" s="47">
+      <c r="R1153" s="43">
         <v>45798.954733796301</v>
       </c>
     </row>
@@ -74418,8 +74426,13 @@
     <sortCondition ref="B1150:B1152"/>
   </sortState>
   <conditionalFormatting sqref="A2:R1152">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>AND($A2&lt;&gt;"",MOD(ROW(),2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1153:R1153">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND($A1153&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -76559,7 +76572,7 @@
     <sortCondition ref="A1:A20"/>
   </sortState>
   <conditionalFormatting sqref="A2:L9999">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND($A2&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -83431,7 +83444,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:D67">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
2025-05-31 @ 18:05 - v6.C.9.xlsb - Pas de code
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71B4FC9-90A2-4273-949A-B82EFA8F4A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A255B1B-0565-4A76-8E06-E21061BB85EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="2640" windowWidth="28800" windowHeight="11385" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="PlanComptable" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Clients!$A$1:$R$1147</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Clients!$A$1:$R$1148</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Fournisseurs!$A$1:$K$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -25669,7 +25669,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -25795,15 +25795,19 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -26141,9 +26145,9 @@
   <dimension ref="A1:R1155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A1141" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A1101" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A1154" sqref="A1154:XFD1154"/>
+      <selection pane="bottomLeft" activeCell="A1111" sqref="A1111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -72469,75 +72473,69 @@
     </row>
     <row r="1110" spans="1:18">
       <c r="A1110" s="3" t="s">
-        <v>6488</v>
+        <v>8457</v>
       </c>
       <c r="B1110" s="46" t="s">
-        <v>45</v>
+        <v>8458</v>
       </c>
       <c r="C1110" s="41" t="s">
-        <v>7450</v>
+        <v>7424</v>
       </c>
       <c r="D1110" s="21" t="s">
-        <v>2243</v>
+        <v>8459</v>
       </c>
       <c r="E1110" s="23" t="s">
         <v>166</v>
       </c>
       <c r="F1110" s="21" t="s">
-        <v>2244</v>
+        <v>8460</v>
       </c>
       <c r="G1110" s="3" t="s">
-        <v>2245</v>
+        <v>8461</v>
       </c>
       <c r="I1110" s="3" t="s">
-        <v>2224</v>
+        <v>245</v>
       </c>
       <c r="J1110" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1110" s="22" t="s">
-        <v>2246</v>
+        <v>8462</v>
       </c>
       <c r="L1110" s="22" t="s">
         <v>153</v>
       </c>
       <c r="M1110" t="s">
-        <v>313</v>
-      </c>
-      <c r="N1110" s="38" t="s">
-        <v>5737</v>
-      </c>
-      <c r="O1110" t="s">
-        <v>313</v>
-      </c>
-      <c r="P1110" t="s">
-        <v>5282</v>
+        <v>3420</v>
       </c>
       <c r="Q1110" t="s">
-        <v>8064</v>
+        <v>8463</v>
       </c>
       <c r="R1110" s="43">
-        <v>45591.506944444402</v>
+        <v>45805.666157407402</v>
       </c>
     </row>
     <row r="1111" spans="1:18">
       <c r="A1111" s="3" t="s">
-        <v>6901</v>
+        <v>6488</v>
       </c>
       <c r="B1111" s="46" t="s">
-        <v>5738</v>
+        <v>45</v>
       </c>
       <c r="C1111" s="41" t="s">
-        <v>7440</v>
+        <v>7450</v>
       </c>
       <c r="D1111" s="21" t="s">
-        <v>6904</v>
+        <v>2243</v>
       </c>
       <c r="E1111" s="23" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="F1111" s="21" t="s">
+        <v>2244</v>
       </c>
       <c r="G1111" s="3" t="s">
-        <v>2247</v>
+        <v>2245</v>
       </c>
       <c r="I1111" s="3" t="s">
         <v>2224</v>
@@ -72546,7 +72544,7 @@
         <v>563</v>
       </c>
       <c r="K1111" s="22" t="s">
-        <v>2248</v>
+        <v>2246</v>
       </c>
       <c r="L1111" s="22" t="s">
         <v>153</v>
@@ -72555,48 +72553,48 @@
         <v>313</v>
       </c>
       <c r="N1111" s="38" t="s">
-        <v>2734</v>
+        <v>5737</v>
       </c>
       <c r="O1111" t="s">
         <v>313</v>
       </c>
+      <c r="P1111" t="s">
+        <v>5282</v>
+      </c>
       <c r="Q1111" t="s">
-        <v>8065</v>
+        <v>8064</v>
       </c>
       <c r="R1111" s="43">
-        <v>45592.251759259299</v>
+        <v>45591.506944444402</v>
       </c>
     </row>
     <row r="1112" spans="1:18">
       <c r="A1112" s="3" t="s">
-        <v>6898</v>
+        <v>6901</v>
       </c>
       <c r="B1112" s="46" t="s">
-        <v>5739</v>
+        <v>5738</v>
       </c>
       <c r="C1112" s="41" t="s">
-        <v>7416</v>
+        <v>7440</v>
       </c>
       <c r="D1112" s="21" t="s">
-        <v>6905</v>
+        <v>6904</v>
       </c>
       <c r="E1112" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="F1112" s="21" t="s">
-        <v>2249</v>
+        <v>165</v>
       </c>
       <c r="G1112" s="3" t="s">
-        <v>2250</v>
+        <v>2247</v>
       </c>
       <c r="I1112" s="3" t="s">
-        <v>245</v>
+        <v>2224</v>
       </c>
       <c r="J1112" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1112" s="22" t="s">
-        <v>2251</v>
+        <v>2248</v>
       </c>
       <c r="L1112" s="22" t="s">
         <v>153</v>
@@ -72605,48 +72603,48 @@
         <v>313</v>
       </c>
       <c r="N1112" s="38" t="s">
-        <v>5558</v>
+        <v>2734</v>
       </c>
       <c r="O1112" t="s">
         <v>313</v>
       </c>
       <c r="Q1112" t="s">
-        <v>8066</v>
+        <v>8065</v>
       </c>
       <c r="R1112" s="43">
-        <v>45591.506944444402</v>
+        <v>45592.251759259299</v>
       </c>
     </row>
     <row r="1113" spans="1:18">
       <c r="A1113" s="3" t="s">
-        <v>6902</v>
+        <v>6898</v>
       </c>
       <c r="B1113" s="46" t="s">
-        <v>5740</v>
+        <v>5739</v>
       </c>
       <c r="C1113" s="41" t="s">
-        <v>7448</v>
+        <v>7416</v>
       </c>
       <c r="D1113" s="21" t="s">
-        <v>6906</v>
+        <v>6905</v>
       </c>
       <c r="E1113" s="23" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F1113" s="21" t="s">
-        <v>1561</v>
+        <v>2249</v>
       </c>
       <c r="G1113" s="3" t="s">
-        <v>2252</v>
+        <v>2250</v>
       </c>
       <c r="I1113" s="3" t="s">
-        <v>154</v>
+        <v>245</v>
       </c>
       <c r="J1113" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1113" s="22" t="s">
-        <v>1563</v>
+        <v>2251</v>
       </c>
       <c r="L1113" s="22" t="s">
         <v>153</v>
@@ -72655,16 +72653,13 @@
         <v>313</v>
       </c>
       <c r="N1113" s="38" t="s">
-        <v>2734</v>
+        <v>5558</v>
       </c>
       <c r="O1113" t="s">
         <v>313</v>
       </c>
-      <c r="P1113" t="s">
-        <v>5282</v>
-      </c>
       <c r="Q1113" t="s">
-        <v>8067</v>
+        <v>8066</v>
       </c>
       <c r="R1113" s="43">
         <v>45591.506944444402</v>
@@ -72672,34 +72667,34 @@
     </row>
     <row r="1114" spans="1:18">
       <c r="A1114" s="3" t="s">
-        <v>6489</v>
+        <v>6902</v>
       </c>
       <c r="B1114" s="46" t="s">
-        <v>5741</v>
+        <v>5740</v>
       </c>
       <c r="C1114" s="41" t="s">
-        <v>7431</v>
+        <v>7448</v>
       </c>
       <c r="D1114" s="21" t="s">
-        <v>2253</v>
+        <v>6906</v>
       </c>
       <c r="E1114" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F1114" s="21" t="s">
-        <v>2254</v>
+        <v>1561</v>
       </c>
       <c r="G1114" s="3" t="s">
-        <v>2255</v>
+        <v>2252</v>
       </c>
       <c r="I1114" s="3" t="s">
-        <v>2256</v>
+        <v>154</v>
       </c>
       <c r="J1114" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1114" s="22" t="s">
-        <v>2257</v>
+        <v>1563</v>
       </c>
       <c r="L1114" s="22" t="s">
         <v>153</v>
@@ -72713,8 +72708,11 @@
       <c r="O1114" t="s">
         <v>313</v>
       </c>
+      <c r="P1114" t="s">
+        <v>5282</v>
+      </c>
       <c r="Q1114" t="s">
-        <v>8068</v>
+        <v>8067</v>
       </c>
       <c r="R1114" s="43">
         <v>45591.506944444402</v>
@@ -72722,34 +72720,34 @@
     </row>
     <row r="1115" spans="1:18">
       <c r="A1115" s="3" t="s">
-        <v>6490</v>
+        <v>6489</v>
       </c>
       <c r="B1115" s="46" t="s">
-        <v>47</v>
+        <v>5741</v>
       </c>
       <c r="C1115" s="41" t="s">
-        <v>7211</v>
+        <v>7431</v>
       </c>
       <c r="D1115" s="21" t="s">
-        <v>2258</v>
+        <v>2253</v>
       </c>
       <c r="E1115" s="23" t="s">
-        <v>2259</v>
+        <v>166</v>
       </c>
       <c r="F1115" s="21" t="s">
-        <v>705</v>
+        <v>2254</v>
       </c>
       <c r="G1115" s="3" t="s">
-        <v>2260</v>
+        <v>2255</v>
       </c>
       <c r="I1115" s="3" t="s">
-        <v>1148</v>
+        <v>2256</v>
       </c>
       <c r="J1115" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1115" s="22" t="s">
-        <v>708</v>
+        <v>2257</v>
       </c>
       <c r="L1115" s="22" t="s">
         <v>153</v>
@@ -72763,11 +72761,8 @@
       <c r="O1115" t="s">
         <v>313</v>
       </c>
-      <c r="P1115" t="s">
-        <v>5750</v>
-      </c>
       <c r="Q1115" t="s">
-        <v>8151</v>
+        <v>8068</v>
       </c>
       <c r="R1115" s="43">
         <v>45591.506944444402</v>
@@ -72775,34 +72770,34 @@
     </row>
     <row r="1116" spans="1:18">
       <c r="A1116" s="3" t="s">
-        <v>6491</v>
+        <v>6490</v>
       </c>
       <c r="B1116" s="46" t="s">
-        <v>5742</v>
+        <v>47</v>
       </c>
       <c r="C1116" s="41" t="s">
-        <v>7496</v>
+        <v>7211</v>
       </c>
       <c r="D1116" s="21" t="s">
-        <v>2261</v>
+        <v>2258</v>
       </c>
       <c r="E1116" s="23" t="s">
         <v>2259</v>
       </c>
       <c r="F1116" s="21" t="s">
-        <v>2262</v>
+        <v>705</v>
       </c>
       <c r="G1116" s="3" t="s">
-        <v>2263</v>
+        <v>2260</v>
       </c>
       <c r="I1116" s="3" t="s">
-        <v>2264</v>
+        <v>1148</v>
       </c>
       <c r="J1116" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1116" s="22" t="s">
-        <v>2265</v>
+        <v>708</v>
       </c>
       <c r="L1116" s="22" t="s">
         <v>153</v>
@@ -72816,8 +72811,11 @@
       <c r="O1116" t="s">
         <v>313</v>
       </c>
+      <c r="P1116" t="s">
+        <v>5750</v>
+      </c>
       <c r="Q1116" t="s">
-        <v>8069</v>
+        <v>8151</v>
       </c>
       <c r="R1116" s="43">
         <v>45591.506944444402</v>
@@ -72825,34 +72823,34 @@
     </row>
     <row r="1117" spans="1:18">
       <c r="A1117" s="3" t="s">
-        <v>6903</v>
+        <v>6491</v>
       </c>
       <c r="B1117" s="46" t="s">
-        <v>5743</v>
+        <v>5742</v>
       </c>
       <c r="C1117" s="41" t="s">
-        <v>7495</v>
+        <v>7496</v>
       </c>
       <c r="D1117" s="21" t="s">
-        <v>6907</v>
+        <v>2261</v>
       </c>
       <c r="E1117" s="23" t="s">
         <v>2259</v>
       </c>
       <c r="F1117" s="21" t="s">
-        <v>2267</v>
+        <v>2262</v>
       </c>
       <c r="G1117" s="3" t="s">
-        <v>2268</v>
+        <v>2263</v>
       </c>
       <c r="I1117" s="3" t="s">
-        <v>412</v>
+        <v>2264</v>
       </c>
       <c r="J1117" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1117" s="22" t="s">
-        <v>2269</v>
+        <v>2265</v>
       </c>
       <c r="L1117" s="22" t="s">
         <v>153</v>
@@ -72866,11 +72864,8 @@
       <c r="O1117" t="s">
         <v>313</v>
       </c>
-      <c r="P1117" t="s">
-        <v>5282</v>
-      </c>
       <c r="Q1117" t="s">
-        <v>8070</v>
+        <v>8069</v>
       </c>
       <c r="R1117" s="43">
         <v>45591.506944444402</v>
@@ -72878,34 +72873,34 @@
     </row>
     <row r="1118" spans="1:18">
       <c r="A1118" s="3" t="s">
-        <v>6492</v>
+        <v>6903</v>
       </c>
       <c r="B1118" s="46" t="s">
-        <v>5744</v>
+        <v>5743</v>
       </c>
       <c r="C1118" s="41" t="s">
-        <v>7532</v>
+        <v>7495</v>
       </c>
       <c r="D1118" s="21" t="s">
-        <v>2270</v>
+        <v>6907</v>
       </c>
       <c r="E1118" s="23" t="s">
-        <v>166</v>
+        <v>2259</v>
       </c>
       <c r="F1118" s="21" t="s">
-        <v>2271</v>
+        <v>2267</v>
       </c>
       <c r="G1118" s="3" t="s">
-        <v>2272</v>
+        <v>2268</v>
       </c>
       <c r="I1118" s="3" t="s">
-        <v>239</v>
+        <v>412</v>
       </c>
       <c r="J1118" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1118" s="22" t="s">
-        <v>2273</v>
+        <v>2269</v>
       </c>
       <c r="L1118" s="22" t="s">
         <v>153</v>
@@ -72923,7 +72918,7 @@
         <v>5282</v>
       </c>
       <c r="Q1118" t="s">
-        <v>7907</v>
+        <v>8070</v>
       </c>
       <c r="R1118" s="43">
         <v>45591.506944444402</v>
@@ -72931,34 +72926,34 @@
     </row>
     <row r="1119" spans="1:18">
       <c r="A1119" s="3" t="s">
-        <v>7769</v>
+        <v>6492</v>
       </c>
       <c r="B1119" s="46" t="s">
-        <v>5745</v>
+        <v>5744</v>
       </c>
       <c r="C1119" s="41" t="s">
-        <v>7429</v>
+        <v>7532</v>
       </c>
       <c r="D1119" s="21" t="s">
-        <v>2274</v>
+        <v>2270</v>
       </c>
       <c r="E1119" s="23" t="s">
         <v>166</v>
       </c>
       <c r="F1119" s="21" t="s">
-        <v>2275</v>
+        <v>2271</v>
       </c>
       <c r="G1119" s="3" t="s">
-        <v>2276</v>
+        <v>2272</v>
       </c>
       <c r="I1119" s="3" t="s">
-        <v>2277</v>
+        <v>239</v>
       </c>
       <c r="J1119" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1119" s="22" t="s">
-        <v>2278</v>
+        <v>2273</v>
       </c>
       <c r="L1119" s="22" t="s">
         <v>153</v>
@@ -72967,48 +72962,51 @@
         <v>313</v>
       </c>
       <c r="N1119" s="38" t="s">
-        <v>5746</v>
+        <v>2734</v>
       </c>
       <c r="O1119" t="s">
         <v>313</v>
       </c>
+      <c r="P1119" t="s">
+        <v>5282</v>
+      </c>
       <c r="Q1119" t="s">
-        <v>8152</v>
+        <v>7907</v>
       </c>
       <c r="R1119" s="43">
-        <v>45626.355034722197</v>
+        <v>45591.506944444402</v>
       </c>
     </row>
     <row r="1120" spans="1:18">
       <c r="A1120" s="3" t="s">
-        <v>6493</v>
+        <v>7769</v>
       </c>
       <c r="B1120" s="46" t="s">
-        <v>5747</v>
+        <v>5745</v>
       </c>
       <c r="C1120" s="41" t="s">
-        <v>7435</v>
+        <v>7429</v>
       </c>
       <c r="D1120" s="21" t="s">
-        <v>2279</v>
+        <v>2274</v>
       </c>
       <c r="E1120" s="23" t="s">
-        <v>2280</v>
+        <v>166</v>
       </c>
       <c r="F1120" s="21" t="s">
-        <v>2281</v>
+        <v>2275</v>
       </c>
       <c r="G1120" s="3" t="s">
-        <v>2282</v>
+        <v>2276</v>
       </c>
       <c r="I1120" s="3" t="s">
-        <v>245</v>
+        <v>2277</v>
       </c>
       <c r="J1120" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1120" s="22" t="s">
-        <v>2283</v>
+        <v>2278</v>
       </c>
       <c r="L1120" s="22" t="s">
         <v>153</v>
@@ -73017,48 +73015,48 @@
         <v>313</v>
       </c>
       <c r="N1120" s="38" t="s">
-        <v>2734</v>
+        <v>5746</v>
       </c>
       <c r="O1120" t="s">
         <v>313</v>
       </c>
       <c r="Q1120" t="s">
-        <v>7908</v>
+        <v>8152</v>
       </c>
       <c r="R1120" s="43">
-        <v>45591.506944444402</v>
+        <v>45626.355034722197</v>
       </c>
     </row>
     <row r="1121" spans="1:18">
       <c r="A1121" s="3" t="s">
-        <v>6494</v>
+        <v>6493</v>
       </c>
       <c r="B1121" s="46" t="s">
-        <v>5748</v>
+        <v>5747</v>
       </c>
       <c r="C1121" s="41" t="s">
-        <v>7243</v>
+        <v>7435</v>
       </c>
       <c r="D1121" s="21" t="s">
-        <v>2284</v>
+        <v>2279</v>
       </c>
       <c r="E1121" s="23" t="s">
-        <v>165</v>
+        <v>2280</v>
       </c>
       <c r="F1121" s="21" t="s">
-        <v>2285</v>
+        <v>2281</v>
       </c>
       <c r="G1121" s="3" t="s">
-        <v>2286</v>
+        <v>2282</v>
       </c>
       <c r="I1121" s="3" t="s">
-        <v>1513</v>
+        <v>245</v>
       </c>
       <c r="J1121" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1121" s="22" t="s">
-        <v>2287</v>
+        <v>2283</v>
       </c>
       <c r="L1121" s="22" t="s">
         <v>153</v>
@@ -73067,13 +73065,13 @@
         <v>313</v>
       </c>
       <c r="N1121" s="38" t="s">
-        <v>5310</v>
+        <v>2734</v>
       </c>
       <c r="O1121" t="s">
         <v>313</v>
       </c>
       <c r="Q1121" t="s">
-        <v>6494</v>
+        <v>7908</v>
       </c>
       <c r="R1121" s="43">
         <v>45591.506944444402</v>
@@ -73081,13 +73079,13 @@
     </row>
     <row r="1122" spans="1:18">
       <c r="A1122" s="3" t="s">
-        <v>6495</v>
+        <v>6494</v>
       </c>
       <c r="B1122" s="46" t="s">
-        <v>5749</v>
+        <v>5748</v>
       </c>
       <c r="C1122" s="41" t="s">
-        <v>7433</v>
+        <v>7243</v>
       </c>
       <c r="D1122" s="21" t="s">
         <v>2284</v>
@@ -73123,7 +73121,7 @@
         <v>313</v>
       </c>
       <c r="Q1122" t="s">
-        <v>7909</v>
+        <v>6494</v>
       </c>
       <c r="R1122" s="43">
         <v>45591.506944444402</v>
@@ -73131,31 +73129,34 @@
     </row>
     <row r="1123" spans="1:18">
       <c r="A1123" s="3" t="s">
-        <v>5812</v>
+        <v>6495</v>
       </c>
       <c r="B1123" s="46" t="s">
-        <v>5281</v>
+        <v>5749</v>
+      </c>
+      <c r="C1123" s="41" t="s">
+        <v>7433</v>
       </c>
       <c r="D1123" s="21" t="s">
-        <v>2258</v>
+        <v>2284</v>
       </c>
       <c r="E1123" s="23" t="s">
-        <v>821</v>
+        <v>165</v>
       </c>
       <c r="F1123" s="21" t="s">
-        <v>705</v>
+        <v>2285</v>
       </c>
       <c r="G1123" s="3" t="s">
-        <v>2260</v>
+        <v>2286</v>
       </c>
       <c r="I1123" s="3" t="s">
-        <v>1148</v>
+        <v>1513</v>
       </c>
       <c r="J1123" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1123" s="22" t="s">
-        <v>708</v>
+        <v>2287</v>
       </c>
       <c r="L1123" s="22" t="s">
         <v>153</v>
@@ -73164,16 +73165,13 @@
         <v>313</v>
       </c>
       <c r="N1123" s="38" t="s">
-        <v>5746</v>
+        <v>5310</v>
       </c>
       <c r="O1123" t="s">
         <v>313</v>
       </c>
-      <c r="P1123" t="s">
-        <v>5282</v>
-      </c>
       <c r="Q1123" t="s">
-        <v>5812</v>
+        <v>7909</v>
       </c>
       <c r="R1123" s="43">
         <v>45591.506944444402</v>
@@ -73181,34 +73179,31 @@
     </row>
     <row r="1124" spans="1:18">
       <c r="A1124" s="3" t="s">
-        <v>6496</v>
+        <v>5812</v>
       </c>
       <c r="B1124" s="46" t="s">
-        <v>5751</v>
-      </c>
-      <c r="C1124" s="41" t="s">
-        <v>7442</v>
+        <v>5281</v>
       </c>
       <c r="D1124" s="21" t="s">
-        <v>2266</v>
+        <v>2258</v>
       </c>
       <c r="E1124" s="23" t="s">
-        <v>844</v>
+        <v>821</v>
       </c>
       <c r="F1124" s="21" t="s">
-        <v>2267</v>
+        <v>705</v>
       </c>
       <c r="G1124" s="3" t="s">
-        <v>2268</v>
+        <v>2260</v>
       </c>
       <c r="I1124" s="3" t="s">
-        <v>412</v>
+        <v>1148</v>
       </c>
       <c r="J1124" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1124" s="22" t="s">
-        <v>2269</v>
+        <v>708</v>
       </c>
       <c r="L1124" s="22" t="s">
         <v>153</v>
@@ -73217,7 +73212,7 @@
         <v>313</v>
       </c>
       <c r="N1124" s="38" t="s">
-        <v>5752</v>
+        <v>5746</v>
       </c>
       <c r="O1124" t="s">
         <v>313</v>
@@ -73226,7 +73221,7 @@
         <v>5282</v>
       </c>
       <c r="Q1124" t="s">
-        <v>7910</v>
+        <v>5812</v>
       </c>
       <c r="R1124" s="43">
         <v>45591.506944444402</v>
@@ -73234,13 +73229,13 @@
     </row>
     <row r="1125" spans="1:18">
       <c r="A1125" s="3" t="s">
-        <v>6497</v>
+        <v>6496</v>
       </c>
       <c r="B1125" s="46" t="s">
-        <v>5753</v>
+        <v>5751</v>
       </c>
       <c r="C1125" s="41" t="s">
-        <v>7476</v>
+        <v>7442</v>
       </c>
       <c r="D1125" s="21" t="s">
         <v>2266</v>
@@ -73279,7 +73274,7 @@
         <v>5282</v>
       </c>
       <c r="Q1125" t="s">
-        <v>7911</v>
+        <v>7910</v>
       </c>
       <c r="R1125" s="43">
         <v>45591.506944444402</v>
@@ -73287,34 +73282,34 @@
     </row>
     <row r="1126" spans="1:18">
       <c r="A1126" s="3" t="s">
-        <v>6899</v>
+        <v>6497</v>
       </c>
       <c r="B1126" s="46" t="s">
-        <v>5754</v>
+        <v>5753</v>
       </c>
       <c r="C1126" s="41" t="s">
-        <v>7372</v>
+        <v>7476</v>
       </c>
       <c r="D1126" s="21" t="s">
-        <v>6908</v>
+        <v>2266</v>
       </c>
       <c r="E1126" s="23" t="s">
         <v>844</v>
       </c>
       <c r="F1126" s="21" t="s">
-        <v>2288</v>
+        <v>2267</v>
       </c>
       <c r="G1126" s="3" t="s">
-        <v>2289</v>
+        <v>2268</v>
       </c>
       <c r="I1126" s="3" t="s">
-        <v>2290</v>
+        <v>412</v>
       </c>
       <c r="J1126" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1126" s="22" t="s">
-        <v>2291</v>
+        <v>2269</v>
       </c>
       <c r="L1126" s="22" t="s">
         <v>153</v>
@@ -73323,13 +73318,16 @@
         <v>313</v>
       </c>
       <c r="N1126" s="38" t="s">
-        <v>2734</v>
+        <v>5752</v>
       </c>
       <c r="O1126" t="s">
-        <v>2292</v>
+        <v>313</v>
+      </c>
+      <c r="P1126" t="s">
+        <v>5282</v>
       </c>
       <c r="Q1126" t="s">
-        <v>7912</v>
+        <v>7911</v>
       </c>
       <c r="R1126" s="43">
         <v>45591.506944444402</v>
@@ -73337,34 +73335,34 @@
     </row>
     <row r="1127" spans="1:18">
       <c r="A1127" s="3" t="s">
-        <v>6498</v>
+        <v>6899</v>
       </c>
       <c r="B1127" s="46" t="s">
-        <v>5755</v>
+        <v>5754</v>
       </c>
       <c r="C1127" s="41" t="s">
-        <v>7536</v>
+        <v>7372</v>
       </c>
       <c r="D1127" s="21" t="s">
-        <v>2293</v>
+        <v>6908</v>
       </c>
       <c r="E1127" s="23" t="s">
-        <v>166</v>
+        <v>844</v>
       </c>
       <c r="F1127" s="21" t="s">
-        <v>2294</v>
+        <v>2288</v>
       </c>
       <c r="G1127" s="3" t="s">
-        <v>2295</v>
+        <v>2289</v>
       </c>
       <c r="I1127" s="3" t="s">
-        <v>164</v>
+        <v>2290</v>
       </c>
       <c r="J1127" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1127" s="22" t="s">
-        <v>2140</v>
+        <v>2291</v>
       </c>
       <c r="L1127" s="22" t="s">
         <v>153</v>
@@ -73373,13 +73371,13 @@
         <v>313</v>
       </c>
       <c r="N1127" s="38" t="s">
-        <v>5719</v>
+        <v>2734</v>
       </c>
       <c r="O1127" t="s">
-        <v>313</v>
+        <v>2292</v>
       </c>
       <c r="Q1127" t="s">
-        <v>7913</v>
+        <v>7912</v>
       </c>
       <c r="R1127" s="43">
         <v>45591.506944444402</v>
@@ -73387,13 +73385,13 @@
     </row>
     <row r="1128" spans="1:18">
       <c r="A1128" s="3" t="s">
-        <v>6499</v>
+        <v>6498</v>
       </c>
       <c r="B1128" s="46" t="s">
-        <v>5756</v>
+        <v>5755</v>
       </c>
       <c r="C1128" s="41" t="s">
-        <v>7419</v>
+        <v>7536</v>
       </c>
       <c r="D1128" s="21" t="s">
         <v>2293</v>
@@ -73402,22 +73400,19 @@
         <v>166</v>
       </c>
       <c r="F1128" s="21" t="s">
-        <v>2296</v>
+        <v>2294</v>
       </c>
       <c r="G1128" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="H1128" s="3" t="s">
-        <v>2297</v>
+        <v>2295</v>
       </c>
       <c r="I1128" s="3" t="s">
-        <v>245</v>
+        <v>164</v>
       </c>
       <c r="J1128" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1128" s="22" t="s">
-        <v>246</v>
+        <v>2140</v>
       </c>
       <c r="L1128" s="22" t="s">
         <v>153</v>
@@ -73426,16 +73421,13 @@
         <v>313</v>
       </c>
       <c r="N1128" s="38" t="s">
-        <v>2734</v>
+        <v>5719</v>
       </c>
       <c r="O1128" t="s">
         <v>313</v>
       </c>
-      <c r="P1128" t="s">
-        <v>2298</v>
-      </c>
       <c r="Q1128" t="s">
-        <v>7914</v>
+        <v>7913</v>
       </c>
       <c r="R1128" s="43">
         <v>45591.506944444402</v>
@@ -73443,34 +73435,37 @@
     </row>
     <row r="1129" spans="1:18">
       <c r="A1129" s="3" t="s">
-        <v>6500</v>
+        <v>6499</v>
       </c>
       <c r="B1129" s="46" t="s">
-        <v>5757</v>
+        <v>5756</v>
       </c>
       <c r="C1129" s="41" t="s">
-        <v>7350</v>
+        <v>7419</v>
       </c>
       <c r="D1129" s="21" t="s">
-        <v>2299</v>
+        <v>2293</v>
       </c>
       <c r="E1129" s="23" t="s">
         <v>166</v>
       </c>
       <c r="F1129" s="21" t="s">
-        <v>2300</v>
+        <v>2296</v>
       </c>
       <c r="G1129" s="3" t="s">
-        <v>2301</v>
+        <v>244</v>
+      </c>
+      <c r="H1129" s="3" t="s">
+        <v>2297</v>
       </c>
       <c r="I1129" s="3" t="s">
-        <v>1628</v>
+        <v>245</v>
       </c>
       <c r="J1129" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1129" s="22" t="s">
-        <v>2302</v>
+        <v>246</v>
       </c>
       <c r="L1129" s="22" t="s">
         <v>153</v>
@@ -73479,13 +73474,16 @@
         <v>313</v>
       </c>
       <c r="N1129" s="38" t="s">
-        <v>5737</v>
+        <v>2734</v>
       </c>
       <c r="O1129" t="s">
         <v>313</v>
       </c>
+      <c r="P1129" t="s">
+        <v>2298</v>
+      </c>
       <c r="Q1129" t="s">
-        <v>7915</v>
+        <v>7914</v>
       </c>
       <c r="R1129" s="43">
         <v>45591.506944444402</v>
@@ -73493,34 +73491,34 @@
     </row>
     <row r="1130" spans="1:18">
       <c r="A1130" s="3" t="s">
-        <v>6501</v>
+        <v>6500</v>
       </c>
       <c r="B1130" s="46" t="s">
-        <v>5283</v>
+        <v>5757</v>
       </c>
       <c r="C1130" s="41" t="s">
-        <v>7487</v>
+        <v>7350</v>
       </c>
       <c r="D1130" s="21" t="s">
-        <v>7630</v>
+        <v>2299</v>
       </c>
       <c r="E1130" s="23" t="s">
         <v>166</v>
       </c>
       <c r="F1130" s="21" t="s">
-        <v>2303</v>
+        <v>2300</v>
       </c>
       <c r="G1130" s="3" t="s">
-        <v>2304</v>
+        <v>2301</v>
       </c>
       <c r="I1130" s="3" t="s">
-        <v>2305</v>
+        <v>1628</v>
       </c>
       <c r="J1130" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1130" s="22" t="s">
-        <v>2306</v>
+        <v>2302</v>
       </c>
       <c r="L1130" s="22" t="s">
         <v>153</v>
@@ -73529,48 +73527,48 @@
         <v>313</v>
       </c>
       <c r="N1130" s="38" t="s">
-        <v>2734</v>
+        <v>5737</v>
       </c>
       <c r="O1130" t="s">
         <v>313</v>
       </c>
       <c r="Q1130" t="s">
-        <v>7916</v>
+        <v>7915</v>
       </c>
       <c r="R1130" s="43">
-        <v>45599.491631944402</v>
+        <v>45591.506944444402</v>
       </c>
     </row>
     <row r="1131" spans="1:18">
       <c r="A1131" s="3" t="s">
-        <v>6502</v>
+        <v>6501</v>
       </c>
       <c r="B1131" s="46" t="s">
-        <v>5758</v>
+        <v>5283</v>
       </c>
       <c r="C1131" s="41" t="s">
-        <v>7434</v>
+        <v>7487</v>
       </c>
       <c r="D1131" s="21" t="s">
-        <v>2307</v>
+        <v>7630</v>
       </c>
       <c r="E1131" s="23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F1131" s="21" t="s">
-        <v>2308</v>
+        <v>2303</v>
       </c>
       <c r="G1131" s="3" t="s">
-        <v>2286</v>
+        <v>2304</v>
       </c>
       <c r="I1131" s="3" t="s">
-        <v>1513</v>
+        <v>2305</v>
       </c>
       <c r="J1131" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1131" s="22" t="s">
-        <v>2287</v>
+        <v>2306</v>
       </c>
       <c r="L1131" s="22" t="s">
         <v>153</v>
@@ -73579,48 +73577,48 @@
         <v>313</v>
       </c>
       <c r="N1131" s="38" t="s">
-        <v>5310</v>
+        <v>2734</v>
       </c>
       <c r="O1131" t="s">
         <v>313</v>
       </c>
       <c r="Q1131" t="s">
-        <v>7917</v>
+        <v>7916</v>
       </c>
       <c r="R1131" s="43">
-        <v>45591.506944444402</v>
+        <v>45599.491631944402</v>
       </c>
     </row>
     <row r="1132" spans="1:18">
       <c r="A1132" s="3" t="s">
-        <v>7648</v>
+        <v>6502</v>
       </c>
       <c r="B1132" s="46" t="s">
-        <v>5759</v>
+        <v>5758</v>
       </c>
       <c r="C1132" s="41" t="s">
-        <v>7175</v>
+        <v>7434</v>
       </c>
       <c r="D1132" s="21" t="s">
-        <v>2279</v>
+        <v>2307</v>
       </c>
       <c r="E1132" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F1132" s="21" t="s">
-        <v>2281</v>
+        <v>2308</v>
       </c>
       <c r="G1132" s="3" t="s">
-        <v>2309</v>
+        <v>2286</v>
       </c>
       <c r="I1132" s="3" t="s">
-        <v>240</v>
+        <v>1513</v>
       </c>
       <c r="J1132" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1132" s="22" t="s">
-        <v>2310</v>
+        <v>2287</v>
       </c>
       <c r="L1132" s="22" t="s">
         <v>153</v>
@@ -73629,51 +73627,48 @@
         <v>313</v>
       </c>
       <c r="N1132" s="38" t="s">
-        <v>5737</v>
+        <v>5310</v>
       </c>
       <c r="O1132" t="s">
         <v>313</v>
       </c>
       <c r="Q1132" t="s">
-        <v>8153</v>
+        <v>7917</v>
       </c>
       <c r="R1132" s="43">
-        <v>45602.572002314802</v>
+        <v>45591.506944444402</v>
       </c>
     </row>
     <row r="1133" spans="1:18">
       <c r="A1133" s="3" t="s">
-        <v>6503</v>
+        <v>7648</v>
       </c>
       <c r="B1133" s="46" t="s">
-        <v>5760</v>
+        <v>5759</v>
       </c>
       <c r="C1133" s="41" t="s">
-        <v>7430</v>
+        <v>7175</v>
       </c>
       <c r="D1133" s="21" t="s">
-        <v>2311</v>
+        <v>2279</v>
       </c>
       <c r="E1133" s="23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F1133" s="21" t="s">
-        <v>2312</v>
+        <v>2281</v>
       </c>
       <c r="G1133" s="3" t="s">
-        <v>2313</v>
-      </c>
-      <c r="H1133" s="3" t="s">
-        <v>2314</v>
+        <v>2309</v>
       </c>
       <c r="I1133" s="3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="J1133" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1133" s="22" t="s">
-        <v>2315</v>
+        <v>2310</v>
       </c>
       <c r="L1133" s="22" t="s">
         <v>153</v>
@@ -73682,48 +73677,51 @@
         <v>313</v>
       </c>
       <c r="N1133" s="38" t="s">
-        <v>5728</v>
+        <v>5737</v>
       </c>
       <c r="O1133" t="s">
         <v>313</v>
       </c>
       <c r="Q1133" t="s">
-        <v>7918</v>
+        <v>8153</v>
       </c>
       <c r="R1133" s="43">
-        <v>45591.506944444402</v>
+        <v>45602.572002314802</v>
       </c>
     </row>
     <row r="1134" spans="1:18">
       <c r="A1134" s="3" t="s">
-        <v>6504</v>
+        <v>6503</v>
       </c>
       <c r="B1134" s="46" t="s">
-        <v>5761</v>
+        <v>5760</v>
       </c>
       <c r="C1134" s="41" t="s">
-        <v>7542</v>
+        <v>7430</v>
       </c>
       <c r="D1134" s="21" t="s">
-        <v>2316</v>
+        <v>2311</v>
       </c>
       <c r="E1134" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F1134" s="21" t="s">
-        <v>2317</v>
+        <v>2312</v>
       </c>
       <c r="G1134" s="3" t="s">
-        <v>2318</v>
+        <v>2313</v>
+      </c>
+      <c r="H1134" s="3" t="s">
+        <v>2314</v>
       </c>
       <c r="I1134" s="3" t="s">
-        <v>2319</v>
+        <v>245</v>
       </c>
       <c r="J1134" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1134" s="22" t="s">
-        <v>2320</v>
+        <v>2315</v>
       </c>
       <c r="L1134" s="22" t="s">
         <v>153</v>
@@ -73738,7 +73736,7 @@
         <v>313</v>
       </c>
       <c r="Q1134" t="s">
-        <v>7919</v>
+        <v>7918</v>
       </c>
       <c r="R1134" s="43">
         <v>45591.506944444402</v>
@@ -73746,34 +73744,34 @@
     </row>
     <row r="1135" spans="1:18">
       <c r="A1135" s="3" t="s">
-        <v>6505</v>
+        <v>6504</v>
       </c>
       <c r="B1135" s="46" t="s">
-        <v>5762</v>
+        <v>5761</v>
       </c>
       <c r="C1135" s="41" t="s">
-        <v>7437</v>
+        <v>7542</v>
       </c>
       <c r="D1135" s="21" t="s">
-        <v>2261</v>
+        <v>2316</v>
       </c>
       <c r="E1135" s="23" t="s">
         <v>166</v>
       </c>
       <c r="F1135" s="21" t="s">
-        <v>2262</v>
+        <v>2317</v>
       </c>
       <c r="G1135" s="3" t="s">
-        <v>2263</v>
+        <v>2318</v>
       </c>
       <c r="I1135" s="3" t="s">
-        <v>2264</v>
+        <v>2319</v>
       </c>
       <c r="J1135" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1135" s="22" t="s">
-        <v>2265</v>
+        <v>2320</v>
       </c>
       <c r="L1135" s="22" t="s">
         <v>153</v>
@@ -73782,13 +73780,13 @@
         <v>313</v>
       </c>
       <c r="N1135" s="38" t="s">
-        <v>2734</v>
+        <v>5728</v>
       </c>
       <c r="O1135" t="s">
         <v>313</v>
       </c>
       <c r="Q1135" t="s">
-        <v>7920</v>
+        <v>7919</v>
       </c>
       <c r="R1135" s="43">
         <v>45591.506944444402</v>
@@ -73796,34 +73794,34 @@
     </row>
     <row r="1136" spans="1:18">
       <c r="A1136" s="3" t="s">
-        <v>7647</v>
+        <v>6505</v>
       </c>
       <c r="B1136" s="46" t="s">
-        <v>6918</v>
+        <v>5762</v>
       </c>
       <c r="C1136" s="41" t="s">
-        <v>7164</v>
+        <v>7437</v>
       </c>
       <c r="D1136" s="21" t="s">
-        <v>2855</v>
+        <v>2261</v>
       </c>
       <c r="E1136" s="23" t="s">
         <v>166</v>
       </c>
       <c r="F1136" s="21" t="s">
-        <v>7783</v>
+        <v>2262</v>
       </c>
       <c r="G1136" s="3" t="s">
-        <v>2856</v>
+        <v>2263</v>
       </c>
       <c r="I1136" s="3" t="s">
-        <v>6919</v>
+        <v>2264</v>
       </c>
       <c r="J1136" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1136" s="22" t="s">
-        <v>2857</v>
+        <v>2265</v>
       </c>
       <c r="L1136" s="22" t="s">
         <v>153</v>
@@ -73832,74 +73830,80 @@
         <v>313</v>
       </c>
       <c r="N1136" s="38" t="s">
-        <v>5558</v>
+        <v>2734</v>
       </c>
       <c r="O1136" t="s">
         <v>313</v>
       </c>
-      <c r="P1136" t="s">
-        <v>5282</v>
-      </c>
       <c r="Q1136" t="s">
-        <v>8154</v>
+        <v>7920</v>
       </c>
       <c r="R1136" s="43">
-        <v>45634.650567129604</v>
+        <v>45591.506944444402</v>
       </c>
     </row>
     <row r="1137" spans="1:18">
       <c r="A1137" s="3" t="s">
-        <v>7636</v>
+        <v>7647</v>
       </c>
       <c r="B1137" s="46" t="s">
-        <v>7637</v>
+        <v>6918</v>
       </c>
       <c r="C1137" s="41" t="s">
-        <v>7638</v>
+        <v>7164</v>
       </c>
       <c r="D1137" s="21" t="s">
-        <v>7639</v>
+        <v>2855</v>
       </c>
       <c r="E1137" s="23" t="s">
         <v>166</v>
       </c>
       <c r="F1137" s="21" t="s">
-        <v>7640</v>
+        <v>7783</v>
       </c>
       <c r="G1137" s="3" t="s">
-        <v>7641</v>
+        <v>2856</v>
       </c>
       <c r="I1137" s="3" t="s">
-        <v>7642</v>
+        <v>6919</v>
       </c>
       <c r="J1137" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1137" s="22" t="s">
-        <v>7643</v>
+        <v>2857</v>
       </c>
       <c r="L1137" s="22" t="s">
         <v>153</v>
       </c>
+      <c r="M1137" t="s">
+        <v>313</v>
+      </c>
       <c r="N1137" s="38" t="s">
-        <v>2734</v>
+        <v>5558</v>
+      </c>
+      <c r="O1137" t="s">
+        <v>313</v>
+      </c>
+      <c r="P1137" t="s">
+        <v>5282</v>
       </c>
       <c r="Q1137" t="s">
-        <v>7921</v>
+        <v>8154</v>
       </c>
       <c r="R1137" s="43">
-        <v>45602.4203935185</v>
+        <v>45634.650567129604</v>
       </c>
     </row>
     <row r="1138" spans="1:18">
       <c r="A1138" s="3" t="s">
-        <v>7644</v>
+        <v>7636</v>
       </c>
       <c r="B1138" s="46" t="s">
-        <v>7645</v>
+        <v>7637</v>
       </c>
       <c r="C1138" s="41" t="s">
-        <v>7646</v>
+        <v>7638</v>
       </c>
       <c r="D1138" s="21" t="s">
         <v>7639</v>
@@ -73929,86 +73933,83 @@
         <v>2734</v>
       </c>
       <c r="Q1138" t="s">
-        <v>7922</v>
+        <v>7921</v>
       </c>
       <c r="R1138" s="43">
-        <v>45602.422002314801</v>
+        <v>45602.4203935185</v>
       </c>
     </row>
     <row r="1139" spans="1:18">
       <c r="A1139" s="3" t="s">
-        <v>8160</v>
+        <v>7644</v>
       </c>
       <c r="B1139" s="46" t="s">
-        <v>8161</v>
+        <v>7645</v>
       </c>
       <c r="C1139" s="41" t="s">
-        <v>8172</v>
+        <v>7646</v>
       </c>
       <c r="D1139" s="21" t="s">
-        <v>8162</v>
+        <v>7639</v>
+      </c>
+      <c r="E1139" s="23" t="s">
+        <v>166</v>
       </c>
       <c r="F1139" s="21" t="s">
-        <v>8163</v>
+        <v>7640</v>
       </c>
       <c r="G1139" s="3" t="s">
-        <v>8164</v>
+        <v>7641</v>
       </c>
       <c r="I1139" s="3" t="s">
-        <v>164</v>
+        <v>7642</v>
       </c>
       <c r="J1139" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1139" s="22" t="s">
-        <v>8165</v>
+        <v>7643</v>
       </c>
       <c r="L1139" s="22" t="s">
         <v>153</v>
-      </c>
-      <c r="M1139" t="s">
-        <v>313</v>
       </c>
       <c r="N1139" s="38" t="s">
         <v>2734</v>
       </c>
-      <c r="O1139" t="s">
-        <v>313</v>
-      </c>
       <c r="Q1139" t="s">
-        <v>8183</v>
+        <v>7922</v>
       </c>
       <c r="R1139" s="43">
-        <v>45685.697800925896</v>
+        <v>45602.422002314801</v>
       </c>
     </row>
     <row r="1140" spans="1:18">
       <c r="A1140" s="3" t="s">
-        <v>8173</v>
+        <v>8160</v>
       </c>
       <c r="B1140" s="46" t="s">
-        <v>8166</v>
+        <v>8161</v>
       </c>
       <c r="C1140" s="41" t="s">
-        <v>8167</v>
+        <v>8172</v>
       </c>
       <c r="D1140" s="21" t="s">
-        <v>8168</v>
-      </c>
-      <c r="E1140" s="23" t="s">
-        <v>166</v>
+        <v>8162</v>
+      </c>
+      <c r="F1140" s="21" t="s">
+        <v>8163</v>
       </c>
       <c r="G1140" s="3" t="s">
-        <v>8169</v>
+        <v>8164</v>
       </c>
       <c r="I1140" s="3" t="s">
-        <v>8170</v>
+        <v>164</v>
       </c>
       <c r="J1140" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1140" s="22" t="s">
-        <v>8171</v>
+        <v>8165</v>
       </c>
       <c r="L1140" s="22" t="s">
         <v>153</v>
@@ -74023,39 +74024,39 @@
         <v>313</v>
       </c>
       <c r="Q1140" t="s">
-        <v>8182</v>
+        <v>8183</v>
       </c>
       <c r="R1140" s="43">
-        <v>45685.697476851798</v>
+        <v>45685.697800925896</v>
       </c>
     </row>
     <row r="1141" spans="1:18">
       <c r="A1141" s="3" t="s">
-        <v>8174</v>
+        <v>8173</v>
       </c>
       <c r="B1141" s="46" t="s">
-        <v>8175</v>
+        <v>8166</v>
       </c>
       <c r="C1141" s="41" t="s">
-        <v>8176</v>
+        <v>8167</v>
       </c>
       <c r="D1141" s="21" t="s">
-        <v>8177</v>
+        <v>8168</v>
       </c>
       <c r="E1141" s="23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G1141" s="3" t="s">
-        <v>8178</v>
+        <v>8169</v>
       </c>
       <c r="I1141" s="3" t="s">
-        <v>8179</v>
+        <v>8170</v>
       </c>
       <c r="J1141" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1141" s="22" t="s">
-        <v>8180</v>
+        <v>8171</v>
       </c>
       <c r="L1141" s="22" t="s">
         <v>153</v>
@@ -74070,36 +74071,39 @@
         <v>313</v>
       </c>
       <c r="Q1141" t="s">
-        <v>8181</v>
+        <v>8182</v>
       </c>
       <c r="R1141" s="43">
-        <v>45685.697141203702</v>
+        <v>45685.697476851798</v>
       </c>
     </row>
     <row r="1142" spans="1:18">
       <c r="A1142" s="3" t="s">
-        <v>8184</v>
+        <v>8174</v>
       </c>
       <c r="B1142" s="46" t="s">
-        <v>8185</v>
+        <v>8175</v>
       </c>
       <c r="C1142" s="41" t="s">
-        <v>8186</v>
+        <v>8176</v>
       </c>
       <c r="D1142" s="21" t="s">
         <v>8177</v>
       </c>
+      <c r="E1142" s="23" t="s">
+        <v>165</v>
+      </c>
       <c r="G1142" s="3" t="s">
-        <v>8187</v>
+        <v>8178</v>
       </c>
       <c r="I1142" s="3" t="s">
-        <v>4557</v>
+        <v>8179</v>
       </c>
       <c r="J1142" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1142" s="22" t="s">
-        <v>4558</v>
+        <v>8180</v>
       </c>
       <c r="L1142" s="22" t="s">
         <v>153</v>
@@ -74107,342 +74111,351 @@
       <c r="M1142" t="s">
         <v>313</v>
       </c>
+      <c r="N1142" s="38" t="s">
+        <v>2734</v>
+      </c>
       <c r="O1142" t="s">
         <v>313</v>
       </c>
       <c r="Q1142" t="s">
-        <v>8188</v>
+        <v>8181</v>
       </c>
       <c r="R1142" s="43">
-        <v>45686.720590277801</v>
+        <v>45685.697141203702</v>
       </c>
     </row>
     <row r="1143" spans="1:18">
       <c r="A1143" s="3" t="s">
-        <v>8264</v>
+        <v>8184</v>
       </c>
       <c r="B1143" s="46" t="s">
-        <v>8217</v>
+        <v>8185</v>
+      </c>
+      <c r="C1143" s="41" t="s">
+        <v>8186</v>
       </c>
       <c r="D1143" s="21" t="s">
-        <v>8218</v>
-      </c>
-      <c r="E1143" s="23" t="s">
-        <v>8219</v>
-      </c>
-      <c r="F1143" s="21" t="s">
-        <v>8220</v>
+        <v>8177</v>
       </c>
       <c r="G1143" s="3" t="s">
-        <v>8265</v>
+        <v>8187</v>
       </c>
       <c r="I1143" s="3" t="s">
-        <v>8266</v>
+        <v>4557</v>
       </c>
       <c r="J1143" s="22" t="s">
-        <v>8267</v>
+        <v>563</v>
       </c>
       <c r="K1143" s="22" t="s">
-        <v>8268</v>
+        <v>4558</v>
+      </c>
+      <c r="L1143" s="22" t="s">
+        <v>153</v>
       </c>
       <c r="M1143" t="s">
-        <v>8221</v>
+        <v>313</v>
+      </c>
+      <c r="O1143" t="s">
+        <v>313</v>
       </c>
       <c r="Q1143" t="s">
-        <v>8264</v>
+        <v>8188</v>
       </c>
       <c r="R1143" s="43">
-        <v>45704.650717592602</v>
+        <v>45686.720590277801</v>
       </c>
     </row>
     <row r="1144" spans="1:18">
       <c r="A1144" s="3" t="s">
-        <v>8342</v>
+        <v>8264</v>
       </c>
       <c r="B1144" s="46" t="s">
-        <v>8343</v>
-      </c>
-      <c r="C1144" s="41" t="s">
-        <v>8344</v>
+        <v>8217</v>
       </c>
       <c r="D1144" s="21" t="s">
-        <v>8345</v>
+        <v>8218</v>
+      </c>
+      <c r="E1144" s="23" t="s">
+        <v>8219</v>
       </c>
       <c r="F1144" s="21" t="s">
-        <v>8346</v>
+        <v>8220</v>
       </c>
       <c r="G1144" s="3" t="s">
-        <v>8347</v>
+        <v>8265</v>
       </c>
       <c r="I1144" s="3" t="s">
-        <v>2433</v>
+        <v>8266</v>
       </c>
       <c r="J1144" s="22" t="s">
-        <v>563</v>
+        <v>8267</v>
       </c>
       <c r="K1144" s="22" t="s">
-        <v>8348</v>
-      </c>
-      <c r="L1144" s="22" t="s">
-        <v>153</v>
+        <v>8268</v>
       </c>
       <c r="M1144" t="s">
-        <v>313</v>
-      </c>
-      <c r="N1144" s="38" t="s">
-        <v>5736</v>
-      </c>
-      <c r="O1144" t="s">
-        <v>313</v>
+        <v>8221</v>
       </c>
       <c r="Q1144" t="s">
-        <v>8349</v>
+        <v>8264</v>
       </c>
       <c r="R1144" s="43">
-        <v>45771.699247685203</v>
+        <v>45704.650717592602</v>
       </c>
     </row>
     <row r="1145" spans="1:18">
       <c r="A1145" s="3" t="s">
-        <v>8231</v>
+        <v>8342</v>
       </c>
       <c r="B1145" s="46" t="s">
-        <v>51</v>
+        <v>8343</v>
+      </c>
+      <c r="C1145" s="41" t="s">
+        <v>8344</v>
+      </c>
+      <c r="D1145" s="21" t="s">
+        <v>8345</v>
+      </c>
+      <c r="F1145" s="21" t="s">
+        <v>8346</v>
+      </c>
+      <c r="G1145" s="3" t="s">
+        <v>8347</v>
+      </c>
+      <c r="I1145" s="3" t="s">
+        <v>2433</v>
+      </c>
+      <c r="J1145" s="22" t="s">
+        <v>563</v>
+      </c>
+      <c r="K1145" s="22" t="s">
+        <v>8348</v>
+      </c>
+      <c r="L1145" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1145" t="s">
+        <v>313</v>
+      </c>
+      <c r="N1145" s="38" t="s">
+        <v>5736</v>
+      </c>
+      <c r="O1145" t="s">
+        <v>313</v>
       </c>
       <c r="Q1145" t="s">
-        <v>8231</v>
+        <v>8349</v>
       </c>
       <c r="R1145" s="43">
-        <v>45716.706921296303</v>
+        <v>45771.699247685203</v>
       </c>
     </row>
     <row r="1146" spans="1:18">
       <c r="A1146" s="3" t="s">
-        <v>8288</v>
+        <v>8231</v>
       </c>
       <c r="B1146" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1146" s="21" t="s">
-        <v>8218</v>
-      </c>
-      <c r="E1146" s="23" t="s">
-        <v>8219</v>
-      </c>
-      <c r="F1146" s="21" t="s">
-        <v>8220</v>
-      </c>
-      <c r="G1146" s="3" t="s">
-        <v>8265</v>
-      </c>
-      <c r="I1146" s="3" t="s">
-        <v>8266</v>
-      </c>
-      <c r="J1146" s="22" t="s">
-        <v>8267</v>
-      </c>
-      <c r="K1146" s="22" t="s">
-        <v>8268</v>
-      </c>
-      <c r="M1146" t="s">
-        <v>8221</v>
+        <v>51</v>
       </c>
       <c r="Q1146" t="s">
-        <v>8264</v>
+        <v>8231</v>
+      </c>
+      <c r="R1146" s="43">
+        <v>45716.706921296303</v>
       </c>
     </row>
     <row r="1147" spans="1:18">
       <c r="A1147" s="3" t="s">
-        <v>8283</v>
+        <v>8288</v>
       </c>
       <c r="B1147" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1147" s="41" t="s">
-        <v>8284</v>
+        <v>92</v>
       </c>
       <c r="D1147" s="21" t="s">
-        <v>8285</v>
+        <v>8218</v>
+      </c>
+      <c r="E1147" s="23" t="s">
+        <v>8219</v>
       </c>
       <c r="F1147" s="21" t="s">
-        <v>8286</v>
+        <v>8220</v>
       </c>
       <c r="G1147" s="3" t="s">
-        <v>8287</v>
+        <v>8265</v>
       </c>
       <c r="I1147" s="3" t="s">
-        <v>245</v>
+        <v>8266</v>
       </c>
       <c r="J1147" s="22" t="s">
-        <v>563</v>
+        <v>8267</v>
+      </c>
+      <c r="K1147" s="22" t="s">
+        <v>8268</v>
+      </c>
+      <c r="M1147" t="s">
+        <v>8221</v>
       </c>
       <c r="Q1147" t="s">
-        <v>8283</v>
+        <v>8264</v>
       </c>
     </row>
     <row r="1148" spans="1:18">
       <c r="A1148" s="3" t="s">
-        <v>8289</v>
+        <v>8283</v>
       </c>
       <c r="B1148" s="46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C1148" s="41" t="s">
-        <v>8290</v>
+        <v>8284</v>
       </c>
       <c r="D1148" s="21" t="s">
-        <v>8291</v>
+        <v>8285</v>
       </c>
       <c r="F1148" s="21" t="s">
-        <v>8292</v>
-      </c>
-      <c r="M1148" t="s">
-        <v>8284</v>
+        <v>8286</v>
+      </c>
+      <c r="G1148" s="3" t="s">
+        <v>8287</v>
+      </c>
+      <c r="I1148" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="J1148" s="22" t="s">
+        <v>563</v>
       </c>
       <c r="Q1148" t="s">
-        <v>8293</v>
-      </c>
-      <c r="R1148" s="43">
-        <v>45732.587546296301</v>
+        <v>8283</v>
       </c>
     </row>
     <row r="1149" spans="1:18">
       <c r="A1149" s="3" t="s">
-        <v>8294</v>
+        <v>8289</v>
       </c>
       <c r="B1149" s="46" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C1149" s="41" t="s">
-        <v>8295</v>
+        <v>8290</v>
       </c>
       <c r="D1149" s="21" t="s">
-        <v>8295</v>
-      </c>
-      <c r="E1149" s="23" t="s">
-        <v>167</v>
+        <v>8291</v>
       </c>
       <c r="F1149" s="21" t="s">
-        <v>8296</v>
+        <v>8292</v>
+      </c>
+      <c r="M1149" t="s">
+        <v>8284</v>
       </c>
       <c r="Q1149" t="s">
-        <v>8294</v>
+        <v>8293</v>
       </c>
       <c r="R1149" s="43">
-        <v>45738.6483449074</v>
+        <v>45732.587546296301</v>
       </c>
     </row>
     <row r="1150" spans="1:18">
       <c r="A1150" s="3" t="s">
-        <v>8297</v>
+        <v>8294</v>
       </c>
       <c r="B1150" s="46" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C1150" s="41" t="s">
-        <v>8297</v>
+        <v>8295</v>
       </c>
       <c r="D1150" s="21" t="s">
-        <v>8297</v>
+        <v>8295</v>
+      </c>
+      <c r="E1150" s="23" t="s">
+        <v>167</v>
       </c>
       <c r="F1150" s="21" t="s">
-        <v>8298</v>
+        <v>8296</v>
       </c>
       <c r="Q1150" t="s">
-        <v>8297</v>
+        <v>8294</v>
       </c>
       <c r="R1150" s="43">
-        <v>45743.487731481502</v>
+        <v>45738.6483449074</v>
       </c>
     </row>
     <row r="1151" spans="1:18">
       <c r="A1151" s="3" t="s">
-        <v>8391</v>
+        <v>8297</v>
       </c>
       <c r="B1151" s="46" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C1151" s="41" t="s">
-        <v>8392</v>
+        <v>8297</v>
       </c>
       <c r="D1151" s="21" t="s">
-        <v>8393</v>
+        <v>8297</v>
       </c>
       <c r="F1151" s="21" t="s">
-        <v>8394</v>
-      </c>
-      <c r="G1151" s="3" t="s">
-        <v>8395</v>
-      </c>
-      <c r="I1151" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="J1151" s="22" t="s">
-        <v>563</v>
-      </c>
-      <c r="K1151" s="22" t="s">
-        <v>4016</v>
+        <v>8298</v>
       </c>
       <c r="Q1151" t="s">
-        <v>8391</v>
+        <v>8297</v>
       </c>
       <c r="R1151" s="43">
-        <v>45784.950891203698</v>
+        <v>45743.487731481502</v>
       </c>
     </row>
     <row r="1152" spans="1:18">
       <c r="A1152" s="3" t="s">
-        <v>8396</v>
+        <v>8391</v>
       </c>
       <c r="B1152" s="46" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C1152" s="41" t="s">
-        <v>8397</v>
+        <v>8392</v>
       </c>
       <c r="D1152" s="21" t="s">
-        <v>8398</v>
+        <v>8393</v>
       </c>
       <c r="F1152" s="21" t="s">
-        <v>8398</v>
+        <v>8394</v>
       </c>
       <c r="G1152" s="3" t="s">
-        <v>8399</v>
+        <v>8395</v>
       </c>
       <c r="I1152" s="3" t="s">
-        <v>245</v>
+        <v>171</v>
       </c>
       <c r="J1152" s="22" t="s">
         <v>563</v>
       </c>
       <c r="K1152" s="22" t="s">
-        <v>8400</v>
+        <v>4016</v>
       </c>
       <c r="Q1152" t="s">
-        <v>8396</v>
+        <v>8391</v>
       </c>
       <c r="R1152" s="43">
-        <v>45784.950520833299</v>
+        <v>45784.950891203698</v>
       </c>
     </row>
     <row r="1153" spans="1:18">
       <c r="A1153" s="3" t="s">
-        <v>8406</v>
+        <v>8396</v>
       </c>
       <c r="B1153" s="46" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C1153" s="41" t="s">
-        <v>8407</v>
+        <v>8397</v>
       </c>
       <c r="D1153" s="21" t="s">
-        <v>8408</v>
+        <v>8398</v>
       </c>
       <c r="F1153" s="21" t="s">
-        <v>8409</v>
+        <v>8398</v>
       </c>
       <c r="G1153" s="3" t="s">
-        <v>8411</v>
+        <v>8399</v>
       </c>
       <c r="I1153" s="3" t="s">
         <v>245</v>
@@ -74451,140 +74464,136 @@
         <v>563</v>
       </c>
       <c r="K1153" s="22" t="s">
-        <v>8412</v>
-      </c>
-      <c r="M1153" s="25" t="s">
-        <v>8410</v>
-      </c>
-      <c r="N1153" s="24"/>
-      <c r="O1153" s="25"/>
-      <c r="P1153" s="25"/>
-      <c r="Q1153" s="25" t="s">
-        <v>8406</v>
+        <v>8400</v>
+      </c>
+      <c r="Q1153" t="s">
+        <v>8396</v>
       </c>
       <c r="R1153" s="43">
-        <v>45785.929756944402</v>
+        <v>45784.950520833299</v>
       </c>
     </row>
     <row r="1154" spans="1:18">
       <c r="A1154" s="3" t="s">
-        <v>8446</v>
+        <v>8406</v>
       </c>
       <c r="B1154" s="46" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C1154" s="41" t="s">
-        <v>8447</v>
-      </c>
-      <c r="E1154" s="23" t="s">
-        <v>6080</v>
+        <v>8407</v>
+      </c>
+      <c r="D1154" s="21" t="s">
+        <v>8408</v>
       </c>
       <c r="F1154" s="21" t="s">
-        <v>8448</v>
+        <v>8409</v>
       </c>
       <c r="G1154" s="3" t="s">
-        <v>8449</v>
+        <v>8411</v>
       </c>
       <c r="I1154" s="3" t="s">
-        <v>8266</v>
+        <v>245</v>
       </c>
       <c r="J1154" s="22" t="s">
-        <v>8267</v>
+        <v>563</v>
       </c>
       <c r="K1154" s="22" t="s">
-        <v>8450</v>
-      </c>
-      <c r="M1154" s="25"/>
+        <v>8412</v>
+      </c>
+      <c r="M1154" s="25" t="s">
+        <v>8410</v>
+      </c>
       <c r="N1154" s="24"/>
       <c r="O1154" s="25"/>
       <c r="P1154" s="25"/>
       <c r="Q1154" s="25" t="s">
+        <v>8406</v>
+      </c>
+      <c r="R1154" s="43">
+        <v>45785.929756944402</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:18">
+      <c r="A1155" s="3" t="s">
         <v>8446</v>
       </c>
-      <c r="R1154" s="43">
+      <c r="B1155" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1155" s="41" t="s">
+        <v>8447</v>
+      </c>
+      <c r="E1155" s="23" t="s">
+        <v>6080</v>
+      </c>
+      <c r="F1155" s="21" t="s">
+        <v>8448</v>
+      </c>
+      <c r="G1155" s="3" t="s">
+        <v>8449</v>
+      </c>
+      <c r="I1155" s="3" t="s">
+        <v>8266</v>
+      </c>
+      <c r="J1155" s="22" t="s">
+        <v>8267</v>
+      </c>
+      <c r="K1155" s="22" t="s">
+        <v>8450</v>
+      </c>
+      <c r="M1155" s="25"/>
+      <c r="N1155" s="24"/>
+      <c r="O1155" s="25"/>
+      <c r="P1155" s="25"/>
+      <c r="Q1155" s="25" t="s">
+        <v>8446</v>
+      </c>
+      <c r="R1155" s="43">
         <v>45798.954733796301</v>
       </c>
     </row>
-    <row r="1155" spans="1:18">
-      <c r="A1155" s="31" t="s">
-        <v>8457</v>
-      </c>
-      <c r="B1155" s="31" t="s">
-        <v>8458</v>
-      </c>
-      <c r="C1155" s="31" t="s">
-        <v>7424</v>
-      </c>
-      <c r="D1155" s="31" t="s">
-        <v>8459</v>
-      </c>
-      <c r="E1155" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="F1155" s="31" t="s">
-        <v>8460</v>
-      </c>
-      <c r="G1155" s="31" t="s">
-        <v>8461</v>
-      </c>
-      <c r="I1155" s="31" t="s">
-        <v>245</v>
-      </c>
-      <c r="J1155" s="31" t="s">
-        <v>563</v>
-      </c>
-      <c r="K1155" s="31" t="s">
-        <v>8462</v>
-      </c>
-      <c r="L1155" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="M1155" s="31" t="s">
-        <v>3420</v>
-      </c>
-      <c r="Q1155" s="31" t="s">
-        <v>8463</v>
-      </c>
-      <c r="R1155" s="47">
-        <v>45805.666157407402</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:R1147" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1151:R1153">
-    <sortCondition ref="B1151:B1153"/>
+  <autoFilter ref="A1:R1148" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1152:R1154">
+    <sortCondition ref="B1152:B1154"/>
   </sortState>
-  <conditionalFormatting sqref="A2:R1154">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="A2:R1109 A1111:R1155">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND($A2&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A1110:R1110">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND($A1110&lt;&gt;"",MOD(ROW(),2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F1135" r:id="rId1" xr:uid="{F456DE86-0DC4-459B-8786-AEB12C0F36B0}"/>
-    <hyperlink ref="F1134" r:id="rId2" xr:uid="{A987B60B-629E-450A-AFE5-A7284329CD96}"/>
-    <hyperlink ref="F1133" r:id="rId3" xr:uid="{BDA96C0A-370D-46F7-82B7-86D5AE155E9F}"/>
-    <hyperlink ref="F1132" r:id="rId4" xr:uid="{E0EF30A2-FEE8-48F7-905E-3DCEE9D90336}"/>
-    <hyperlink ref="F1131" r:id="rId5" xr:uid="{F5EE9F94-288C-4D35-98F2-B7DF314331DE}"/>
-    <hyperlink ref="F1130" r:id="rId6" xr:uid="{A71B48CB-C499-456A-8FFD-47EFE60A828E}"/>
-    <hyperlink ref="F1129" r:id="rId7" xr:uid="{AF04FF5C-ADCA-44DC-B3B2-A425FC0DCFD9}"/>
-    <hyperlink ref="F1128" r:id="rId8" xr:uid="{F55EAFC5-5519-4A1F-80D4-95B4D202FE38}"/>
-    <hyperlink ref="F1127" r:id="rId9" xr:uid="{5FE20200-FB86-452E-8BE1-863A3C65BD07}"/>
-    <hyperlink ref="F1126" r:id="rId10" xr:uid="{8F88B4B6-197E-4940-B572-1769D2C402A3}"/>
-    <hyperlink ref="F1125" r:id="rId11" xr:uid="{DACEA89F-4573-408A-AA3D-AAFC4DF8DB2E}"/>
-    <hyperlink ref="F1124" r:id="rId12" xr:uid="{BF25E2D2-8541-4371-99B7-17A8B86CC8F6}"/>
-    <hyperlink ref="F1123" r:id="rId13" xr:uid="{57CD897B-E530-431D-A4B5-59D9C0F63217}"/>
-    <hyperlink ref="F1122" r:id="rId14" xr:uid="{CEEE77DB-0464-4890-9DA6-629F365AAC93}"/>
-    <hyperlink ref="F1121" r:id="rId15" xr:uid="{D183A8CF-2618-4DDD-8523-A347B0789735}"/>
-    <hyperlink ref="F1120" r:id="rId16" xr:uid="{B44DC245-3939-4FC4-B86F-7F55F80E20F1}"/>
-    <hyperlink ref="F1119" r:id="rId17" xr:uid="{77BEB31C-67F9-4892-974A-C42D173ACEC7}"/>
-    <hyperlink ref="F1118" r:id="rId18" xr:uid="{802015E0-18C1-4D8F-BD48-60606EF00558}"/>
-    <hyperlink ref="F1117" r:id="rId19" xr:uid="{185AA3D8-0081-42DB-B36C-3B1B4DF6AE78}"/>
-    <hyperlink ref="F1116" r:id="rId20" xr:uid="{C92F0FF0-F014-47C6-8A1D-37500F8CB37C}"/>
-    <hyperlink ref="F1115" r:id="rId21" xr:uid="{A79E531F-E421-48DC-B313-0C433AA33C66}"/>
-    <hyperlink ref="F1114" r:id="rId22" xr:uid="{CF6C1299-30F9-427A-9C11-CDEF3096DB13}"/>
-    <hyperlink ref="F1113" r:id="rId23" xr:uid="{B0ED86D2-3643-405A-B6A7-581D3F444E88}"/>
-    <hyperlink ref="F1112" r:id="rId24" xr:uid="{3643C6A3-6F1E-403F-B5BD-A7251D505F5B}"/>
-    <hyperlink ref="F1110" r:id="rId25" xr:uid="{0E92FFCB-F966-4697-91BE-A3130C1CAE25}"/>
+    <hyperlink ref="F1136" r:id="rId1" xr:uid="{F456DE86-0DC4-459B-8786-AEB12C0F36B0}"/>
+    <hyperlink ref="F1135" r:id="rId2" xr:uid="{A987B60B-629E-450A-AFE5-A7284329CD96}"/>
+    <hyperlink ref="F1134" r:id="rId3" xr:uid="{BDA96C0A-370D-46F7-82B7-86D5AE155E9F}"/>
+    <hyperlink ref="F1133" r:id="rId4" xr:uid="{E0EF30A2-FEE8-48F7-905E-3DCEE9D90336}"/>
+    <hyperlink ref="F1132" r:id="rId5" xr:uid="{F5EE9F94-288C-4D35-98F2-B7DF314331DE}"/>
+    <hyperlink ref="F1131" r:id="rId6" xr:uid="{A71B48CB-C499-456A-8FFD-47EFE60A828E}"/>
+    <hyperlink ref="F1130" r:id="rId7" xr:uid="{AF04FF5C-ADCA-44DC-B3B2-A425FC0DCFD9}"/>
+    <hyperlink ref="F1129" r:id="rId8" xr:uid="{F55EAFC5-5519-4A1F-80D4-95B4D202FE38}"/>
+    <hyperlink ref="F1128" r:id="rId9" xr:uid="{5FE20200-FB86-452E-8BE1-863A3C65BD07}"/>
+    <hyperlink ref="F1127" r:id="rId10" xr:uid="{8F88B4B6-197E-4940-B572-1769D2C402A3}"/>
+    <hyperlink ref="F1126" r:id="rId11" xr:uid="{DACEA89F-4573-408A-AA3D-AAFC4DF8DB2E}"/>
+    <hyperlink ref="F1125" r:id="rId12" xr:uid="{BF25E2D2-8541-4371-99B7-17A8B86CC8F6}"/>
+    <hyperlink ref="F1124" r:id="rId13" xr:uid="{57CD897B-E530-431D-A4B5-59D9C0F63217}"/>
+    <hyperlink ref="F1123" r:id="rId14" xr:uid="{CEEE77DB-0464-4890-9DA6-629F365AAC93}"/>
+    <hyperlink ref="F1122" r:id="rId15" xr:uid="{D183A8CF-2618-4DDD-8523-A347B0789735}"/>
+    <hyperlink ref="F1121" r:id="rId16" xr:uid="{B44DC245-3939-4FC4-B86F-7F55F80E20F1}"/>
+    <hyperlink ref="F1120" r:id="rId17" xr:uid="{77BEB31C-67F9-4892-974A-C42D173ACEC7}"/>
+    <hyperlink ref="F1119" r:id="rId18" xr:uid="{802015E0-18C1-4D8F-BD48-60606EF00558}"/>
+    <hyperlink ref="F1118" r:id="rId19" xr:uid="{185AA3D8-0081-42DB-B36C-3B1B4DF6AE78}"/>
+    <hyperlink ref="F1117" r:id="rId20" xr:uid="{C92F0FF0-F014-47C6-8A1D-37500F8CB37C}"/>
+    <hyperlink ref="F1116" r:id="rId21" xr:uid="{A79E531F-E421-48DC-B313-0C433AA33C66}"/>
+    <hyperlink ref="F1115" r:id="rId22" xr:uid="{CF6C1299-30F9-427A-9C11-CDEF3096DB13}"/>
+    <hyperlink ref="F1114" r:id="rId23" xr:uid="{B0ED86D2-3643-405A-B6A7-581D3F444E88}"/>
+    <hyperlink ref="F1113" r:id="rId24" xr:uid="{3643C6A3-6F1E-403F-B5BD-A7251D505F5B}"/>
+    <hyperlink ref="F1111" r:id="rId25" xr:uid="{0E92FFCB-F966-4697-91BE-A3130C1CAE25}"/>
     <hyperlink ref="F373" r:id="rId26" xr:uid="{B4AE46D0-0113-43B5-920F-41BAD7FB12F3}"/>
     <hyperlink ref="F360" r:id="rId27" xr:uid="{6A53CFF1-B4AE-4894-AF74-B4B080E1676D}"/>
     <hyperlink ref="F357" r:id="rId28" xr:uid="{FC91B321-7F3C-4B7C-978D-FF322BE215D6}"/>
@@ -76696,7 +76705,7 @@
     <sortCondition ref="A1:A20"/>
   </sortState>
   <conditionalFormatting sqref="A2:L9999">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND($A2&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -83568,7 +83577,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:D67">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
2025-06-12 @ 07:43 - Nouvel ordinateur
* Application
- Changer 'Robert M. Vigneault' pour 'RobertMV'
- Ajustement à la taille de certaines formes ???
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Entrée.xlsx
+++ b/DataFiles/GCF_BD_Entrée.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\APP\GCF\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29B4762-5DEB-4268-BE3B-7AA24746DF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BF78CA-AB5B-4055-A554-EA2045932C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="11385" xr2:uid="{1149FE03-DBFD-48E8-9634-6F1E7CDFC6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14871" uniqueCount="8478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14914" uniqueCount="8500">
   <si>
     <t>GL_ID</t>
   </si>
@@ -25476,6 +25476,72 @@
   </si>
   <si>
     <t>Saint-Roch-del'Achigan</t>
+  </si>
+  <si>
+    <t>Gépercom Inc. [Joanny Théberge]</t>
+  </si>
+  <si>
+    <t>1835</t>
+  </si>
+  <si>
+    <t>Gépercom Inc.</t>
+  </si>
+  <si>
+    <t>Joanny Théberge</t>
+  </si>
+  <si>
+    <t>jtheberge@planipret.com</t>
+  </si>
+  <si>
+    <t>12 Place Nelson</t>
+  </si>
+  <si>
+    <t>J6A 3V3</t>
+  </si>
+  <si>
+    <t>Alliance Lambert Inc. [Sébastien Lambert]</t>
+  </si>
+  <si>
+    <t>1836</t>
+  </si>
+  <si>
+    <t>Lessard CPA Inc.</t>
+  </si>
+  <si>
+    <t>Sébastien Lambert</t>
+  </si>
+  <si>
+    <t>200 ch. de la Grande-Carrière</t>
+  </si>
+  <si>
+    <t>J5V 2J7</t>
+  </si>
+  <si>
+    <t>Alliance Lambert Inc. [Sébastien Lambert] Lessard</t>
+  </si>
+  <si>
+    <t>RP Métal Inc. [René Paquin]</t>
+  </si>
+  <si>
+    <t>1837</t>
+  </si>
+  <si>
+    <t>René Paquin</t>
+  </si>
+  <si>
+    <t>rpmetal@hotmail.com</t>
+  </si>
+  <si>
+    <t>1720 rang des Chutes</t>
+  </si>
+  <si>
+    <t>Saint-Ursule</t>
+  </si>
+  <si>
+    <t>J)K 3M0</t>
+  </si>
+  <si>
+    <t>RP Métal Inc. [René Paquin] Lessard</t>
   </si>
 </sst>
 </file>
@@ -25711,7 +25777,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -25836,6 +25902,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -26177,7 +26246,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A0F7D9-502A-4056-B648-6EA13DB3BC6F}">
   <sheetPr codeName="wshClients"/>
-  <dimension ref="A1:R1157"/>
+  <dimension ref="A1:R1160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A1101" activePane="bottomLeft" state="frozen"/>
@@ -74677,6 +74746,150 @@
       </c>
       <c r="R1157" s="43">
         <v>45798.954733796301</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:18">
+      <c r="A1158" s="31" t="s">
+        <v>8478</v>
+      </c>
+      <c r="B1158" s="31" t="s">
+        <v>8479</v>
+      </c>
+      <c r="C1158" s="31" t="s">
+        <v>8480</v>
+      </c>
+      <c r="D1158" s="31" t="s">
+        <v>8481</v>
+      </c>
+      <c r="F1158" s="31" t="s">
+        <v>8482</v>
+      </c>
+      <c r="G1158" s="31" t="s">
+        <v>8483</v>
+      </c>
+      <c r="I1158" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="J1158" s="31" t="s">
+        <v>563</v>
+      </c>
+      <c r="K1158" s="31" t="s">
+        <v>8484</v>
+      </c>
+      <c r="L1158" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1158" s="31" t="s">
+        <v>740</v>
+      </c>
+      <c r="N1158" s="31" t="s">
+        <v>5736</v>
+      </c>
+      <c r="O1158" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q1158" s="31" t="s">
+        <v>8478</v>
+      </c>
+      <c r="R1158" s="47">
+        <v>45817.529340277797</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:18">
+      <c r="A1159" s="31" t="s">
+        <v>8485</v>
+      </c>
+      <c r="B1159" s="31" t="s">
+        <v>8486</v>
+      </c>
+      <c r="C1159" s="31" t="s">
+        <v>8487</v>
+      </c>
+      <c r="D1159" s="31" t="s">
+        <v>8488</v>
+      </c>
+      <c r="E1159" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1159" s="31" t="s">
+        <v>8489</v>
+      </c>
+      <c r="I1159" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="J1159" s="31" t="s">
+        <v>563</v>
+      </c>
+      <c r="K1159" s="31" t="s">
+        <v>8490</v>
+      </c>
+      <c r="L1159" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1159" s="31" t="s">
+        <v>8487</v>
+      </c>
+      <c r="N1159" s="31" t="s">
+        <v>5737</v>
+      </c>
+      <c r="O1159" s="31" t="s">
+        <v>8487</v>
+      </c>
+      <c r="Q1159" s="31" t="s">
+        <v>8491</v>
+      </c>
+      <c r="R1159" s="47">
+        <v>45817.537696759297</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:18">
+      <c r="A1160" s="31" t="s">
+        <v>8492</v>
+      </c>
+      <c r="B1160" s="31" t="s">
+        <v>8493</v>
+      </c>
+      <c r="C1160" s="31" t="s">
+        <v>8487</v>
+      </c>
+      <c r="D1160" s="31" t="s">
+        <v>8494</v>
+      </c>
+      <c r="E1160" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1160" s="31" t="s">
+        <v>8495</v>
+      </c>
+      <c r="G1160" s="31" t="s">
+        <v>8496</v>
+      </c>
+      <c r="I1160" s="31" t="s">
+        <v>8497</v>
+      </c>
+      <c r="J1160" s="31" t="s">
+        <v>563</v>
+      </c>
+      <c r="K1160" s="31" t="s">
+        <v>8498</v>
+      </c>
+      <c r="L1160" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1160" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1160" s="31" t="s">
+        <v>5752</v>
+      </c>
+      <c r="O1160" s="31" t="s">
+        <v>8487</v>
+      </c>
+      <c r="Q1160" s="31" t="s">
+        <v>8499</v>
+      </c>
+      <c r="R1160" s="47">
+        <v>45817.626562500001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>